<commit_message>
Updated Partner Management Status Tracking
</commit_message>
<xml_diff>
--- a/_files/requirements/requirements_detailing_references/Partner Management/Pending_Backlog_Stories_Status Tracking.xlsx
+++ b/_files/requirements/requirements_detailing_references/Partner Management/Pending_Backlog_Stories_Status Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\Project\PMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{58034C1B-DC63-412C-879B-1D0C16F76DC0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{66B78959-4FD4-4345-A1B5-1D137DEFF9D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Admin!$A$2:$I$115</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ID-Authentication'!$A$2:$J$44</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Kernel!$A$2:$I$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Partner Management'!$A$2:$K$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Partner Management'!$A$2:$K$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Pre-registration'!$A$2:$I$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Registration Client'!$A$2:$I$73</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Registration Processor'!$A$2:$I$31</definedName>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2214" uniqueCount="1241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2194" uniqueCount="1222">
   <si>
     <t>Story Backlog: Pre-registration</t>
   </si>
@@ -3640,12 +3640,6 @@
     <t>As the MOSIP system, I should be able to distribute Public Key to Partners for Encryption of auth/KYC Request</t>
   </si>
   <si>
-    <t>As the MOSIP system, I should be able to Validate and Re-Issue the Digital Certificate provided by a Partner</t>
-  </si>
-  <si>
-    <t>As the MOSIP system, I should be able to check status of a Partner</t>
-  </si>
-  <si>
     <t>As the Partner Manager, I should be able to deactivate Auth/E-KYC Partners</t>
   </si>
   <si>
@@ -3688,9 +3682,6 @@
     <t>Tech Story - integrate with Kernel (IAM) for Role Mangement for PM services</t>
   </si>
   <si>
-    <t>As the MOSIP system - PM, I should be able to integrate with kernel for Partner  Certificate signing and resigning</t>
-  </si>
-  <si>
     <t>MOS-26026</t>
   </si>
   <si>
@@ -3733,36 +3724,9 @@
     <t>MOS-26013</t>
   </si>
   <si>
-    <t>MOS-26012</t>
-  </si>
-  <si>
-    <t>MOS-26011</t>
-  </si>
-  <si>
-    <t>MOS-26010</t>
-  </si>
-  <si>
-    <t>MOS-26009</t>
-  </si>
-  <si>
-    <t>MOS-26008</t>
-  </si>
-  <si>
-    <t>MOS-26007</t>
-  </si>
-  <si>
-    <t>MOS-26005</t>
-  </si>
-  <si>
-    <t>MOS-26003</t>
-  </si>
-  <si>
     <t>MOS-24505</t>
   </si>
   <si>
-    <t>MOS-24504</t>
-  </si>
-  <si>
     <t>MOS-24503</t>
   </si>
   <si>
@@ -3832,9 +3796,6 @@
     <t>MOS-24071</t>
   </si>
   <si>
-    <t>MOS-24070</t>
-  </si>
-  <si>
     <t>MOS-24069</t>
   </si>
   <si>
@@ -3850,9 +3811,6 @@
     <t>ID/Key Generation and Validation</t>
   </si>
   <si>
-    <t xml:space="preserve">User Management - Admin </t>
-  </si>
-  <si>
     <t>Digital Certificate Signing/Resigning</t>
   </si>
   <si>
@@ -3910,30 +3868,6 @@
     <t>Delivery Dates</t>
   </si>
   <si>
-    <t>As the MOSIP Admin, I should be able to Create Policy Managers [To be deleted]</t>
-  </si>
-  <si>
-    <t>As the MOSIP Admin, I should be able to retrieve Policy Managers  [To be deleted]</t>
-  </si>
-  <si>
-    <t>As the MOSIP Admin, I should be able to update Policy Manager  [To be deleted]</t>
-  </si>
-  <si>
-    <t>As the MOSIP Admin, I should be able to deactivate Policy Managers  [To be deleted]</t>
-  </si>
-  <si>
-    <t>As the MOSIP Admin, I should be able to Create Partner Managers  [To be deleted]</t>
-  </si>
-  <si>
-    <t>As the MOSIP Admin, I should be able to retrieve Partner Managers  [To be deleted]</t>
-  </si>
-  <si>
-    <t>As the MOSIP Admin, I should be able to update Partner  Managers  [To be deleted]</t>
-  </si>
-  <si>
-    <t>As the MOSIP Admin, I should be able to deactivate Partner Managers  [To be deleted]</t>
-  </si>
-  <si>
     <t xml:space="preserve">As the MOSIP system I should be able to validate Partner api key pattern </t>
   </si>
   <si>
@@ -3949,18 +3883,12 @@
     <t>As the MOSIP system, I should be able to generate MISP ID</t>
   </si>
   <si>
-    <t>As the MOSIP system- PM, I should be able to integrate with kernel  to integrate kernel dependencies [To be deleted]</t>
-  </si>
-  <si>
     <t>As the MOSIP system , I should be able to accomodate key Management related features - key Generation, key Validation and Key Re-generation</t>
   </si>
   <si>
     <t xml:space="preserve">As the MOSIP system, I should be able to validate MISP License Key Pattern </t>
   </si>
   <si>
-    <t>Tech Story - Integrate with kernel for MISP ID Generation [To be deleted]</t>
-  </si>
-  <si>
     <t>As the MOSIP system, I should be able to validate Partner ID pattern</t>
   </si>
   <si>
@@ -3974,13 +3902,28 @@
   </si>
   <si>
     <t>MOS-24496</t>
+  </si>
+  <si>
+    <t>As the Partner, I should be able to download MOSIP digital certificate</t>
+  </si>
+  <si>
+    <t>As the Partner, I should be able to upload MOSIP digital certificate</t>
+  </si>
+  <si>
+    <t>MOS-27240</t>
+  </si>
+  <si>
+    <t>As the Partner Manger, I should be able to retrieve Auth/E-KYC Policy for my policy group so that I can assign relevant policy to partner api key</t>
+  </si>
+  <si>
+    <t>As the MOSIP system - IDA, I should be able to validate MISP License key</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4171,12 +4114,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF7030A0"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
     </font>
@@ -4191,6 +4128,18 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Cambria"/>
       <family val="1"/>
     </font>
@@ -4605,7 +4554,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -4648,8 +4597,9 @@
     <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4776,60 +4726,66 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="27" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="26" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4864,38 +4820,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -4935,6 +4888,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -5271,12 +5225,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="67" t="s">
         <v>984</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="67"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="69"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -5825,17 +5779,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -5870,7 +5824,7 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="70" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -5897,7 +5851,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="69"/>
+      <c r="B4" s="71"/>
       <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
@@ -5922,7 +5876,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="69"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
@@ -5947,7 +5901,7 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="69"/>
+      <c r="B6" s="71"/>
       <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
@@ -5972,7 +5926,7 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="69"/>
+      <c r="B7" s="71"/>
       <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
@@ -5999,7 +5953,7 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="70"/>
+      <c r="B8" s="72"/>
       <c r="C8" s="6" t="s">
         <v>30</v>
       </c>
@@ -6227,7 +6181,7 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="70" t="s">
         <v>67</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -6254,7 +6208,7 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="70"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="6" t="s">
         <v>71</v>
       </c>
@@ -6279,7 +6233,7 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="70" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -6306,7 +6260,7 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="70"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="6" t="s">
         <v>64</v>
       </c>
@@ -6428,17 +6382,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -6500,7 +6454,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="73" t="s">
         <v>1020</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -6527,7 +6481,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="72"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="6" t="s">
         <v>92</v>
       </c>
@@ -6776,7 +6730,7 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="73" t="s">
         <v>1055</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -6805,7 +6759,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="72"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="6" t="s">
         <v>121</v>
       </c>
@@ -6994,7 +6948,7 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="73" t="s">
         <v>1038</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -7021,7 +6975,7 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="73"/>
+      <c r="B23" s="75"/>
       <c r="C23" s="6" t="s">
         <v>185</v>
       </c>
@@ -7046,7 +7000,7 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="72"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="6" t="s">
         <v>188</v>
       </c>
@@ -7210,7 +7164,7 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="71" t="s">
+      <c r="B30" s="73" t="s">
         <v>1057</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -7239,7 +7193,7 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="72"/>
+      <c r="B31" s="74"/>
       <c r="C31" s="6" t="s">
         <v>142</v>
       </c>
@@ -7266,7 +7220,7 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="71" t="s">
+      <c r="B32" s="73" t="s">
         <v>1058</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -7295,7 +7249,7 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="72"/>
+      <c r="B33" s="74"/>
       <c r="C33" s="6" t="s">
         <v>147</v>
       </c>
@@ -7519,7 +7473,7 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="71" t="s">
+      <c r="B41" s="73" t="s">
         <v>194</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -7548,7 +7502,7 @@
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="72"/>
+      <c r="B42" s="74"/>
       <c r="C42" s="6" t="s">
         <v>197</v>
       </c>
@@ -7602,7 +7556,7 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="71" t="s">
+      <c r="B44" s="73" t="s">
         <v>1034</v>
       </c>
       <c r="C44" s="6" t="s">
@@ -7631,7 +7585,7 @@
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" s="72"/>
+      <c r="B45" s="74"/>
       <c r="C45" s="6" t="s">
         <v>208</v>
       </c>
@@ -7714,7 +7668,7 @@
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="71" t="s">
+      <c r="B48" s="73" t="s">
         <v>222</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -7735,7 +7689,7 @@
       <c r="H48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I48" s="68" t="s">
+      <c r="I48" s="70" t="s">
         <v>1000</v>
       </c>
     </row>
@@ -7743,7 +7697,7 @@
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" s="73"/>
+      <c r="B49" s="75"/>
       <c r="C49" s="6" t="s">
         <v>226</v>
       </c>
@@ -7762,13 +7716,13 @@
       <c r="H49" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I49" s="69"/>
+      <c r="I49" s="71"/>
     </row>
     <row r="50" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="73"/>
+      <c r="B50" s="75"/>
       <c r="C50" s="6" t="s">
         <v>229</v>
       </c>
@@ -7787,13 +7741,13 @@
       <c r="H50" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I50" s="69"/>
+      <c r="I50" s="71"/>
     </row>
     <row r="51" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" s="73"/>
+      <c r="B51" s="75"/>
       <c r="C51" s="6" t="s">
         <v>232</v>
       </c>
@@ -7812,13 +7766,13 @@
       <c r="H51" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I51" s="69"/>
+      <c r="I51" s="71"/>
     </row>
     <row r="52" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" s="73"/>
+      <c r="B52" s="75"/>
       <c r="C52" s="6" t="s">
         <v>235</v>
       </c>
@@ -7837,13 +7791,13 @@
       <c r="H52" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I52" s="69"/>
+      <c r="I52" s="71"/>
     </row>
     <row r="53" spans="1:9" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="B53" s="73"/>
+      <c r="B53" s="75"/>
       <c r="C53" s="6" t="s">
         <v>238</v>
       </c>
@@ -7862,13 +7816,13 @@
       <c r="H53" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I53" s="69"/>
+      <c r="I53" s="71"/>
     </row>
     <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54" s="73"/>
+      <c r="B54" s="75"/>
       <c r="C54" s="6" t="s">
         <v>241</v>
       </c>
@@ -7887,13 +7841,13 @@
       <c r="H54" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I54" s="69"/>
+      <c r="I54" s="71"/>
     </row>
     <row r="55" spans="1:9" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55" s="73"/>
+      <c r="B55" s="75"/>
       <c r="C55" s="6" t="s">
         <v>244</v>
       </c>
@@ -7912,13 +7866,13 @@
       <c r="H55" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I55" s="69"/>
+      <c r="I55" s="71"/>
     </row>
     <row r="56" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56" s="73"/>
+      <c r="B56" s="75"/>
       <c r="C56" s="6" t="s">
         <v>1041</v>
       </c>
@@ -7933,13 +7887,13 @@
         <v>987</v>
       </c>
       <c r="H56" s="4"/>
-      <c r="I56" s="69"/>
+      <c r="I56" s="71"/>
     </row>
     <row r="57" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57" s="72"/>
+      <c r="B57" s="74"/>
       <c r="C57" s="6" t="s">
         <v>247</v>
       </c>
@@ -7958,13 +7912,13 @@
       <c r="H57" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I57" s="70"/>
+      <c r="I57" s="72"/>
     </row>
     <row r="58" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58" s="71" t="s">
+      <c r="B58" s="73" t="s">
         <v>222</v>
       </c>
       <c r="C58" s="6" t="s">
@@ -7985,7 +7939,7 @@
       <c r="H58" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I58" s="68" t="s">
+      <c r="I58" s="70" t="s">
         <v>1000</v>
       </c>
     </row>
@@ -7993,7 +7947,7 @@
       <c r="A59" s="1">
         <v>57</v>
       </c>
-      <c r="B59" s="73"/>
+      <c r="B59" s="75"/>
       <c r="C59" s="6" t="s">
         <v>253</v>
       </c>
@@ -8012,13 +7966,13 @@
       <c r="H59" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I59" s="69"/>
+      <c r="I59" s="71"/>
     </row>
     <row r="60" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
-      <c r="B60" s="73"/>
+      <c r="B60" s="75"/>
       <c r="C60" s="6" t="s">
         <v>256</v>
       </c>
@@ -8037,13 +7991,13 @@
       <c r="H60" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I60" s="69"/>
+      <c r="I60" s="71"/>
     </row>
     <row r="61" spans="1:9" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61" s="73"/>
+      <c r="B61" s="75"/>
       <c r="C61" s="6" t="s">
         <v>259</v>
       </c>
@@ -8062,13 +8016,13 @@
       <c r="H61" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I61" s="69"/>
+      <c r="I61" s="71"/>
     </row>
     <row r="62" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" s="73"/>
+      <c r="B62" s="75"/>
       <c r="C62" s="6" t="s">
         <v>262</v>
       </c>
@@ -8087,13 +8041,13 @@
       <c r="H62" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I62" s="69"/>
+      <c r="I62" s="71"/>
     </row>
     <row r="63" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" s="73"/>
+      <c r="B63" s="75"/>
       <c r="C63" s="6" t="s">
         <v>264</v>
       </c>
@@ -8112,13 +8066,13 @@
       <c r="H63" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I63" s="69"/>
+      <c r="I63" s="71"/>
     </row>
     <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" s="73"/>
+      <c r="B64" s="75"/>
       <c r="C64" s="6" t="s">
         <v>75</v>
       </c>
@@ -8137,13 +8091,13 @@
       <c r="H64" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I64" s="69"/>
+      <c r="I64" s="71"/>
     </row>
     <row r="65" spans="1:9" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" s="73"/>
+      <c r="B65" s="75"/>
       <c r="C65" s="6" t="s">
         <v>268</v>
       </c>
@@ -8162,13 +8116,13 @@
       <c r="H65" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I65" s="69"/>
+      <c r="I65" s="71"/>
     </row>
     <row r="66" spans="1:9" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" s="73"/>
+      <c r="B66" s="75"/>
       <c r="C66" s="6" t="s">
         <v>271</v>
       </c>
@@ -8187,13 +8141,13 @@
       <c r="H66" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I66" s="69"/>
+      <c r="I66" s="71"/>
     </row>
     <row r="67" spans="1:9" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" s="73"/>
+      <c r="B67" s="75"/>
       <c r="C67" s="6" t="s">
         <v>274</v>
       </c>
@@ -8212,13 +8166,13 @@
       <c r="H67" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I67" s="69"/>
+      <c r="I67" s="71"/>
     </row>
     <row r="68" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" s="73"/>
+      <c r="B68" s="75"/>
       <c r="C68" s="6" t="s">
         <v>277</v>
       </c>
@@ -8237,13 +8191,13 @@
       <c r="H68" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I68" s="69"/>
+      <c r="I68" s="71"/>
     </row>
     <row r="69" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69" s="73"/>
+      <c r="B69" s="75"/>
       <c r="C69" s="6" t="s">
         <v>280</v>
       </c>
@@ -8262,13 +8216,13 @@
       <c r="H69" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I69" s="69"/>
+      <c r="I69" s="71"/>
     </row>
     <row r="70" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
-      <c r="B70" s="73"/>
+      <c r="B70" s="75"/>
       <c r="C70" s="6" t="s">
         <v>283</v>
       </c>
@@ -8287,13 +8241,13 @@
       <c r="H70" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I70" s="69"/>
+      <c r="I70" s="71"/>
     </row>
     <row r="71" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" s="72"/>
+      <c r="B71" s="74"/>
       <c r="C71" s="6" t="s">
         <v>285</v>
       </c>
@@ -8312,7 +8266,7 @@
       <c r="H71" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I71" s="70"/>
+      <c r="I71" s="72"/>
     </row>
     <row r="72" spans="1:9" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
@@ -8507,17 +8461,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="67" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -9368,17 +9322,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="67" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -9523,7 +9477,7 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="73" t="s">
         <v>398</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -9550,7 +9504,7 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="74"/>
+      <c r="B8" s="76"/>
       <c r="C8" s="6" t="s">
         <v>402</v>
       </c>
@@ -9575,7 +9529,7 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="74"/>
+      <c r="B9" s="76"/>
       <c r="C9" s="6" t="s">
         <v>405</v>
       </c>
@@ -9600,7 +9554,7 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="74"/>
+      <c r="B10" s="76"/>
       <c r="C10" s="6" t="s">
         <v>408</v>
       </c>
@@ -9625,7 +9579,7 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="74"/>
+      <c r="B11" s="76"/>
       <c r="C11" s="6" t="s">
         <v>411</v>
       </c>
@@ -9650,7 +9604,7 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="74"/>
+      <c r="B12" s="76"/>
       <c r="C12" s="6" t="s">
         <v>414</v>
       </c>
@@ -9675,7 +9629,7 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="74"/>
+      <c r="B13" s="76"/>
       <c r="C13" s="6" t="s">
         <v>417</v>
       </c>
@@ -9700,7 +9654,7 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="75"/>
+      <c r="B14" s="77"/>
       <c r="C14" s="6" t="s">
         <v>420</v>
       </c>
@@ -9920,7 +9874,7 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="73" t="s">
         <v>448</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -9947,7 +9901,7 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="74"/>
+      <c r="B23" s="76"/>
       <c r="C23" s="38" t="s">
         <v>452</v>
       </c>
@@ -9974,7 +9928,7 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="74"/>
+      <c r="B24" s="76"/>
       <c r="C24" s="6" t="s">
         <v>455</v>
       </c>
@@ -9999,7 +9953,7 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="74"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="6" t="s">
         <v>457</v>
       </c>
@@ -10024,7 +9978,7 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="74"/>
+      <c r="B26" s="76"/>
       <c r="C26" s="38" t="s">
         <v>459</v>
       </c>
@@ -10051,7 +10005,7 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="75"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="6" t="s">
         <v>462</v>
       </c>
@@ -10130,7 +10084,7 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="71" t="s">
+      <c r="B30" s="73" t="s">
         <v>471</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -10157,7 +10111,7 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="74"/>
+      <c r="B31" s="76"/>
       <c r="C31" s="6" t="s">
         <v>475</v>
       </c>
@@ -10182,7 +10136,7 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="74"/>
+      <c r="B32" s="76"/>
       <c r="C32" s="6" t="s">
         <v>478</v>
       </c>
@@ -10207,7 +10161,7 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="75"/>
+      <c r="B33" s="77"/>
       <c r="C33" s="6" t="s">
         <v>481</v>
       </c>
@@ -10371,7 +10325,7 @@
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="71" t="s">
+      <c r="B39" s="73" t="s">
         <v>502</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -10398,7 +10352,7 @@
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="74"/>
+      <c r="B40" s="76"/>
       <c r="C40" s="6" t="s">
         <v>506</v>
       </c>
@@ -10423,7 +10377,7 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="75"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="6" t="s">
         <v>509</v>
       </c>
@@ -10448,7 +10402,7 @@
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="71" t="s">
+      <c r="B42" s="73" t="s">
         <v>512</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -10473,7 +10427,7 @@
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" s="74"/>
+      <c r="B43" s="76"/>
       <c r="C43" s="6" t="s">
         <v>516</v>
       </c>
@@ -10496,7 +10450,7 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="75"/>
+      <c r="B44" s="77"/>
       <c r="C44" s="6" t="s">
         <v>519</v>
       </c>
@@ -10566,17 +10520,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="67" t="s">
         <v>522</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -10943,17 +10897,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="67" t="s">
         <v>550</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -11284,7 +11238,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="70" t="s">
         <v>601</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -11309,7 +11263,7 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="70"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="6" t="s">
         <v>605</v>
       </c>
@@ -11448,18 +11402,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="67" t="s">
         <v>616</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="69"/>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -11497,7 +11451,7 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="73" t="s">
         <v>618</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -11521,7 +11475,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="72"/>
+      <c r="B4" s="74"/>
       <c r="C4" s="8" t="s">
         <v>621</v>
       </c>
@@ -11543,7 +11497,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="73" t="s">
         <v>623</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -11567,7 +11521,7 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="72"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="8" t="s">
         <v>626</v>
       </c>
@@ -11613,7 +11567,7 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="73" t="s">
         <v>631</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -11637,7 +11591,7 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="72"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="8" t="s">
         <v>634</v>
       </c>
@@ -11685,7 +11639,7 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="73" t="s">
         <v>640</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -11711,7 +11665,7 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="72"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="8" t="s">
         <v>643</v>
       </c>
@@ -11757,7 +11711,7 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="73" t="s">
         <v>648</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -11781,7 +11735,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="72"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="8" t="s">
         <v>651</v>
       </c>
@@ -11801,7 +11755,7 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="71" t="s">
+      <c r="B16" s="73" t="s">
         <v>653</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -11825,7 +11779,7 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="73"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="8" t="s">
         <v>656</v>
       </c>
@@ -11849,7 +11803,7 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="72"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="8" t="s">
         <v>658</v>
       </c>
@@ -11893,7 +11847,7 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="73" t="s">
         <v>663</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -11915,7 +11869,7 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="72"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="8" t="s">
         <v>666</v>
       </c>
@@ -11959,7 +11913,7 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="71" t="s">
+      <c r="B23" s="73" t="s">
         <v>671</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -11983,7 +11937,7 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="72"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="8" t="s">
         <v>674</v>
       </c>
@@ -12029,7 +11983,7 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="71" t="s">
+      <c r="B26" s="73" t="s">
         <v>679</v>
       </c>
       <c r="C26" s="8" t="s">
@@ -12053,7 +12007,7 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="73"/>
+      <c r="B27" s="75"/>
       <c r="C27" s="8" t="s">
         <v>682</v>
       </c>
@@ -12077,7 +12031,7 @@
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="72"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="8" t="s">
         <v>684</v>
       </c>
@@ -12097,7 +12051,7 @@
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="71" t="s">
+      <c r="B29" s="73" t="s">
         <v>686</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -12121,7 +12075,7 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="72"/>
+      <c r="B30" s="74"/>
       <c r="C30" s="8" t="s">
         <v>689</v>
       </c>
@@ -12167,7 +12121,7 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="71" t="s">
+      <c r="B32" s="73" t="s">
         <v>694</v>
       </c>
       <c r="C32" s="8" t="s">
@@ -12191,7 +12145,7 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="72"/>
+      <c r="B33" s="74"/>
       <c r="C33" s="8" t="s">
         <v>697</v>
       </c>
@@ -12213,7 +12167,7 @@
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="71" t="s">
+      <c r="B34" s="73" t="s">
         <v>699</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -12237,7 +12191,7 @@
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" s="72"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="8" t="s">
         <v>702</v>
       </c>
@@ -12305,7 +12259,7 @@
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" s="71" t="s">
+      <c r="B38" s="73" t="s">
         <v>710</v>
       </c>
       <c r="C38" s="8" t="s">
@@ -12329,7 +12283,7 @@
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="72"/>
+      <c r="B39" s="74"/>
       <c r="C39" s="8" t="s">
         <v>713</v>
       </c>
@@ -12351,7 +12305,7 @@
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="71" t="s">
+      <c r="B40" s="73" t="s">
         <v>715</v>
       </c>
       <c r="C40" s="8" t="s">
@@ -12375,7 +12329,7 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="72"/>
+      <c r="B41" s="74"/>
       <c r="C41" s="8" t="s">
         <v>718</v>
       </c>
@@ -12421,7 +12375,7 @@
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" s="71" t="s">
+      <c r="B43" s="73" t="s">
         <v>723</v>
       </c>
       <c r="C43" s="8" t="s">
@@ -12445,7 +12399,7 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="72"/>
+      <c r="B44" s="74"/>
       <c r="C44" s="8" t="s">
         <v>726</v>
       </c>
@@ -12467,7 +12421,7 @@
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" s="71" t="s">
+      <c r="B45" s="73" t="s">
         <v>728</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -12491,7 +12445,7 @@
       <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="B46" s="72"/>
+      <c r="B46" s="74"/>
       <c r="C46" s="8" t="s">
         <v>731</v>
       </c>
@@ -12515,7 +12469,7 @@
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" s="71" t="s">
+      <c r="B47" s="73" t="s">
         <v>733</v>
       </c>
       <c r="C47" s="8" t="s">
@@ -12539,7 +12493,7 @@
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="72"/>
+      <c r="B48" s="74"/>
       <c r="C48" s="8" t="s">
         <v>736</v>
       </c>
@@ -12559,7 +12513,7 @@
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" s="71" t="s">
+      <c r="B49" s="73" t="s">
         <v>738</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -12583,7 +12537,7 @@
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="72"/>
+      <c r="B50" s="74"/>
       <c r="C50" s="8" t="s">
         <v>741</v>
       </c>
@@ -12607,7 +12561,7 @@
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" s="71" t="s">
+      <c r="B51" s="73" t="s">
         <v>743</v>
       </c>
       <c r="C51" s="8" t="s">
@@ -12629,7 +12583,7 @@
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" s="72"/>
+      <c r="B52" s="74"/>
       <c r="C52" s="8" t="s">
         <v>746</v>
       </c>
@@ -12673,7 +12627,7 @@
       <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54" s="71" t="s">
+      <c r="B54" s="73" t="s">
         <v>751</v>
       </c>
       <c r="C54" s="8" t="s">
@@ -12697,7 +12651,7 @@
       <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55" s="73"/>
+      <c r="B55" s="75"/>
       <c r="C55" s="8" t="s">
         <v>754</v>
       </c>
@@ -12721,7 +12675,7 @@
       <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56" s="72"/>
+      <c r="B56" s="74"/>
       <c r="C56" s="8" t="s">
         <v>756</v>
       </c>
@@ -12741,7 +12695,7 @@
       <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57" s="71" t="s">
+      <c r="B57" s="73" t="s">
         <v>758</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -12765,7 +12719,7 @@
       <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58" s="72"/>
+      <c r="B58" s="74"/>
       <c r="C58" s="8" t="s">
         <v>761</v>
       </c>
@@ -12837,7 +12791,7 @@
       <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61" s="71" t="s">
+      <c r="B61" s="73" t="s">
         <v>769</v>
       </c>
       <c r="C61" s="8" t="s">
@@ -12861,7 +12815,7 @@
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" s="72"/>
+      <c r="B62" s="74"/>
       <c r="C62" s="8" t="s">
         <v>772</v>
       </c>
@@ -12885,7 +12839,7 @@
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" s="71" t="s">
+      <c r="B63" s="73" t="s">
         <v>774</v>
       </c>
       <c r="C63" s="8" t="s">
@@ -12909,7 +12863,7 @@
       <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" s="72"/>
+      <c r="B64" s="74"/>
       <c r="C64" s="8" t="s">
         <v>777</v>
       </c>
@@ -12935,7 +12889,7 @@
       <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" s="71" t="s">
+      <c r="B65" s="73" t="s">
         <v>780</v>
       </c>
       <c r="C65" s="8" t="s">
@@ -12959,7 +12913,7 @@
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" s="73"/>
+      <c r="B66" s="75"/>
       <c r="C66" s="8" t="s">
         <v>783</v>
       </c>
@@ -12981,7 +12935,7 @@
       <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" s="73"/>
+      <c r="B67" s="75"/>
       <c r="C67" s="8" t="s">
         <v>785</v>
       </c>
@@ -13003,7 +12957,7 @@
       <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" s="73"/>
+      <c r="B68" s="75"/>
       <c r="C68" s="8" t="s">
         <v>787</v>
       </c>
@@ -13025,7 +12979,7 @@
       <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69" s="72"/>
+      <c r="B69" s="74"/>
       <c r="C69" s="8" t="s">
         <v>789</v>
       </c>
@@ -13071,7 +13025,7 @@
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" s="71" t="s">
+      <c r="B71" s="73" t="s">
         <v>794</v>
       </c>
       <c r="C71" s="8" t="s">
@@ -13095,7 +13049,7 @@
       <c r="A72" s="1">
         <v>70</v>
       </c>
-      <c r="B72" s="72"/>
+      <c r="B72" s="74"/>
       <c r="C72" s="8" t="s">
         <v>797</v>
       </c>
@@ -13139,7 +13093,7 @@
       <c r="A74" s="1">
         <v>72</v>
       </c>
-      <c r="B74" s="71" t="s">
+      <c r="B74" s="73" t="s">
         <v>802</v>
       </c>
       <c r="C74" s="8" t="s">
@@ -13163,7 +13117,7 @@
       <c r="A75" s="1">
         <v>73</v>
       </c>
-      <c r="B75" s="72"/>
+      <c r="B75" s="74"/>
       <c r="C75" s="8" t="s">
         <v>805</v>
       </c>
@@ -13233,7 +13187,7 @@
       <c r="A78" s="1">
         <v>76</v>
       </c>
-      <c r="B78" s="71" t="s">
+      <c r="B78" s="73" t="s">
         <v>813</v>
       </c>
       <c r="C78" s="8" t="s">
@@ -13257,7 +13211,7 @@
       <c r="A79" s="1">
         <v>77</v>
       </c>
-      <c r="B79" s="72"/>
+      <c r="B79" s="74"/>
       <c r="C79" s="8" t="s">
         <v>816</v>
       </c>
@@ -13281,7 +13235,7 @@
       <c r="A80" s="1">
         <v>78</v>
       </c>
-      <c r="B80" s="71" t="s">
+      <c r="B80" s="73" t="s">
         <v>818</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -13305,7 +13259,7 @@
       <c r="A81" s="1">
         <v>79</v>
       </c>
-      <c r="B81" s="72"/>
+      <c r="B81" s="74"/>
       <c r="C81" s="8" t="s">
         <v>821</v>
       </c>
@@ -13329,7 +13283,7 @@
       <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B82" s="71" t="s">
+      <c r="B82" s="73" t="s">
         <v>823</v>
       </c>
       <c r="C82" s="8" t="s">
@@ -13353,7 +13307,7 @@
       <c r="A83" s="1">
         <v>81</v>
       </c>
-      <c r="B83" s="73"/>
+      <c r="B83" s="75"/>
       <c r="C83" s="8" t="s">
         <v>826</v>
       </c>
@@ -13375,7 +13329,7 @@
       <c r="A84" s="1">
         <v>82</v>
       </c>
-      <c r="B84" s="73"/>
+      <c r="B84" s="75"/>
       <c r="C84" s="8" t="s">
         <v>828</v>
       </c>
@@ -13397,7 +13351,7 @@
       <c r="A85" s="1">
         <v>83</v>
       </c>
-      <c r="B85" s="72"/>
+      <c r="B85" s="74"/>
       <c r="C85" s="8" t="s">
         <v>830</v>
       </c>
@@ -13441,7 +13395,7 @@
       <c r="A87" s="1">
         <v>85</v>
       </c>
-      <c r="B87" s="71" t="s">
+      <c r="B87" s="73" t="s">
         <v>834</v>
       </c>
       <c r="C87" s="8" t="s">
@@ -13465,7 +13419,7 @@
       <c r="A88" s="1">
         <v>86</v>
       </c>
-      <c r="B88" s="73"/>
+      <c r="B88" s="75"/>
       <c r="C88" s="8" t="s">
         <v>837</v>
       </c>
@@ -13487,7 +13441,7 @@
       <c r="A89" s="1">
         <v>87</v>
       </c>
-      <c r="B89" s="72"/>
+      <c r="B89" s="74"/>
       <c r="C89" s="8" t="s">
         <v>839</v>
       </c>
@@ -13509,7 +13463,7 @@
       <c r="A90" s="1">
         <v>88</v>
       </c>
-      <c r="B90" s="71" t="s">
+      <c r="B90" s="73" t="s">
         <v>841</v>
       </c>
       <c r="C90" s="8" t="s">
@@ -13533,7 +13487,7 @@
       <c r="A91" s="1">
         <v>89</v>
       </c>
-      <c r="B91" s="73"/>
+      <c r="B91" s="75"/>
       <c r="C91" s="8" t="s">
         <v>844</v>
       </c>
@@ -13553,7 +13507,7 @@
       <c r="A92" s="1">
         <v>90</v>
       </c>
-      <c r="B92" s="72"/>
+      <c r="B92" s="74"/>
       <c r="C92" s="8" t="s">
         <v>846</v>
       </c>
@@ -13573,7 +13527,7 @@
       <c r="A93" s="1">
         <v>91</v>
       </c>
-      <c r="B93" s="71" t="s">
+      <c r="B93" s="73" t="s">
         <v>848</v>
       </c>
       <c r="C93" s="8" t="s">
@@ -13597,7 +13551,7 @@
       <c r="A94" s="1">
         <v>92</v>
       </c>
-      <c r="B94" s="72"/>
+      <c r="B94" s="74"/>
       <c r="C94" s="8" t="s">
         <v>851</v>
       </c>
@@ -13621,7 +13575,7 @@
       <c r="A95" s="1">
         <v>93</v>
       </c>
-      <c r="B95" s="71" t="s">
+      <c r="B95" s="73" t="s">
         <v>853</v>
       </c>
       <c r="C95" s="8" t="s">
@@ -13643,7 +13597,7 @@
       <c r="A96" s="1">
         <v>94</v>
       </c>
-      <c r="B96" s="72"/>
+      <c r="B96" s="74"/>
       <c r="C96" s="8" t="s">
         <v>856</v>
       </c>
@@ -13687,7 +13641,7 @@
       <c r="A98" s="1">
         <v>96</v>
       </c>
-      <c r="B98" s="71" t="s">
+      <c r="B98" s="73" t="s">
         <v>861</v>
       </c>
       <c r="C98" s="8" t="s">
@@ -13711,7 +13665,7 @@
       <c r="A99" s="1">
         <v>97</v>
       </c>
-      <c r="B99" s="73"/>
+      <c r="B99" s="75"/>
       <c r="C99" s="8" t="s">
         <v>864</v>
       </c>
@@ -13735,7 +13689,7 @@
       <c r="A100" s="1">
         <v>98</v>
       </c>
-      <c r="B100" s="72"/>
+      <c r="B100" s="74"/>
       <c r="C100" s="8" t="s">
         <v>866</v>
       </c>
@@ -13755,7 +13709,7 @@
       <c r="A101" s="1">
         <v>99</v>
       </c>
-      <c r="B101" s="71" t="s">
+      <c r="B101" s="73" t="s">
         <v>868</v>
       </c>
       <c r="C101" s="8" t="s">
@@ -13779,7 +13733,7 @@
       <c r="A102" s="1">
         <v>100</v>
       </c>
-      <c r="B102" s="72"/>
+      <c r="B102" s="74"/>
       <c r="C102" s="8" t="s">
         <v>871</v>
       </c>
@@ -13827,7 +13781,7 @@
       <c r="A104" s="1">
         <v>102</v>
       </c>
-      <c r="B104" s="71" t="s">
+      <c r="B104" s="73" t="s">
         <v>876</v>
       </c>
       <c r="C104" s="8" t="s">
@@ -13851,7 +13805,7 @@
       <c r="A105" s="1">
         <v>103</v>
       </c>
-      <c r="B105" s="73"/>
+      <c r="B105" s="75"/>
       <c r="C105" s="8" t="s">
         <v>879</v>
       </c>
@@ -13873,7 +13827,7 @@
       <c r="A106" s="1">
         <v>104</v>
       </c>
-      <c r="B106" s="73"/>
+      <c r="B106" s="75"/>
       <c r="C106" s="8" t="s">
         <v>881</v>
       </c>
@@ -13895,7 +13849,7 @@
       <c r="A107" s="1">
         <v>105</v>
       </c>
-      <c r="B107" s="72"/>
+      <c r="B107" s="74"/>
       <c r="C107" s="8" t="s">
         <v>883</v>
       </c>
@@ -13945,7 +13899,7 @@
       <c r="A109" s="1">
         <v>107</v>
       </c>
-      <c r="B109" s="71" t="s">
+      <c r="B109" s="73" t="s">
         <v>888</v>
       </c>
       <c r="C109" s="8" t="s">
@@ -13967,7 +13921,7 @@
       <c r="A110" s="1">
         <v>108</v>
       </c>
-      <c r="B110" s="72"/>
+      <c r="B110" s="74"/>
       <c r="C110" s="8" t="s">
         <v>891</v>
       </c>
@@ -13987,7 +13941,7 @@
       <c r="A111" s="1">
         <v>109</v>
       </c>
-      <c r="B111" s="71" t="s">
+      <c r="B111" s="73" t="s">
         <v>893</v>
       </c>
       <c r="C111" s="8" t="s">
@@ -14011,7 +13965,7 @@
       <c r="A112" s="1">
         <v>110</v>
       </c>
-      <c r="B112" s="72"/>
+      <c r="B112" s="74"/>
       <c r="C112" s="8" t="s">
         <v>896</v>
       </c>
@@ -14057,7 +14011,7 @@
       <c r="A114" s="1">
         <v>112</v>
       </c>
-      <c r="B114" s="71" t="s">
+      <c r="B114" s="73" t="s">
         <v>901</v>
       </c>
       <c r="C114" s="8" t="s">
@@ -14081,7 +14035,7 @@
       <c r="A115" s="1">
         <v>113</v>
       </c>
-      <c r="B115" s="72"/>
+      <c r="B115" s="74"/>
       <c r="C115" s="8" t="s">
         <v>904</v>
       </c>
@@ -14125,7 +14079,7 @@
       <c r="A117" s="1">
         <v>115</v>
       </c>
-      <c r="B117" s="71" t="s">
+      <c r="B117" s="73" t="s">
         <v>909</v>
       </c>
       <c r="C117" s="8" t="s">
@@ -14147,7 +14101,7 @@
       <c r="A118" s="1">
         <v>116</v>
       </c>
-      <c r="B118" s="73"/>
+      <c r="B118" s="75"/>
       <c r="C118" s="8" t="s">
         <v>912</v>
       </c>
@@ -14167,7 +14121,7 @@
       <c r="A119" s="1">
         <v>117</v>
       </c>
-      <c r="B119" s="73"/>
+      <c r="B119" s="75"/>
       <c r="C119" s="8" t="s">
         <v>914</v>
       </c>
@@ -14187,7 +14141,7 @@
       <c r="A120" s="1">
         <v>118</v>
       </c>
-      <c r="B120" s="72"/>
+      <c r="B120" s="74"/>
       <c r="C120" s="8" t="s">
         <v>916</v>
       </c>
@@ -14207,7 +14161,7 @@
       <c r="A121" s="1">
         <v>119</v>
       </c>
-      <c r="B121" s="71" t="s">
+      <c r="B121" s="73" t="s">
         <v>918</v>
       </c>
       <c r="C121" s="8" t="s">
@@ -14231,7 +14185,7 @@
       <c r="A122" s="1">
         <v>120</v>
       </c>
-      <c r="B122" s="73"/>
+      <c r="B122" s="75"/>
       <c r="C122" s="8" t="s">
         <v>921</v>
       </c>
@@ -14253,7 +14207,7 @@
       <c r="A123" s="1">
         <v>121</v>
       </c>
-      <c r="B123" s="72"/>
+      <c r="B123" s="74"/>
       <c r="C123" s="8" t="s">
         <v>923</v>
       </c>
@@ -14299,7 +14253,7 @@
       <c r="A125" s="1">
         <v>123</v>
       </c>
-      <c r="B125" s="71" t="s">
+      <c r="B125" s="73" t="s">
         <v>928</v>
       </c>
       <c r="C125" s="8" t="s">
@@ -14323,7 +14277,7 @@
       <c r="A126" s="1">
         <v>124</v>
       </c>
-      <c r="B126" s="73"/>
+      <c r="B126" s="75"/>
       <c r="C126" s="8" t="s">
         <v>931</v>
       </c>
@@ -14345,7 +14299,7 @@
       <c r="A127" s="1">
         <v>125</v>
       </c>
-      <c r="B127" s="73"/>
+      <c r="B127" s="75"/>
       <c r="C127" s="8" t="s">
         <v>933</v>
       </c>
@@ -14369,7 +14323,7 @@
       <c r="A128" s="1">
         <v>126</v>
       </c>
-      <c r="B128" s="73"/>
+      <c r="B128" s="75"/>
       <c r="C128" s="8" t="s">
         <v>935</v>
       </c>
@@ -14391,7 +14345,7 @@
       <c r="A129" s="1">
         <v>127</v>
       </c>
-      <c r="B129" s="73"/>
+      <c r="B129" s="75"/>
       <c r="C129" s="8" t="s">
         <v>937</v>
       </c>
@@ -14413,7 +14367,7 @@
       <c r="A130" s="1">
         <v>128</v>
       </c>
-      <c r="B130" s="72"/>
+      <c r="B130" s="74"/>
       <c r="C130" s="8" t="s">
         <v>939</v>
       </c>
@@ -14459,7 +14413,7 @@
       <c r="A132" s="1">
         <v>130</v>
       </c>
-      <c r="B132" s="71" t="s">
+      <c r="B132" s="73" t="s">
         <v>944</v>
       </c>
       <c r="C132" s="8" t="s">
@@ -14483,7 +14437,7 @@
       <c r="A133" s="1">
         <v>131</v>
       </c>
-      <c r="B133" s="72"/>
+      <c r="B133" s="74"/>
       <c r="C133" s="8" t="s">
         <v>947</v>
       </c>
@@ -14629,7 +14583,7 @@
       <c r="A139" s="1">
         <v>137</v>
       </c>
-      <c r="B139" s="71" t="s">
+      <c r="B139" s="73" t="s">
         <v>964</v>
       </c>
       <c r="C139" s="8" t="s">
@@ -14653,7 +14607,7 @@
       <c r="A140" s="1">
         <v>138</v>
       </c>
-      <c r="B140" s="72"/>
+      <c r="B140" s="74"/>
       <c r="C140" s="8" t="s">
         <v>967</v>
       </c>
@@ -14678,6 +14632,41 @@
     </sortState>
   </autoFilter>
   <mergeCells count="45">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="B90:B92"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="B98:B100"/>
     <mergeCell ref="B101:B102"/>
     <mergeCell ref="B104:B107"/>
     <mergeCell ref="B109:B110"/>
@@ -14688,41 +14677,6 @@
     <mergeCell ref="B121:B123"/>
     <mergeCell ref="B125:B130"/>
     <mergeCell ref="B132:B133"/>
-    <mergeCell ref="B87:B89"/>
-    <mergeCell ref="B90:B92"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B65:B69"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -14731,16 +14685,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E61" sqref="E61"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="38.5703125" style="2" customWidth="1"/>
@@ -14757,19 +14711,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>969</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="78"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="80"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
@@ -14782,7 +14736,7 @@
         <v>617</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>1218</v>
+        <v>1204</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>551</v>
@@ -14810,20 +14764,20 @@
       <c r="A3" s="52">
         <v>1</v>
       </c>
-      <c r="B3" s="79" t="s">
-        <v>1200</v>
+      <c r="B3" s="81" t="s">
+        <v>1186</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>1215</v>
+        <v>1201</v>
       </c>
       <c r="D3" s="48">
         <v>43657</v>
       </c>
       <c r="E3" s="54" t="s">
-        <v>1129</v>
+        <v>1217</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>1173</v>
+        <v>1161</v>
       </c>
       <c r="G3" s="54"/>
       <c r="H3" s="55"/>
@@ -14835,18 +14789,18 @@
       <c r="A4" s="52">
         <v>2</v>
       </c>
-      <c r="B4" s="81"/>
+      <c r="B4" s="83"/>
       <c r="C4" s="47" t="s">
-        <v>1215</v>
+        <v>1201</v>
       </c>
       <c r="D4" s="48">
         <v>43657</v>
       </c>
       <c r="E4" s="54" t="s">
-        <v>1145</v>
+        <v>1218</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>1195</v>
+        <v>1182</v>
       </c>
       <c r="G4" s="54"/>
       <c r="H4" s="55"/>
@@ -14858,20 +14812,20 @@
       <c r="A5" s="52">
         <v>3</v>
       </c>
-      <c r="B5" s="79" t="s">
-        <v>1198</v>
+      <c r="B5" s="81" t="s">
+        <v>1185</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>1216</v>
+        <v>1202</v>
       </c>
       <c r="D5" s="48">
         <v>43664</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>1238</v>
+        <v>1214</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>1194</v>
+        <v>1181</v>
       </c>
       <c r="G5" s="52"/>
       <c r="H5" s="55"/>
@@ -14883,18 +14837,18 @@
       <c r="A6" s="52">
         <v>4</v>
       </c>
-      <c r="B6" s="80"/>
+      <c r="B6" s="82"/>
       <c r="C6" s="47" t="s">
-        <v>1216</v>
+        <v>1202</v>
       </c>
       <c r="D6" s="48">
         <v>43664</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>1227</v>
+        <v>1205</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="G6" s="52"/>
       <c r="H6" s="55"/>
@@ -14906,18 +14860,18 @@
       <c r="A7" s="52">
         <v>5</v>
       </c>
-      <c r="B7" s="80"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="47" t="s">
-        <v>1216</v>
+        <v>1202</v>
       </c>
       <c r="D7" s="48">
         <v>43664</v>
       </c>
       <c r="E7" s="46" t="s">
-        <v>1228</v>
+        <v>1206</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="G7" s="52"/>
       <c r="H7" s="55"/>
@@ -14929,18 +14883,18 @@
       <c r="A8" s="52">
         <v>6</v>
       </c>
-      <c r="B8" s="80"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="47" t="s">
-        <v>1216</v>
+        <v>1202</v>
       </c>
       <c r="D8" s="48">
         <v>43664</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>1229</v>
+        <v>1207</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
@@ -14952,18 +14906,18 @@
       <c r="A9" s="52">
         <v>7</v>
       </c>
-      <c r="B9" s="80"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="47" t="s">
-        <v>1216</v>
+        <v>1202</v>
       </c>
       <c r="D9" s="48">
         <v>43664</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>1230</v>
+        <v>1208</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="G9" s="52"/>
       <c r="H9" s="55"/>
@@ -14975,18 +14929,18 @@
       <c r="A10" s="52">
         <v>8</v>
       </c>
-      <c r="B10" s="80"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="47" t="s">
-        <v>1216</v>
+        <v>1202</v>
       </c>
       <c r="D10" s="48">
         <v>43664</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>1231</v>
+        <v>1209</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="G10" s="52"/>
       <c r="H10" s="55"/>
@@ -14994,22 +14948,22 @@
       <c r="J10" s="55"/>
       <c r="K10" s="55"/>
     </row>
-    <row r="11" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="52">
-        <v>9</v>
-      </c>
-      <c r="B11" s="80"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="82"/>
       <c r="C11" s="47" t="s">
-        <v>1216</v>
+        <v>1202</v>
       </c>
       <c r="D11" s="48">
         <v>43664</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>1232</v>
+        <v>1210</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>1169</v>
+        <v>1179</v>
       </c>
       <c r="G11" s="52"/>
       <c r="H11" s="55"/>
@@ -15017,22 +14971,22 @@
       <c r="J11" s="55"/>
       <c r="K11" s="55"/>
     </row>
-    <row r="12" spans="1:11" ht="28.5" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="52">
-        <v>10</v>
-      </c>
-      <c r="B12" s="80"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="82"/>
       <c r="C12" s="47" t="s">
-        <v>1216</v>
+        <v>1202</v>
       </c>
       <c r="D12" s="48">
         <v>43664</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>1233</v>
+        <v>1211</v>
       </c>
       <c r="F12" s="52" t="s">
-        <v>1191</v>
+        <v>1180</v>
       </c>
       <c r="G12" s="52"/>
       <c r="H12" s="55"/>
@@ -15042,20 +14996,20 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="52">
-        <v>11</v>
-      </c>
-      <c r="B13" s="80"/>
+        <v>13</v>
+      </c>
+      <c r="B13" s="82"/>
       <c r="C13" s="47" t="s">
-        <v>1216</v>
+        <v>1202</v>
       </c>
       <c r="D13" s="48">
         <v>43664</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>1234</v>
+        <v>1212</v>
       </c>
       <c r="F13" s="52" t="s">
-        <v>1192</v>
+        <v>1183</v>
       </c>
       <c r="G13" s="52"/>
       <c r="H13" s="55"/>
@@ -15063,22 +15017,22 @@
       <c r="J13" s="55"/>
       <c r="K13" s="55"/>
     </row>
-    <row r="14" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="52">
-        <v>12</v>
-      </c>
-      <c r="B14" s="80"/>
+        <v>14</v>
+      </c>
+      <c r="B14" s="83"/>
       <c r="C14" s="47" t="s">
-        <v>1216</v>
+        <v>1202</v>
       </c>
       <c r="D14" s="48">
         <v>43664</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>1235</v>
+        <v>1213</v>
       </c>
       <c r="F14" s="52" t="s">
-        <v>1193</v>
+        <v>1184</v>
       </c>
       <c r="G14" s="52"/>
       <c r="H14" s="55"/>
@@ -15086,22 +15040,24 @@
       <c r="J14" s="55"/>
       <c r="K14" s="55"/>
     </row>
-    <row r="15" spans="1:11" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="52">
-        <v>13</v>
-      </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="47" t="s">
-        <v>1216</v>
+        <v>15</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C15" s="52" t="s">
+        <v>1203</v>
       </c>
       <c r="D15" s="48">
-        <v>43664</v>
-      </c>
-      <c r="E15" s="46" t="s">
-        <v>1236</v>
+        <v>43670</v>
+      </c>
+      <c r="E15" s="54" t="s">
+        <v>1126</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>1196</v>
+        <v>1158</v>
       </c>
       <c r="G15" s="52"/>
       <c r="H15" s="55"/>
@@ -15111,20 +15067,22 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="52">
-        <v>14</v>
-      </c>
-      <c r="B16" s="81"/>
-      <c r="C16" s="47" t="s">
-        <v>1216</v>
-      </c>
-      <c r="D16" s="48">
-        <v>43664</v>
-      </c>
-      <c r="E16" s="46" t="s">
-        <v>1237</v>
-      </c>
-      <c r="F16" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="54" t="s">
         <v>1197</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D16" s="57">
+        <v>43654</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F16" s="59" t="s">
+        <v>1171</v>
       </c>
       <c r="G16" s="52"/>
       <c r="H16" s="55"/>
@@ -15134,22 +15092,22 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="52">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>1206</v>
+        <v>1198</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>1217</v>
+        <v>1203</v>
       </c>
       <c r="D17" s="48">
         <v>43670</v>
       </c>
       <c r="E17" s="54" t="s">
-        <v>1126</v>
+        <v>1136</v>
       </c>
       <c r="F17" s="52" t="s">
-        <v>1170</v>
+        <v>1172</v>
       </c>
       <c r="G17" s="52"/>
       <c r="H17" s="55"/>
@@ -15159,22 +15117,22 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="52">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18" s="54" t="s">
-        <v>1211</v>
-      </c>
-      <c r="C18" s="60" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D18" s="58">
-        <v>43654</v>
-      </c>
-      <c r="E18" s="59" t="s">
-        <v>1137</v>
-      </c>
-      <c r="F18" s="60" t="s">
-        <v>1183</v>
+        <v>448</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>1202</v>
+      </c>
+      <c r="D18" s="48">
+        <v>43664</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F18" s="52" t="s">
+        <v>1157</v>
       </c>
       <c r="G18" s="52"/>
       <c r="H18" s="55"/>
@@ -15184,22 +15142,22 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="52">
-        <v>17</v>
-      </c>
-      <c r="B19" s="54" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C19" s="52" t="s">
-        <v>1217</v>
-      </c>
-      <c r="D19" s="48">
-        <v>43670</v>
-      </c>
-      <c r="E19" s="54" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F19" s="52" t="s">
-        <v>1184</v>
+        <v>19</v>
+      </c>
+      <c r="B19" s="81" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C19" s="60" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D19" s="57">
+        <v>43664</v>
+      </c>
+      <c r="E19" s="58" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F19" s="85" t="s">
+        <v>1143</v>
       </c>
       <c r="G19" s="52"/>
       <c r="H19" s="55"/>
@@ -15209,22 +15167,20 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="52">
-        <v>18</v>
-      </c>
-      <c r="B20" s="54" t="s">
-        <v>448</v>
-      </c>
-      <c r="C20" s="47" t="s">
-        <v>1216</v>
-      </c>
-      <c r="D20" s="48">
+        <v>20</v>
+      </c>
+      <c r="B20" s="82"/>
+      <c r="C20" s="60" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D20" s="57">
         <v>43664</v>
       </c>
-      <c r="E20" s="54" t="s">
-        <v>1125</v>
-      </c>
-      <c r="F20" s="52" t="s">
-        <v>1168</v>
+      <c r="E20" s="58" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F20" s="85" t="s">
+        <v>1149</v>
       </c>
       <c r="G20" s="52"/>
       <c r="H20" s="55"/>
@@ -15234,22 +15190,20 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="52">
-        <v>19</v>
-      </c>
-      <c r="B21" s="79" t="s">
-        <v>1202</v>
-      </c>
-      <c r="C21" s="53" t="s">
-        <v>1216</v>
-      </c>
-      <c r="D21" s="48">
-        <v>43664</v>
-      </c>
-      <c r="E21" s="56" t="s">
-        <v>1116</v>
-      </c>
-      <c r="F21" s="52" t="s">
-        <v>1146</v>
+        <v>21</v>
+      </c>
+      <c r="B21" s="82"/>
+      <c r="C21" s="60" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D21" s="57">
+        <v>43657</v>
+      </c>
+      <c r="E21" s="58" t="s">
+        <v>1118</v>
+      </c>
+      <c r="F21" s="85" t="s">
+        <v>1150</v>
       </c>
       <c r="G21" s="52"/>
       <c r="H21" s="55"/>
@@ -15259,20 +15213,20 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="52">
-        <v>20</v>
-      </c>
-      <c r="B22" s="80"/>
-      <c r="C22" s="53" t="s">
-        <v>1216</v>
-      </c>
-      <c r="D22" s="48">
-        <v>43664</v>
-      </c>
-      <c r="E22" s="56" t="s">
-        <v>1117</v>
-      </c>
-      <c r="F22" s="52" t="s">
-        <v>1152</v>
+        <v>22</v>
+      </c>
+      <c r="B22" s="82"/>
+      <c r="C22" s="60" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D22" s="57">
+        <v>43657</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F22" s="85" t="s">
+        <v>1151</v>
       </c>
       <c r="G22" s="52"/>
       <c r="H22" s="55"/>
@@ -15282,20 +15236,20 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="52">
-        <v>21</v>
-      </c>
-      <c r="B23" s="80"/>
-      <c r="C23" s="53" t="s">
-        <v>1215</v>
-      </c>
-      <c r="D23" s="48">
+        <v>23</v>
+      </c>
+      <c r="B23" s="82"/>
+      <c r="C23" s="60" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D23" s="57">
         <v>43657</v>
       </c>
-      <c r="E23" s="54" t="s">
-        <v>1118</v>
-      </c>
-      <c r="F23" s="52" t="s">
-        <v>1153</v>
+      <c r="E23" s="58" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F23" s="85" t="s">
+        <v>1162</v>
       </c>
       <c r="G23" s="52"/>
       <c r="H23" s="55"/>
@@ -15303,22 +15257,20 @@
       <c r="J23" s="55"/>
       <c r="K23" s="55"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="52">
-        <v>22</v>
-      </c>
-      <c r="B24" s="80"/>
-      <c r="C24" s="53" t="s">
-        <v>1215</v>
-      </c>
-      <c r="D24" s="48">
+    <row r="24" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="52"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="60" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D24" s="57">
         <v>43657</v>
       </c>
-      <c r="E24" s="54" t="s">
-        <v>1119</v>
-      </c>
-      <c r="F24" s="52" t="s">
-        <v>1154</v>
+      <c r="E24" s="86" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F24" s="85" t="s">
+        <v>1219</v>
       </c>
       <c r="G24" s="52"/>
       <c r="H24" s="55"/>
@@ -15328,20 +15280,20 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="52">
-        <v>23</v>
-      </c>
-      <c r="B25" s="80"/>
-      <c r="C25" s="53" t="s">
-        <v>1215</v>
-      </c>
-      <c r="D25" s="48">
+        <v>24</v>
+      </c>
+      <c r="B25" s="83"/>
+      <c r="C25" s="59" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D25" s="57">
         <v>43657</v>
       </c>
-      <c r="E25" s="54" t="s">
-        <v>1208</v>
-      </c>
-      <c r="F25" s="52" t="s">
-        <v>1174</v>
+      <c r="E25" s="58" t="s">
+        <v>1195</v>
+      </c>
+      <c r="F25" s="85" t="s">
+        <v>1163</v>
       </c>
       <c r="G25" s="52"/>
       <c r="H25" s="55"/>
@@ -15351,20 +15303,22 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="52">
-        <v>24</v>
-      </c>
-      <c r="B26" s="81"/>
-      <c r="C26" s="52" t="s">
-        <v>1215</v>
+        <v>25</v>
+      </c>
+      <c r="B26" s="81" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C26" s="53" t="s">
+        <v>1202</v>
       </c>
       <c r="D26" s="48">
-        <v>43657</v>
-      </c>
-      <c r="E26" s="54" t="s">
-        <v>1209</v>
+        <v>43664</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>1137</v>
       </c>
       <c r="F26" s="52" t="s">
-        <v>1175</v>
+        <v>1164</v>
       </c>
       <c r="G26" s="52"/>
       <c r="H26" s="55"/>
@@ -15374,22 +15328,20 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="52">
-        <v>25</v>
-      </c>
-      <c r="B27" s="79" t="s">
-        <v>1210</v>
-      </c>
-      <c r="C27" s="53" t="s">
-        <v>1216</v>
+        <v>26</v>
+      </c>
+      <c r="B27" s="83"/>
+      <c r="C27" s="47" t="s">
+        <v>1202</v>
       </c>
       <c r="D27" s="48">
         <v>43664</v>
       </c>
-      <c r="E27" s="54" t="s">
-        <v>1130</v>
-      </c>
-      <c r="F27" s="52" t="s">
-        <v>1176</v>
+      <c r="E27" s="33" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F27" s="84" t="s">
+        <v>1173</v>
       </c>
       <c r="G27" s="52"/>
       <c r="H27" s="55"/>
@@ -15399,20 +15351,22 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="52">
-        <v>26</v>
-      </c>
-      <c r="B28" s="81"/>
-      <c r="C28" s="47" t="s">
-        <v>1216</v>
-      </c>
-      <c r="D28" s="48">
-        <v>43664</v>
-      </c>
-      <c r="E28" s="54" t="s">
-        <v>1139</v>
-      </c>
-      <c r="F28" s="52" t="s">
-        <v>1185</v>
+        <v>27</v>
+      </c>
+      <c r="B28" s="81" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C28" s="60" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D28" s="57">
+        <v>43657</v>
+      </c>
+      <c r="E28" s="58" t="s">
+        <v>1120</v>
+      </c>
+      <c r="F28" s="85" t="s">
+        <v>1152</v>
       </c>
       <c r="G28" s="52"/>
       <c r="H28" s="55"/>
@@ -15422,22 +15376,20 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="52">
-        <v>27</v>
-      </c>
-      <c r="B29" s="79" t="s">
-        <v>1203</v>
-      </c>
-      <c r="C29" s="53" t="s">
-        <v>1215</v>
-      </c>
-      <c r="D29" s="48">
+        <v>28</v>
+      </c>
+      <c r="B29" s="83"/>
+      <c r="C29" s="59" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D29" s="57">
         <v>43657</v>
       </c>
-      <c r="E29" s="54" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F29" s="64" t="s">
-        <v>1155</v>
+      <c r="E29" s="58" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F29" s="85" t="s">
+        <v>1165</v>
       </c>
       <c r="G29" s="52"/>
       <c r="H29" s="55"/>
@@ -15447,20 +15399,22 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="52">
-        <v>28</v>
-      </c>
-      <c r="B30" s="81"/>
-      <c r="C30" s="52" t="s">
-        <v>1215</v>
-      </c>
-      <c r="D30" s="48">
-        <v>43657</v>
-      </c>
-      <c r="E30" s="54" t="s">
-        <v>1131</v>
-      </c>
-      <c r="F30" s="52" t="s">
-        <v>1177</v>
+        <v>29</v>
+      </c>
+      <c r="B30" s="81" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C30" s="60" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D30" s="57">
+        <v>43654</v>
+      </c>
+      <c r="E30" s="58" t="s">
+        <v>1121</v>
+      </c>
+      <c r="F30" s="59" t="s">
+        <v>1153</v>
       </c>
       <c r="G30" s="52"/>
       <c r="H30" s="55"/>
@@ -15470,22 +15424,20 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="52">
-        <v>29</v>
-      </c>
-      <c r="B31" s="79" t="s">
-        <v>1204</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B31" s="82"/>
       <c r="C31" s="61" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D31" s="58">
+        <v>1200</v>
+      </c>
+      <c r="D31" s="57">
         <v>43654</v>
       </c>
-      <c r="E31" s="59" t="s">
-        <v>1121</v>
-      </c>
-      <c r="F31" s="60" t="s">
-        <v>1156</v>
+      <c r="E31" s="58" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F31" s="59" t="s">
+        <v>1154</v>
       </c>
       <c r="G31" s="52"/>
       <c r="H31" s="55"/>
@@ -15495,20 +15447,20 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="52">
-        <v>30</v>
-      </c>
-      <c r="B32" s="80"/>
-      <c r="C32" s="62" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D32" s="58">
+        <v>31</v>
+      </c>
+      <c r="B32" s="82"/>
+      <c r="C32" s="61" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D32" s="57">
         <v>43654</v>
       </c>
-      <c r="E32" s="59" t="s">
-        <v>1122</v>
-      </c>
-      <c r="F32" s="60" t="s">
-        <v>1157</v>
+      <c r="E32" s="58" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F32" s="59" t="s">
+        <v>1166</v>
       </c>
       <c r="G32" s="52"/>
       <c r="H32" s="55"/>
@@ -15518,20 +15470,20 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="52">
-        <v>31</v>
-      </c>
-      <c r="B33" s="80"/>
-      <c r="C33" s="62" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D33" s="58">
+        <v>32</v>
+      </c>
+      <c r="B33" s="82"/>
+      <c r="C33" s="61" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D33" s="57">
         <v>43654</v>
       </c>
-      <c r="E33" s="59" t="s">
-        <v>1132</v>
-      </c>
-      <c r="F33" s="60" t="s">
-        <v>1178</v>
+      <c r="E33" s="58" t="s">
+        <v>1131</v>
+      </c>
+      <c r="F33" s="59" t="s">
+        <v>1167</v>
       </c>
       <c r="G33" s="52"/>
       <c r="H33" s="55"/>
@@ -15540,21 +15492,19 @@
       <c r="K33" s="55"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="52">
-        <v>32</v>
-      </c>
-      <c r="B34" s="80"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="82"/>
       <c r="C34" s="62" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D34" s="58">
+        <v>1200</v>
+      </c>
+      <c r="D34" s="63">
         <v>43654</v>
       </c>
-      <c r="E34" s="59" t="s">
-        <v>1133</v>
-      </c>
-      <c r="F34" s="60" t="s">
-        <v>1179</v>
+      <c r="E34" s="64" t="s">
+        <v>1215</v>
+      </c>
+      <c r="F34" s="65" t="s">
+        <v>1216</v>
       </c>
       <c r="G34" s="52"/>
       <c r="H34" s="55"/>
@@ -15563,19 +15513,21 @@
       <c r="K34" s="55"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="52"/>
-      <c r="B35" s="80"/>
-      <c r="C35" s="82" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D35" s="83">
+      <c r="A35" s="52">
+        <v>33</v>
+      </c>
+      <c r="B35" s="83"/>
+      <c r="C35" s="61" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D35" s="57">
         <v>43654</v>
       </c>
-      <c r="E35" s="84" t="s">
-        <v>1239</v>
-      </c>
-      <c r="F35" s="85" t="s">
-        <v>1240</v>
+      <c r="E35" s="58" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F35" s="59" t="s">
+        <v>1168</v>
       </c>
       <c r="G35" s="52"/>
       <c r="H35" s="55"/>
@@ -15585,20 +15537,22 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="52">
-        <v>33</v>
-      </c>
-      <c r="B36" s="81"/>
-      <c r="C36" s="62" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D36" s="58">
-        <v>43654</v>
-      </c>
-      <c r="E36" s="59" t="s">
-        <v>1134</v>
-      </c>
-      <c r="F36" s="60" t="s">
-        <v>1180</v>
+        <v>34</v>
+      </c>
+      <c r="B36" s="81" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C36" s="56" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D36" s="57">
+        <v>43647</v>
+      </c>
+      <c r="E36" s="58" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F36" s="59" t="s">
+        <v>1155</v>
       </c>
       <c r="G36" s="52"/>
       <c r="H36" s="55"/>
@@ -15608,22 +15562,20 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="52">
-        <v>34</v>
-      </c>
-      <c r="B37" s="79" t="s">
-        <v>1205</v>
-      </c>
-      <c r="C37" s="57" t="s">
-        <v>1213</v>
-      </c>
-      <c r="D37" s="58">
+        <v>35</v>
+      </c>
+      <c r="B37" s="82"/>
+      <c r="C37" s="56" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D37" s="57">
         <v>43647</v>
       </c>
-      <c r="E37" s="59" t="s">
-        <v>1123</v>
-      </c>
-      <c r="F37" s="60" t="s">
-        <v>1158</v>
+      <c r="E37" s="58" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F37" s="59" t="s">
+        <v>1156</v>
       </c>
       <c r="G37" s="52"/>
       <c r="H37" s="55"/>
@@ -15633,20 +15585,20 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="52">
-        <v>35</v>
-      </c>
-      <c r="B38" s="80"/>
-      <c r="C38" s="57" t="s">
-        <v>1213</v>
-      </c>
-      <c r="D38" s="58">
+        <v>36</v>
+      </c>
+      <c r="B38" s="82"/>
+      <c r="C38" s="56" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D38" s="57">
         <v>43647</v>
       </c>
-      <c r="E38" s="59" t="s">
-        <v>1124</v>
-      </c>
-      <c r="F38" s="60" t="s">
-        <v>1159</v>
+      <c r="E38" s="58" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F38" s="59" t="s">
+        <v>1169</v>
       </c>
       <c r="G38" s="52"/>
       <c r="H38" s="55"/>
@@ -15656,20 +15608,20 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="52">
-        <v>36</v>
-      </c>
-      <c r="B39" s="80"/>
-      <c r="C39" s="57" t="s">
-        <v>1213</v>
-      </c>
-      <c r="D39" s="58">
+        <v>37</v>
+      </c>
+      <c r="B39" s="83"/>
+      <c r="C39" s="56" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D39" s="57">
         <v>43647</v>
       </c>
-      <c r="E39" s="59" t="s">
-        <v>1135</v>
-      </c>
-      <c r="F39" s="60" t="s">
-        <v>1181</v>
+      <c r="E39" s="58" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F39" s="59" t="s">
+        <v>1170</v>
       </c>
       <c r="G39" s="52"/>
       <c r="H39" s="55"/>
@@ -15679,20 +15631,22 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="52">
-        <v>37</v>
-      </c>
-      <c r="B40" s="81"/>
-      <c r="C40" s="57" t="s">
-        <v>1213</v>
-      </c>
-      <c r="D40" s="58">
-        <v>43647</v>
-      </c>
-      <c r="E40" s="59" t="s">
-        <v>1136</v>
-      </c>
-      <c r="F40" s="60" t="s">
-        <v>1182</v>
+        <v>38</v>
+      </c>
+      <c r="B40" s="81" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C40" s="53" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D40" s="48">
+        <v>43657</v>
+      </c>
+      <c r="E40" s="54" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F40" s="52" t="s">
+        <v>1159</v>
       </c>
       <c r="G40" s="52"/>
       <c r="H40" s="55"/>
@@ -15702,22 +15656,20 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="52">
-        <v>38</v>
-      </c>
-      <c r="B41" s="79" t="s">
-        <v>1207</v>
-      </c>
-      <c r="C41" s="53" t="s">
-        <v>1215</v>
+        <v>39</v>
+      </c>
+      <c r="B41" s="83"/>
+      <c r="C41" s="47" t="s">
+        <v>1201</v>
       </c>
       <c r="D41" s="48">
         <v>43657</v>
       </c>
       <c r="E41" s="54" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="F41" s="52" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="G41" s="52"/>
       <c r="H41" s="55"/>
@@ -15727,20 +15679,22 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="52">
-        <v>39</v>
-      </c>
-      <c r="B42" s="81"/>
-      <c r="C42" s="47" t="s">
-        <v>1215</v>
-      </c>
-      <c r="D42" s="48">
-        <v>43657</v>
-      </c>
-      <c r="E42" s="54" t="s">
-        <v>1128</v>
-      </c>
-      <c r="F42" s="52" t="s">
-        <v>1172</v>
+        <v>40</v>
+      </c>
+      <c r="B42" s="52" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C42" s="61" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D42" s="57">
+        <v>43654</v>
+      </c>
+      <c r="E42" s="58" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F42" s="59" t="s">
+        <v>1178</v>
       </c>
       <c r="G42" s="52"/>
       <c r="H42" s="55"/>
@@ -15748,24 +15702,22 @@
       <c r="J42" s="55"/>
       <c r="K42" s="55"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="52">
-        <v>40</v>
-      </c>
-      <c r="B43" s="52" t="s">
-        <v>1201</v>
-      </c>
-      <c r="C43" s="62" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D43" s="58">
-        <v>43654</v>
-      </c>
-      <c r="E43" s="59" t="s">
-        <v>1144</v>
-      </c>
-      <c r="F43" s="60" t="s">
-        <v>1190</v>
+        <v>49</v>
+      </c>
+      <c r="B43" s="82"/>
+      <c r="C43" s="56" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D43" s="57">
+        <v>43647</v>
+      </c>
+      <c r="E43" s="58" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F43" s="59" t="s">
+        <v>1174</v>
       </c>
       <c r="G43" s="52"/>
       <c r="H43" s="55"/>
@@ -15773,20 +15725,22 @@
       <c r="J43" s="55"/>
       <c r="K43" s="55"/>
     </row>
-    <row r="44" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="52">
-        <v>41</v>
-      </c>
-      <c r="B44" s="79" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="82"/>
+      <c r="C44" s="56" t="s">
         <v>1199</v>
       </c>
-      <c r="C44" s="63"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="54" t="s">
-        <v>1226</v>
-      </c>
-      <c r="F44" s="52" t="s">
-        <v>1160</v>
+      <c r="D44" s="57">
+        <v>43647</v>
+      </c>
+      <c r="E44" s="58" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F44" s="59" t="s">
+        <v>1175</v>
       </c>
       <c r="G44" s="52"/>
       <c r="H44" s="55"/>
@@ -15794,18 +15748,22 @@
       <c r="J44" s="55"/>
       <c r="K44" s="55"/>
     </row>
-    <row r="45" spans="1:11" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="52">
-        <v>42</v>
-      </c>
-      <c r="B45" s="80"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="58"/>
-      <c r="E45" s="54" t="s">
-        <v>1225</v>
-      </c>
-      <c r="F45" s="52" t="s">
-        <v>1161</v>
+        <v>51</v>
+      </c>
+      <c r="B45" s="82"/>
+      <c r="C45" s="56" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D45" s="57">
+        <v>43647</v>
+      </c>
+      <c r="E45" s="58" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F45" s="59" t="s">
+        <v>1176</v>
       </c>
       <c r="G45" s="52"/>
       <c r="H45" s="55"/>
@@ -15813,18 +15771,22 @@
       <c r="J45" s="55"/>
       <c r="K45" s="55"/>
     </row>
-    <row r="46" spans="1:11" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="52">
-        <v>43</v>
-      </c>
-      <c r="B46" s="80"/>
-      <c r="C46" s="63"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="54" t="s">
-        <v>1224</v>
-      </c>
-      <c r="F46" s="52" t="s">
-        <v>1162</v>
+        <v>52</v>
+      </c>
+      <c r="B46" s="83"/>
+      <c r="C46" s="56" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D46" s="57">
+        <v>43647</v>
+      </c>
+      <c r="E46" s="58" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F46" s="59" t="s">
+        <v>1177</v>
       </c>
       <c r="G46" s="52"/>
       <c r="H46" s="55"/>
@@ -15832,209 +15794,25 @@
       <c r="J46" s="55"/>
       <c r="K46" s="55"/>
     </row>
-    <row r="47" spans="1:11" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="52">
-        <v>44</v>
-      </c>
-      <c r="B47" s="80"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="54" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F47" s="52" t="s">
-        <v>1163</v>
-      </c>
-      <c r="G47" s="52"/>
-      <c r="H47" s="55"/>
-      <c r="I47" s="55"/>
-      <c r="J47" s="55"/>
-      <c r="K47" s="55"/>
-    </row>
-    <row r="48" spans="1:11" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="52">
-        <v>45</v>
-      </c>
-      <c r="B48" s="80"/>
-      <c r="C48" s="63"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="54" t="s">
-        <v>1222</v>
-      </c>
-      <c r="F48" s="52" t="s">
-        <v>1164</v>
-      </c>
-      <c r="G48" s="52"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="55"/>
-      <c r="J48" s="55"/>
-      <c r="K48" s="55"/>
-    </row>
-    <row r="49" spans="1:11" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="52">
-        <v>46</v>
-      </c>
-      <c r="B49" s="80"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="54" t="s">
-        <v>1221</v>
-      </c>
-      <c r="F49" s="52" t="s">
-        <v>1165</v>
-      </c>
-      <c r="G49" s="52"/>
-      <c r="H49" s="55"/>
-      <c r="I49" s="55"/>
-      <c r="J49" s="55"/>
-      <c r="K49" s="55"/>
-    </row>
-    <row r="50" spans="1:11" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="52">
-        <v>47</v>
-      </c>
-      <c r="B50" s="80"/>
-      <c r="C50" s="63"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="54" t="s">
-        <v>1220</v>
-      </c>
-      <c r="F50" s="52" t="s">
-        <v>1166</v>
-      </c>
-      <c r="G50" s="52"/>
-      <c r="H50" s="55"/>
-      <c r="I50" s="55"/>
-      <c r="J50" s="55"/>
-      <c r="K50" s="55"/>
-    </row>
-    <row r="51" spans="1:11" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="52">
-        <v>48</v>
-      </c>
-      <c r="B51" s="80"/>
-      <c r="C51" s="63"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="54" t="s">
-        <v>1219</v>
-      </c>
-      <c r="F51" s="52" t="s">
-        <v>1167</v>
-      </c>
-      <c r="G51" s="52"/>
-      <c r="H51" s="55"/>
-      <c r="I51" s="55"/>
-      <c r="J51" s="55"/>
-      <c r="K51" s="55"/>
-    </row>
-    <row r="52" spans="1:11" ht="14.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="52">
-        <v>49</v>
-      </c>
-      <c r="B52" s="80"/>
-      <c r="C52" s="57" t="s">
-        <v>1213</v>
-      </c>
-      <c r="D52" s="58">
-        <v>43647</v>
-      </c>
-      <c r="E52" s="59" t="s">
-        <v>1140</v>
-      </c>
-      <c r="F52" s="60" t="s">
-        <v>1186</v>
-      </c>
-      <c r="G52" s="52"/>
-      <c r="H52" s="55"/>
-      <c r="I52" s="55"/>
-      <c r="J52" s="55"/>
-      <c r="K52" s="55"/>
-    </row>
-    <row r="53" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="52">
-        <v>50</v>
-      </c>
-      <c r="B53" s="80"/>
-      <c r="C53" s="57" t="s">
-        <v>1213</v>
-      </c>
-      <c r="D53" s="58">
-        <v>43647</v>
-      </c>
-      <c r="E53" s="59" t="s">
-        <v>1141</v>
-      </c>
-      <c r="F53" s="60" t="s">
-        <v>1187</v>
-      </c>
-      <c r="G53" s="52"/>
-      <c r="H53" s="55"/>
-      <c r="I53" s="55"/>
-      <c r="J53" s="55"/>
-      <c r="K53" s="55"/>
-    </row>
-    <row r="54" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="52">
-        <v>51</v>
-      </c>
-      <c r="B54" s="80"/>
-      <c r="C54" s="57" t="s">
-        <v>1213</v>
-      </c>
-      <c r="D54" s="58">
-        <v>43647</v>
-      </c>
-      <c r="E54" s="59" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F54" s="60" t="s">
-        <v>1188</v>
-      </c>
-      <c r="G54" s="52"/>
-      <c r="H54" s="55"/>
-      <c r="I54" s="55"/>
-      <c r="J54" s="55"/>
-      <c r="K54" s="55"/>
-    </row>
-    <row r="55" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="52">
-        <v>52</v>
-      </c>
-      <c r="B55" s="81"/>
-      <c r="C55" s="57" t="s">
-        <v>1213</v>
-      </c>
-      <c r="D55" s="58">
-        <v>43647</v>
-      </c>
-      <c r="E55" s="59" t="s">
-        <v>1143</v>
-      </c>
-      <c r="F55" s="60" t="s">
-        <v>1189</v>
-      </c>
-      <c r="G55" s="52"/>
-      <c r="H55" s="55"/>
-      <c r="I55" s="55"/>
-      <c r="J55" s="55"/>
-      <c r="K55" s="55"/>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E57" s="66"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:K55" xr:uid="{C6B0F034-955C-4BFB-9151-0B32E8F7F8DB}"/>
-  <sortState ref="A3:K55">
-    <sortCondition ref="B3:B55"/>
+  <autoFilter ref="A2:K46" xr:uid="{C6B0F034-955C-4BFB-9151-0B32E8F7F8DB}"/>
+  <sortState ref="A3:K46">
+    <sortCondition ref="B3:B46"/>
   </sortState>
   <mergeCells count="10">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="B44:B55"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="B43:B46"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B16"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B5:B14"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B40:B41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -16042,6 +15820,41 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16248,42 +16061,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7F7E23-FE37-4AB8-A4B3-5025B5D9E450}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16300,29 +16103,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated status tracking file for status tracking for Partner Management
</commit_message>
<xml_diff>
--- a/_files/requirements/requirements_detailing_references/Partner Management/Pending_Backlog_Stories_Status Tracking.xlsx
+++ b/_files/requirements/requirements_detailing_references/Partner Management/Pending_Backlog_Stories_Status Tracking.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\Project\PMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP wiki Open Source\Requirements\_files\requirements\requirements_detailing_references\Partner Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{66B78959-4FD4-4345-A1B5-1D137DEFF9D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CA984C9F-169D-4C46-A306-4CBB4E669A3D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3634,12 +3634,6 @@
     <t>As the MOSIP system- PM, I should be able to integrate with IDA to provide IDA requested services</t>
   </si>
   <si>
-    <t>As the MOSIP system, I should be able to retrieve Public key from Partners for encryption of e-kyc response</t>
-  </si>
-  <si>
-    <t>As the MOSIP system, I should be able to distribute Public Key to Partners for Encryption of auth/KYC Request</t>
-  </si>
-  <si>
     <t>As the Partner Manager, I should be able to deactivate Auth/E-KYC Partners</t>
   </si>
   <si>
@@ -3874,12 +3868,6 @@
     <t xml:space="preserve">As the MOSIP system, I should be able to generate Partner api key </t>
   </si>
   <si>
-    <t>As the MOSIP system , I should be able to generate Partner Manager ID</t>
-  </si>
-  <si>
-    <t>As the MOSIP system, I should be able to generate Policy Manager ID</t>
-  </si>
-  <si>
     <t>As the MOSIP system, I should be able to generate MISP ID</t>
   </si>
   <si>
@@ -3917,13 +3905,63 @@
   </si>
   <si>
     <t>As the MOSIP system - IDA, I should be able to validate MISP License key</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As the MOSIP system, I should be able to generate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Partner</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Manager ID</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As the MOSIP system , I should be able to generate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Policy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Manager ID</t>
+    </r>
+  </si>
+  <si>
+    <t>As the MOSIP system, I should be able to retrieve Public key from Partners for encryption of e-kyc response [To be deleted]</t>
+  </si>
+  <si>
+    <t>As the MOSIP system, I should be able to distribute Public Key to Partners for Encryption of auth/KYC Request [To be deleted]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4140,6 +4178,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Cambria"/>
       <family val="1"/>
     </font>
@@ -4599,7 +4643,7 @@
     <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4787,6 +4831,15 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4838,14 +4891,14 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -5225,12 +5278,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="70" t="s">
         <v>984</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="69"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="72"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -5779,17 +5832,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="69"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="72"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -5824,7 +5877,7 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -5851,7 +5904,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="71"/>
+      <c r="B4" s="74"/>
       <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
@@ -5876,7 +5929,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="71"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
@@ -5901,7 +5954,7 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="71"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
@@ -5926,7 +5979,7 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="71"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
@@ -5953,7 +6006,7 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="72"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="6" t="s">
         <v>30</v>
       </c>
@@ -6181,7 +6234,7 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="73" t="s">
         <v>67</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -6208,7 +6261,7 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="72"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="6" t="s">
         <v>71</v>
       </c>
@@ -6233,7 +6286,7 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="73" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -6260,7 +6313,7 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="72"/>
+      <c r="B19" s="75"/>
       <c r="C19" s="6" t="s">
         <v>64</v>
       </c>
@@ -6382,17 +6435,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="69"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="72"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -6454,7 +6507,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="76" t="s">
         <v>1020</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -6481,7 +6534,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="74"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="6" t="s">
         <v>92</v>
       </c>
@@ -6730,7 +6783,7 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="76" t="s">
         <v>1055</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -6759,7 +6812,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="74"/>
+      <c r="B15" s="77"/>
       <c r="C15" s="6" t="s">
         <v>121</v>
       </c>
@@ -6948,7 +7001,7 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="76" t="s">
         <v>1038</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -6975,7 +7028,7 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="75"/>
+      <c r="B23" s="78"/>
       <c r="C23" s="6" t="s">
         <v>185</v>
       </c>
@@ -7000,7 +7053,7 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="74"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="6" t="s">
         <v>188</v>
       </c>
@@ -7164,7 +7217,7 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="73" t="s">
+      <c r="B30" s="76" t="s">
         <v>1057</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -7193,7 +7246,7 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="74"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="6" t="s">
         <v>142</v>
       </c>
@@ -7220,7 +7273,7 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="73" t="s">
+      <c r="B32" s="76" t="s">
         <v>1058</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -7249,7 +7302,7 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="74"/>
+      <c r="B33" s="77"/>
       <c r="C33" s="6" t="s">
         <v>147</v>
       </c>
@@ -7473,7 +7526,7 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="73" t="s">
+      <c r="B41" s="76" t="s">
         <v>194</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -7502,7 +7555,7 @@
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="74"/>
+      <c r="B42" s="77"/>
       <c r="C42" s="6" t="s">
         <v>197</v>
       </c>
@@ -7556,7 +7609,7 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="73" t="s">
+      <c r="B44" s="76" t="s">
         <v>1034</v>
       </c>
       <c r="C44" s="6" t="s">
@@ -7585,7 +7638,7 @@
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" s="74"/>
+      <c r="B45" s="77"/>
       <c r="C45" s="6" t="s">
         <v>208</v>
       </c>
@@ -7668,7 +7721,7 @@
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="73" t="s">
+      <c r="B48" s="76" t="s">
         <v>222</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -7689,7 +7742,7 @@
       <c r="H48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I48" s="70" t="s">
+      <c r="I48" s="73" t="s">
         <v>1000</v>
       </c>
     </row>
@@ -7697,7 +7750,7 @@
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" s="75"/>
+      <c r="B49" s="78"/>
       <c r="C49" s="6" t="s">
         <v>226</v>
       </c>
@@ -7716,13 +7769,13 @@
       <c r="H49" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I49" s="71"/>
+      <c r="I49" s="74"/>
     </row>
     <row r="50" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="75"/>
+      <c r="B50" s="78"/>
       <c r="C50" s="6" t="s">
         <v>229</v>
       </c>
@@ -7741,13 +7794,13 @@
       <c r="H50" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I50" s="71"/>
+      <c r="I50" s="74"/>
     </row>
     <row r="51" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" s="75"/>
+      <c r="B51" s="78"/>
       <c r="C51" s="6" t="s">
         <v>232</v>
       </c>
@@ -7766,13 +7819,13 @@
       <c r="H51" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I51" s="71"/>
+      <c r="I51" s="74"/>
     </row>
     <row r="52" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" s="75"/>
+      <c r="B52" s="78"/>
       <c r="C52" s="6" t="s">
         <v>235</v>
       </c>
@@ -7791,13 +7844,13 @@
       <c r="H52" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I52" s="71"/>
+      <c r="I52" s="74"/>
     </row>
     <row r="53" spans="1:9" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="B53" s="75"/>
+      <c r="B53" s="78"/>
       <c r="C53" s="6" t="s">
         <v>238</v>
       </c>
@@ -7816,13 +7869,13 @@
       <c r="H53" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I53" s="71"/>
+      <c r="I53" s="74"/>
     </row>
     <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54" s="75"/>
+      <c r="B54" s="78"/>
       <c r="C54" s="6" t="s">
         <v>241</v>
       </c>
@@ -7841,13 +7894,13 @@
       <c r="H54" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I54" s="71"/>
+      <c r="I54" s="74"/>
     </row>
     <row r="55" spans="1:9" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55" s="75"/>
+      <c r="B55" s="78"/>
       <c r="C55" s="6" t="s">
         <v>244</v>
       </c>
@@ -7866,13 +7919,13 @@
       <c r="H55" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I55" s="71"/>
+      <c r="I55" s="74"/>
     </row>
     <row r="56" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56" s="75"/>
+      <c r="B56" s="78"/>
       <c r="C56" s="6" t="s">
         <v>1041</v>
       </c>
@@ -7887,13 +7940,13 @@
         <v>987</v>
       </c>
       <c r="H56" s="4"/>
-      <c r="I56" s="71"/>
+      <c r="I56" s="74"/>
     </row>
     <row r="57" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57" s="74"/>
+      <c r="B57" s="77"/>
       <c r="C57" s="6" t="s">
         <v>247</v>
       </c>
@@ -7912,13 +7965,13 @@
       <c r="H57" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I57" s="72"/>
+      <c r="I57" s="75"/>
     </row>
     <row r="58" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58" s="73" t="s">
+      <c r="B58" s="76" t="s">
         <v>222</v>
       </c>
       <c r="C58" s="6" t="s">
@@ -7939,7 +7992,7 @@
       <c r="H58" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I58" s="70" t="s">
+      <c r="I58" s="73" t="s">
         <v>1000</v>
       </c>
     </row>
@@ -7947,7 +8000,7 @@
       <c r="A59" s="1">
         <v>57</v>
       </c>
-      <c r="B59" s="75"/>
+      <c r="B59" s="78"/>
       <c r="C59" s="6" t="s">
         <v>253</v>
       </c>
@@ -7966,13 +8019,13 @@
       <c r="H59" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I59" s="71"/>
+      <c r="I59" s="74"/>
     </row>
     <row r="60" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
-      <c r="B60" s="75"/>
+      <c r="B60" s="78"/>
       <c r="C60" s="6" t="s">
         <v>256</v>
       </c>
@@ -7991,13 +8044,13 @@
       <c r="H60" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I60" s="71"/>
+      <c r="I60" s="74"/>
     </row>
     <row r="61" spans="1:9" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61" s="75"/>
+      <c r="B61" s="78"/>
       <c r="C61" s="6" t="s">
         <v>259</v>
       </c>
@@ -8016,13 +8069,13 @@
       <c r="H61" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I61" s="71"/>
+      <c r="I61" s="74"/>
     </row>
     <row r="62" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" s="75"/>
+      <c r="B62" s="78"/>
       <c r="C62" s="6" t="s">
         <v>262</v>
       </c>
@@ -8041,13 +8094,13 @@
       <c r="H62" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I62" s="71"/>
+      <c r="I62" s="74"/>
     </row>
     <row r="63" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" s="75"/>
+      <c r="B63" s="78"/>
       <c r="C63" s="6" t="s">
         <v>264</v>
       </c>
@@ -8066,13 +8119,13 @@
       <c r="H63" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I63" s="71"/>
+      <c r="I63" s="74"/>
     </row>
     <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" s="75"/>
+      <c r="B64" s="78"/>
       <c r="C64" s="6" t="s">
         <v>75</v>
       </c>
@@ -8091,13 +8144,13 @@
       <c r="H64" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I64" s="71"/>
+      <c r="I64" s="74"/>
     </row>
     <row r="65" spans="1:9" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" s="75"/>
+      <c r="B65" s="78"/>
       <c r="C65" s="6" t="s">
         <v>268</v>
       </c>
@@ -8116,13 +8169,13 @@
       <c r="H65" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I65" s="71"/>
+      <c r="I65" s="74"/>
     </row>
     <row r="66" spans="1:9" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" s="75"/>
+      <c r="B66" s="78"/>
       <c r="C66" s="6" t="s">
         <v>271</v>
       </c>
@@ -8141,13 +8194,13 @@
       <c r="H66" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I66" s="71"/>
+      <c r="I66" s="74"/>
     </row>
     <row r="67" spans="1:9" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" s="75"/>
+      <c r="B67" s="78"/>
       <c r="C67" s="6" t="s">
         <v>274</v>
       </c>
@@ -8166,13 +8219,13 @@
       <c r="H67" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I67" s="71"/>
+      <c r="I67" s="74"/>
     </row>
     <row r="68" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" s="75"/>
+      <c r="B68" s="78"/>
       <c r="C68" s="6" t="s">
         <v>277</v>
       </c>
@@ -8191,13 +8244,13 @@
       <c r="H68" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I68" s="71"/>
+      <c r="I68" s="74"/>
     </row>
     <row r="69" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69" s="75"/>
+      <c r="B69" s="78"/>
       <c r="C69" s="6" t="s">
         <v>280</v>
       </c>
@@ -8216,13 +8269,13 @@
       <c r="H69" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I69" s="71"/>
+      <c r="I69" s="74"/>
     </row>
     <row r="70" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
-      <c r="B70" s="75"/>
+      <c r="B70" s="78"/>
       <c r="C70" s="6" t="s">
         <v>283</v>
       </c>
@@ -8241,13 +8294,13 @@
       <c r="H70" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I70" s="71"/>
+      <c r="I70" s="74"/>
     </row>
     <row r="71" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" s="74"/>
+      <c r="B71" s="77"/>
       <c r="C71" s="6" t="s">
         <v>285</v>
       </c>
@@ -8266,7 +8319,7 @@
       <c r="H71" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I71" s="72"/>
+      <c r="I71" s="75"/>
     </row>
     <row r="72" spans="1:9" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
@@ -8461,17 +8514,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="70" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="69"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="72"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -9322,17 +9375,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="70" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="69"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="72"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -9477,7 +9530,7 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="76" t="s">
         <v>398</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -9504,7 +9557,7 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="76"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="6" t="s">
         <v>402</v>
       </c>
@@ -9529,7 +9582,7 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="76"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="6" t="s">
         <v>405</v>
       </c>
@@ -9554,7 +9607,7 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="76"/>
+      <c r="B10" s="79"/>
       <c r="C10" s="6" t="s">
         <v>408</v>
       </c>
@@ -9579,7 +9632,7 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="76"/>
+      <c r="B11" s="79"/>
       <c r="C11" s="6" t="s">
         <v>411</v>
       </c>
@@ -9604,7 +9657,7 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="76"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="6" t="s">
         <v>414</v>
       </c>
@@ -9629,7 +9682,7 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="76"/>
+      <c r="B13" s="79"/>
       <c r="C13" s="6" t="s">
         <v>417</v>
       </c>
@@ -9654,7 +9707,7 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="77"/>
+      <c r="B14" s="80"/>
       <c r="C14" s="6" t="s">
         <v>420</v>
       </c>
@@ -9874,7 +9927,7 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="76" t="s">
         <v>448</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -9901,7 +9954,7 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="76"/>
+      <c r="B23" s="79"/>
       <c r="C23" s="38" t="s">
         <v>452</v>
       </c>
@@ -9928,7 +9981,7 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="76"/>
+      <c r="B24" s="79"/>
       <c r="C24" s="6" t="s">
         <v>455</v>
       </c>
@@ -9953,7 +10006,7 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="76"/>
+      <c r="B25" s="79"/>
       <c r="C25" s="6" t="s">
         <v>457</v>
       </c>
@@ -9978,7 +10031,7 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="76"/>
+      <c r="B26" s="79"/>
       <c r="C26" s="38" t="s">
         <v>459</v>
       </c>
@@ -10005,7 +10058,7 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="77"/>
+      <c r="B27" s="80"/>
       <c r="C27" s="6" t="s">
         <v>462</v>
       </c>
@@ -10084,7 +10137,7 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="73" t="s">
+      <c r="B30" s="76" t="s">
         <v>471</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -10111,7 +10164,7 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="76"/>
+      <c r="B31" s="79"/>
       <c r="C31" s="6" t="s">
         <v>475</v>
       </c>
@@ -10136,7 +10189,7 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="76"/>
+      <c r="B32" s="79"/>
       <c r="C32" s="6" t="s">
         <v>478</v>
       </c>
@@ -10161,7 +10214,7 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="77"/>
+      <c r="B33" s="80"/>
       <c r="C33" s="6" t="s">
         <v>481</v>
       </c>
@@ -10325,7 +10378,7 @@
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="73" t="s">
+      <c r="B39" s="76" t="s">
         <v>502</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -10352,7 +10405,7 @@
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="76"/>
+      <c r="B40" s="79"/>
       <c r="C40" s="6" t="s">
         <v>506</v>
       </c>
@@ -10377,7 +10430,7 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="77"/>
+      <c r="B41" s="80"/>
       <c r="C41" s="6" t="s">
         <v>509</v>
       </c>
@@ -10402,7 +10455,7 @@
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="73" t="s">
+      <c r="B42" s="76" t="s">
         <v>512</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -10427,7 +10480,7 @@
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" s="76"/>
+      <c r="B43" s="79"/>
       <c r="C43" s="6" t="s">
         <v>516</v>
       </c>
@@ -10450,7 +10503,7 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="77"/>
+      <c r="B44" s="80"/>
       <c r="C44" s="6" t="s">
         <v>519</v>
       </c>
@@ -10520,17 +10573,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="70" t="s">
         <v>522</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="69"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="72"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -10897,17 +10950,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="70" t="s">
         <v>550</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="69"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="72"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -11238,7 +11291,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="73" t="s">
         <v>601</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -11263,7 +11316,7 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="72"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="6" t="s">
         <v>605</v>
       </c>
@@ -11402,18 +11455,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="70" t="s">
         <v>616</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="69"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="72"/>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -11451,7 +11504,7 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="76" t="s">
         <v>618</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -11475,7 +11528,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="74"/>
+      <c r="B4" s="77"/>
       <c r="C4" s="8" t="s">
         <v>621</v>
       </c>
@@ -11497,7 +11550,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="76" t="s">
         <v>623</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -11521,7 +11574,7 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="74"/>
+      <c r="B6" s="77"/>
       <c r="C6" s="8" t="s">
         <v>626</v>
       </c>
@@ -11567,7 +11620,7 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="76" t="s">
         <v>631</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -11591,7 +11644,7 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="74"/>
+      <c r="B9" s="77"/>
       <c r="C9" s="8" t="s">
         <v>634</v>
       </c>
@@ -11639,7 +11692,7 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="76" t="s">
         <v>640</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -11665,7 +11718,7 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="74"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="8" t="s">
         <v>643</v>
       </c>
@@ -11711,7 +11764,7 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="76" t="s">
         <v>648</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -11735,7 +11788,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="74"/>
+      <c r="B15" s="77"/>
       <c r="C15" s="8" t="s">
         <v>651</v>
       </c>
@@ -11755,7 +11808,7 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="76" t="s">
         <v>653</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -11779,7 +11832,7 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="75"/>
+      <c r="B17" s="78"/>
       <c r="C17" s="8" t="s">
         <v>656</v>
       </c>
@@ -11803,7 +11856,7 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="74"/>
+      <c r="B18" s="77"/>
       <c r="C18" s="8" t="s">
         <v>658</v>
       </c>
@@ -11847,7 +11900,7 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="76" t="s">
         <v>663</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -11869,7 +11922,7 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="74"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="8" t="s">
         <v>666</v>
       </c>
@@ -11913,7 +11966,7 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="76" t="s">
         <v>671</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -11937,7 +11990,7 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="74"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="8" t="s">
         <v>674</v>
       </c>
@@ -11983,7 +12036,7 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="73" t="s">
+      <c r="B26" s="76" t="s">
         <v>679</v>
       </c>
       <c r="C26" s="8" t="s">
@@ -12007,7 +12060,7 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="75"/>
+      <c r="B27" s="78"/>
       <c r="C27" s="8" t="s">
         <v>682</v>
       </c>
@@ -12031,7 +12084,7 @@
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="74"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="8" t="s">
         <v>684</v>
       </c>
@@ -12051,7 +12104,7 @@
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="76" t="s">
         <v>686</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -12075,7 +12128,7 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="74"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="8" t="s">
         <v>689</v>
       </c>
@@ -12121,7 +12174,7 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="73" t="s">
+      <c r="B32" s="76" t="s">
         <v>694</v>
       </c>
       <c r="C32" s="8" t="s">
@@ -12145,7 +12198,7 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="74"/>
+      <c r="B33" s="77"/>
       <c r="C33" s="8" t="s">
         <v>697</v>
       </c>
@@ -12167,7 +12220,7 @@
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="73" t="s">
+      <c r="B34" s="76" t="s">
         <v>699</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -12191,7 +12244,7 @@
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" s="74"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="8" t="s">
         <v>702</v>
       </c>
@@ -12259,7 +12312,7 @@
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" s="73" t="s">
+      <c r="B38" s="76" t="s">
         <v>710</v>
       </c>
       <c r="C38" s="8" t="s">
@@ -12283,7 +12336,7 @@
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="74"/>
+      <c r="B39" s="77"/>
       <c r="C39" s="8" t="s">
         <v>713</v>
       </c>
@@ -12305,7 +12358,7 @@
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="73" t="s">
+      <c r="B40" s="76" t="s">
         <v>715</v>
       </c>
       <c r="C40" s="8" t="s">
@@ -12329,7 +12382,7 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="74"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="8" t="s">
         <v>718</v>
       </c>
@@ -12375,7 +12428,7 @@
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" s="73" t="s">
+      <c r="B43" s="76" t="s">
         <v>723</v>
       </c>
       <c r="C43" s="8" t="s">
@@ -12399,7 +12452,7 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="74"/>
+      <c r="B44" s="77"/>
       <c r="C44" s="8" t="s">
         <v>726</v>
       </c>
@@ -12421,7 +12474,7 @@
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" s="73" t="s">
+      <c r="B45" s="76" t="s">
         <v>728</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -12445,7 +12498,7 @@
       <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="B46" s="74"/>
+      <c r="B46" s="77"/>
       <c r="C46" s="8" t="s">
         <v>731</v>
       </c>
@@ -12469,7 +12522,7 @@
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" s="73" t="s">
+      <c r="B47" s="76" t="s">
         <v>733</v>
       </c>
       <c r="C47" s="8" t="s">
@@ -12493,7 +12546,7 @@
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="74"/>
+      <c r="B48" s="77"/>
       <c r="C48" s="8" t="s">
         <v>736</v>
       </c>
@@ -12513,7 +12566,7 @@
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" s="73" t="s">
+      <c r="B49" s="76" t="s">
         <v>738</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -12537,7 +12590,7 @@
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="74"/>
+      <c r="B50" s="77"/>
       <c r="C50" s="8" t="s">
         <v>741</v>
       </c>
@@ -12561,7 +12614,7 @@
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" s="73" t="s">
+      <c r="B51" s="76" t="s">
         <v>743</v>
       </c>
       <c r="C51" s="8" t="s">
@@ -12583,7 +12636,7 @@
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" s="74"/>
+      <c r="B52" s="77"/>
       <c r="C52" s="8" t="s">
         <v>746</v>
       </c>
@@ -12627,7 +12680,7 @@
       <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54" s="73" t="s">
+      <c r="B54" s="76" t="s">
         <v>751</v>
       </c>
       <c r="C54" s="8" t="s">
@@ -12651,7 +12704,7 @@
       <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55" s="75"/>
+      <c r="B55" s="78"/>
       <c r="C55" s="8" t="s">
         <v>754</v>
       </c>
@@ -12675,7 +12728,7 @@
       <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56" s="74"/>
+      <c r="B56" s="77"/>
       <c r="C56" s="8" t="s">
         <v>756</v>
       </c>
@@ -12695,7 +12748,7 @@
       <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57" s="73" t="s">
+      <c r="B57" s="76" t="s">
         <v>758</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -12719,7 +12772,7 @@
       <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58" s="74"/>
+      <c r="B58" s="77"/>
       <c r="C58" s="8" t="s">
         <v>761</v>
       </c>
@@ -12791,7 +12844,7 @@
       <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61" s="73" t="s">
+      <c r="B61" s="76" t="s">
         <v>769</v>
       </c>
       <c r="C61" s="8" t="s">
@@ -12815,7 +12868,7 @@
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" s="74"/>
+      <c r="B62" s="77"/>
       <c r="C62" s="8" t="s">
         <v>772</v>
       </c>
@@ -12839,7 +12892,7 @@
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" s="73" t="s">
+      <c r="B63" s="76" t="s">
         <v>774</v>
       </c>
       <c r="C63" s="8" t="s">
@@ -12863,7 +12916,7 @@
       <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" s="74"/>
+      <c r="B64" s="77"/>
       <c r="C64" s="8" t="s">
         <v>777</v>
       </c>
@@ -12889,7 +12942,7 @@
       <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" s="73" t="s">
+      <c r="B65" s="76" t="s">
         <v>780</v>
       </c>
       <c r="C65" s="8" t="s">
@@ -12913,7 +12966,7 @@
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" s="75"/>
+      <c r="B66" s="78"/>
       <c r="C66" s="8" t="s">
         <v>783</v>
       </c>
@@ -12935,7 +12988,7 @@
       <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" s="75"/>
+      <c r="B67" s="78"/>
       <c r="C67" s="8" t="s">
         <v>785</v>
       </c>
@@ -12957,7 +13010,7 @@
       <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" s="75"/>
+      <c r="B68" s="78"/>
       <c r="C68" s="8" t="s">
         <v>787</v>
       </c>
@@ -12979,7 +13032,7 @@
       <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69" s="74"/>
+      <c r="B69" s="77"/>
       <c r="C69" s="8" t="s">
         <v>789</v>
       </c>
@@ -13025,7 +13078,7 @@
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" s="73" t="s">
+      <c r="B71" s="76" t="s">
         <v>794</v>
       </c>
       <c r="C71" s="8" t="s">
@@ -13049,7 +13102,7 @@
       <c r="A72" s="1">
         <v>70</v>
       </c>
-      <c r="B72" s="74"/>
+      <c r="B72" s="77"/>
       <c r="C72" s="8" t="s">
         <v>797</v>
       </c>
@@ -13093,7 +13146,7 @@
       <c r="A74" s="1">
         <v>72</v>
       </c>
-      <c r="B74" s="73" t="s">
+      <c r="B74" s="76" t="s">
         <v>802</v>
       </c>
       <c r="C74" s="8" t="s">
@@ -13117,7 +13170,7 @@
       <c r="A75" s="1">
         <v>73</v>
       </c>
-      <c r="B75" s="74"/>
+      <c r="B75" s="77"/>
       <c r="C75" s="8" t="s">
         <v>805</v>
       </c>
@@ -13187,7 +13240,7 @@
       <c r="A78" s="1">
         <v>76</v>
       </c>
-      <c r="B78" s="73" t="s">
+      <c r="B78" s="76" t="s">
         <v>813</v>
       </c>
       <c r="C78" s="8" t="s">
@@ -13211,7 +13264,7 @@
       <c r="A79" s="1">
         <v>77</v>
       </c>
-      <c r="B79" s="74"/>
+      <c r="B79" s="77"/>
       <c r="C79" s="8" t="s">
         <v>816</v>
       </c>
@@ -13235,7 +13288,7 @@
       <c r="A80" s="1">
         <v>78</v>
       </c>
-      <c r="B80" s="73" t="s">
+      <c r="B80" s="76" t="s">
         <v>818</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -13259,7 +13312,7 @@
       <c r="A81" s="1">
         <v>79</v>
       </c>
-      <c r="B81" s="74"/>
+      <c r="B81" s="77"/>
       <c r="C81" s="8" t="s">
         <v>821</v>
       </c>
@@ -13283,7 +13336,7 @@
       <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B82" s="73" t="s">
+      <c r="B82" s="76" t="s">
         <v>823</v>
       </c>
       <c r="C82" s="8" t="s">
@@ -13307,7 +13360,7 @@
       <c r="A83" s="1">
         <v>81</v>
       </c>
-      <c r="B83" s="75"/>
+      <c r="B83" s="78"/>
       <c r="C83" s="8" t="s">
         <v>826</v>
       </c>
@@ -13329,7 +13382,7 @@
       <c r="A84" s="1">
         <v>82</v>
       </c>
-      <c r="B84" s="75"/>
+      <c r="B84" s="78"/>
       <c r="C84" s="8" t="s">
         <v>828</v>
       </c>
@@ -13351,7 +13404,7 @@
       <c r="A85" s="1">
         <v>83</v>
       </c>
-      <c r="B85" s="74"/>
+      <c r="B85" s="77"/>
       <c r="C85" s="8" t="s">
         <v>830</v>
       </c>
@@ -13395,7 +13448,7 @@
       <c r="A87" s="1">
         <v>85</v>
       </c>
-      <c r="B87" s="73" t="s">
+      <c r="B87" s="76" t="s">
         <v>834</v>
       </c>
       <c r="C87" s="8" t="s">
@@ -13419,7 +13472,7 @@
       <c r="A88" s="1">
         <v>86</v>
       </c>
-      <c r="B88" s="75"/>
+      <c r="B88" s="78"/>
       <c r="C88" s="8" t="s">
         <v>837</v>
       </c>
@@ -13441,7 +13494,7 @@
       <c r="A89" s="1">
         <v>87</v>
       </c>
-      <c r="B89" s="74"/>
+      <c r="B89" s="77"/>
       <c r="C89" s="8" t="s">
         <v>839</v>
       </c>
@@ -13463,7 +13516,7 @@
       <c r="A90" s="1">
         <v>88</v>
       </c>
-      <c r="B90" s="73" t="s">
+      <c r="B90" s="76" t="s">
         <v>841</v>
       </c>
       <c r="C90" s="8" t="s">
@@ -13487,7 +13540,7 @@
       <c r="A91" s="1">
         <v>89</v>
       </c>
-      <c r="B91" s="75"/>
+      <c r="B91" s="78"/>
       <c r="C91" s="8" t="s">
         <v>844</v>
       </c>
@@ -13507,7 +13560,7 @@
       <c r="A92" s="1">
         <v>90</v>
       </c>
-      <c r="B92" s="74"/>
+      <c r="B92" s="77"/>
       <c r="C92" s="8" t="s">
         <v>846</v>
       </c>
@@ -13527,7 +13580,7 @@
       <c r="A93" s="1">
         <v>91</v>
       </c>
-      <c r="B93" s="73" t="s">
+      <c r="B93" s="76" t="s">
         <v>848</v>
       </c>
       <c r="C93" s="8" t="s">
@@ -13551,7 +13604,7 @@
       <c r="A94" s="1">
         <v>92</v>
       </c>
-      <c r="B94" s="74"/>
+      <c r="B94" s="77"/>
       <c r="C94" s="8" t="s">
         <v>851</v>
       </c>
@@ -13575,7 +13628,7 @@
       <c r="A95" s="1">
         <v>93</v>
       </c>
-      <c r="B95" s="73" t="s">
+      <c r="B95" s="76" t="s">
         <v>853</v>
       </c>
       <c r="C95" s="8" t="s">
@@ -13597,7 +13650,7 @@
       <c r="A96" s="1">
         <v>94</v>
       </c>
-      <c r="B96" s="74"/>
+      <c r="B96" s="77"/>
       <c r="C96" s="8" t="s">
         <v>856</v>
       </c>
@@ -13641,7 +13694,7 @@
       <c r="A98" s="1">
         <v>96</v>
       </c>
-      <c r="B98" s="73" t="s">
+      <c r="B98" s="76" t="s">
         <v>861</v>
       </c>
       <c r="C98" s="8" t="s">
@@ -13665,7 +13718,7 @@
       <c r="A99" s="1">
         <v>97</v>
       </c>
-      <c r="B99" s="75"/>
+      <c r="B99" s="78"/>
       <c r="C99" s="8" t="s">
         <v>864</v>
       </c>
@@ -13689,7 +13742,7 @@
       <c r="A100" s="1">
         <v>98</v>
       </c>
-      <c r="B100" s="74"/>
+      <c r="B100" s="77"/>
       <c r="C100" s="8" t="s">
         <v>866</v>
       </c>
@@ -13709,7 +13762,7 @@
       <c r="A101" s="1">
         <v>99</v>
       </c>
-      <c r="B101" s="73" t="s">
+      <c r="B101" s="76" t="s">
         <v>868</v>
       </c>
       <c r="C101" s="8" t="s">
@@ -13733,7 +13786,7 @@
       <c r="A102" s="1">
         <v>100</v>
       </c>
-      <c r="B102" s="74"/>
+      <c r="B102" s="77"/>
       <c r="C102" s="8" t="s">
         <v>871</v>
       </c>
@@ -13781,7 +13834,7 @@
       <c r="A104" s="1">
         <v>102</v>
       </c>
-      <c r="B104" s="73" t="s">
+      <c r="B104" s="76" t="s">
         <v>876</v>
       </c>
       <c r="C104" s="8" t="s">
@@ -13805,7 +13858,7 @@
       <c r="A105" s="1">
         <v>103</v>
       </c>
-      <c r="B105" s="75"/>
+      <c r="B105" s="78"/>
       <c r="C105" s="8" t="s">
         <v>879</v>
       </c>
@@ -13827,7 +13880,7 @@
       <c r="A106" s="1">
         <v>104</v>
       </c>
-      <c r="B106" s="75"/>
+      <c r="B106" s="78"/>
       <c r="C106" s="8" t="s">
         <v>881</v>
       </c>
@@ -13849,7 +13902,7 @@
       <c r="A107" s="1">
         <v>105</v>
       </c>
-      <c r="B107" s="74"/>
+      <c r="B107" s="77"/>
       <c r="C107" s="8" t="s">
         <v>883</v>
       </c>
@@ -13899,7 +13952,7 @@
       <c r="A109" s="1">
         <v>107</v>
       </c>
-      <c r="B109" s="73" t="s">
+      <c r="B109" s="76" t="s">
         <v>888</v>
       </c>
       <c r="C109" s="8" t="s">
@@ -13921,7 +13974,7 @@
       <c r="A110" s="1">
         <v>108</v>
       </c>
-      <c r="B110" s="74"/>
+      <c r="B110" s="77"/>
       <c r="C110" s="8" t="s">
         <v>891</v>
       </c>
@@ -13941,7 +13994,7 @@
       <c r="A111" s="1">
         <v>109</v>
       </c>
-      <c r="B111" s="73" t="s">
+      <c r="B111" s="76" t="s">
         <v>893</v>
       </c>
       <c r="C111" s="8" t="s">
@@ -13965,7 +14018,7 @@
       <c r="A112" s="1">
         <v>110</v>
       </c>
-      <c r="B112" s="74"/>
+      <c r="B112" s="77"/>
       <c r="C112" s="8" t="s">
         <v>896</v>
       </c>
@@ -14011,7 +14064,7 @@
       <c r="A114" s="1">
         <v>112</v>
       </c>
-      <c r="B114" s="73" t="s">
+      <c r="B114" s="76" t="s">
         <v>901</v>
       </c>
       <c r="C114" s="8" t="s">
@@ -14035,7 +14088,7 @@
       <c r="A115" s="1">
         <v>113</v>
       </c>
-      <c r="B115" s="74"/>
+      <c r="B115" s="77"/>
       <c r="C115" s="8" t="s">
         <v>904</v>
       </c>
@@ -14079,7 +14132,7 @@
       <c r="A117" s="1">
         <v>115</v>
       </c>
-      <c r="B117" s="73" t="s">
+      <c r="B117" s="76" t="s">
         <v>909</v>
       </c>
       <c r="C117" s="8" t="s">
@@ -14101,7 +14154,7 @@
       <c r="A118" s="1">
         <v>116</v>
       </c>
-      <c r="B118" s="75"/>
+      <c r="B118" s="78"/>
       <c r="C118" s="8" t="s">
         <v>912</v>
       </c>
@@ -14121,7 +14174,7 @@
       <c r="A119" s="1">
         <v>117</v>
       </c>
-      <c r="B119" s="75"/>
+      <c r="B119" s="78"/>
       <c r="C119" s="8" t="s">
         <v>914</v>
       </c>
@@ -14141,7 +14194,7 @@
       <c r="A120" s="1">
         <v>118</v>
       </c>
-      <c r="B120" s="74"/>
+      <c r="B120" s="77"/>
       <c r="C120" s="8" t="s">
         <v>916</v>
       </c>
@@ -14161,7 +14214,7 @@
       <c r="A121" s="1">
         <v>119</v>
       </c>
-      <c r="B121" s="73" t="s">
+      <c r="B121" s="76" t="s">
         <v>918</v>
       </c>
       <c r="C121" s="8" t="s">
@@ -14185,7 +14238,7 @@
       <c r="A122" s="1">
         <v>120</v>
       </c>
-      <c r="B122" s="75"/>
+      <c r="B122" s="78"/>
       <c r="C122" s="8" t="s">
         <v>921</v>
       </c>
@@ -14207,7 +14260,7 @@
       <c r="A123" s="1">
         <v>121</v>
       </c>
-      <c r="B123" s="74"/>
+      <c r="B123" s="77"/>
       <c r="C123" s="8" t="s">
         <v>923</v>
       </c>
@@ -14253,7 +14306,7 @@
       <c r="A125" s="1">
         <v>123</v>
       </c>
-      <c r="B125" s="73" t="s">
+      <c r="B125" s="76" t="s">
         <v>928</v>
       </c>
       <c r="C125" s="8" t="s">
@@ -14277,7 +14330,7 @@
       <c r="A126" s="1">
         <v>124</v>
       </c>
-      <c r="B126" s="75"/>
+      <c r="B126" s="78"/>
       <c r="C126" s="8" t="s">
         <v>931</v>
       </c>
@@ -14299,7 +14352,7 @@
       <c r="A127" s="1">
         <v>125</v>
       </c>
-      <c r="B127" s="75"/>
+      <c r="B127" s="78"/>
       <c r="C127" s="8" t="s">
         <v>933</v>
       </c>
@@ -14323,7 +14376,7 @@
       <c r="A128" s="1">
         <v>126</v>
       </c>
-      <c r="B128" s="75"/>
+      <c r="B128" s="78"/>
       <c r="C128" s="8" t="s">
         <v>935</v>
       </c>
@@ -14345,7 +14398,7 @@
       <c r="A129" s="1">
         <v>127</v>
       </c>
-      <c r="B129" s="75"/>
+      <c r="B129" s="78"/>
       <c r="C129" s="8" t="s">
         <v>937</v>
       </c>
@@ -14367,7 +14420,7 @@
       <c r="A130" s="1">
         <v>128</v>
       </c>
-      <c r="B130" s="74"/>
+      <c r="B130" s="77"/>
       <c r="C130" s="8" t="s">
         <v>939</v>
       </c>
@@ -14413,7 +14466,7 @@
       <c r="A132" s="1">
         <v>130</v>
       </c>
-      <c r="B132" s="73" t="s">
+      <c r="B132" s="76" t="s">
         <v>944</v>
       </c>
       <c r="C132" s="8" t="s">
@@ -14437,7 +14490,7 @@
       <c r="A133" s="1">
         <v>131</v>
       </c>
-      <c r="B133" s="74"/>
+      <c r="B133" s="77"/>
       <c r="C133" s="8" t="s">
         <v>947</v>
       </c>
@@ -14583,7 +14636,7 @@
       <c r="A139" s="1">
         <v>137</v>
       </c>
-      <c r="B139" s="73" t="s">
+      <c r="B139" s="76" t="s">
         <v>964</v>
       </c>
       <c r="C139" s="8" t="s">
@@ -14607,7 +14660,7 @@
       <c r="A140" s="1">
         <v>138</v>
       </c>
-      <c r="B140" s="74"/>
+      <c r="B140" s="77"/>
       <c r="C140" s="8" t="s">
         <v>967</v>
       </c>
@@ -14632,41 +14685,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="45">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B65:B69"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B87:B89"/>
-    <mergeCell ref="B90:B92"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="B98:B100"/>
     <mergeCell ref="B101:B102"/>
     <mergeCell ref="B104:B107"/>
     <mergeCell ref="B109:B110"/>
@@ -14677,6 +14695,41 @@
     <mergeCell ref="B121:B123"/>
     <mergeCell ref="B125:B130"/>
     <mergeCell ref="B132:B133"/>
+    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="B90:B92"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -14688,10 +14741,10 @@
   <dimension ref="A1:K57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14711,19 +14764,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="81" t="s">
         <v>969</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="83"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
@@ -14736,7 +14789,7 @@
         <v>617</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>551</v>
@@ -14764,20 +14817,20 @@
       <c r="A3" s="52">
         <v>1</v>
       </c>
-      <c r="B3" s="81" t="s">
-        <v>1186</v>
+      <c r="B3" s="84" t="s">
+        <v>1184</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D3" s="48">
         <v>43657</v>
       </c>
-      <c r="E3" s="54" t="s">
-        <v>1217</v>
-      </c>
-      <c r="F3" s="52" t="s">
-        <v>1161</v>
+      <c r="E3" s="33" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F3" s="67" t="s">
+        <v>1159</v>
       </c>
       <c r="G3" s="54"/>
       <c r="H3" s="55"/>
@@ -14789,18 +14842,18 @@
       <c r="A4" s="52">
         <v>2</v>
       </c>
-      <c r="B4" s="83"/>
+      <c r="B4" s="86"/>
       <c r="C4" s="47" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D4" s="48">
         <v>43657</v>
       </c>
-      <c r="E4" s="54" t="s">
-        <v>1218</v>
-      </c>
-      <c r="F4" s="52" t="s">
-        <v>1182</v>
+      <c r="E4" s="33" t="s">
+        <v>1214</v>
+      </c>
+      <c r="F4" s="67" t="s">
+        <v>1180</v>
       </c>
       <c r="G4" s="54"/>
       <c r="H4" s="55"/>
@@ -14812,20 +14865,20 @@
       <c r="A5" s="52">
         <v>3</v>
       </c>
-      <c r="B5" s="81" t="s">
-        <v>1185</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>1202</v>
-      </c>
-      <c r="D5" s="48">
+      <c r="B5" s="84" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D5" s="57">
         <v>43664</v>
       </c>
-      <c r="E5" s="46" t="s">
-        <v>1214</v>
-      </c>
-      <c r="F5" s="52" t="s">
-        <v>1181</v>
+      <c r="E5" s="87" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F5" s="88" t="s">
+        <v>1179</v>
       </c>
       <c r="G5" s="52"/>
       <c r="H5" s="55"/>
@@ -14837,18 +14890,18 @@
       <c r="A6" s="52">
         <v>4</v>
       </c>
-      <c r="B6" s="82"/>
+      <c r="B6" s="85"/>
       <c r="C6" s="47" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="D6" s="48">
         <v>43664</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>1205</v>
-      </c>
-      <c r="F6" s="52" t="s">
-        <v>1144</v>
+        <v>1203</v>
+      </c>
+      <c r="F6" s="67" t="s">
+        <v>1142</v>
       </c>
       <c r="G6" s="52"/>
       <c r="H6" s="55"/>
@@ -14860,18 +14913,18 @@
       <c r="A7" s="52">
         <v>5</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="47" t="s">
-        <v>1202</v>
-      </c>
-      <c r="D7" s="48">
+      <c r="B7" s="85"/>
+      <c r="C7" s="56" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D7" s="57">
         <v>43664</v>
       </c>
-      <c r="E7" s="46" t="s">
-        <v>1206</v>
-      </c>
-      <c r="F7" s="52" t="s">
-        <v>1145</v>
+      <c r="E7" s="87" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F7" s="88" t="s">
+        <v>1143</v>
       </c>
       <c r="G7" s="52"/>
       <c r="H7" s="55"/>
@@ -14883,18 +14936,18 @@
       <c r="A8" s="52">
         <v>6</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="47" t="s">
-        <v>1202</v>
-      </c>
-      <c r="D8" s="48">
+      <c r="B8" s="85"/>
+      <c r="C8" s="56" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D8" s="57">
         <v>43664</v>
       </c>
-      <c r="E8" s="46" t="s">
-        <v>1207</v>
-      </c>
-      <c r="F8" s="52" t="s">
-        <v>1146</v>
+      <c r="E8" s="87" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F8" s="88" t="s">
+        <v>1144</v>
       </c>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
@@ -14906,18 +14959,18 @@
       <c r="A9" s="52">
         <v>7</v>
       </c>
-      <c r="B9" s="82"/>
-      <c r="C9" s="47" t="s">
-        <v>1202</v>
-      </c>
-      <c r="D9" s="48">
+      <c r="B9" s="85"/>
+      <c r="C9" s="56" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D9" s="57">
         <v>43664</v>
       </c>
-      <c r="E9" s="46" t="s">
-        <v>1208</v>
-      </c>
-      <c r="F9" s="52" t="s">
-        <v>1147</v>
+      <c r="E9" s="87" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F9" s="88" t="s">
+        <v>1145</v>
       </c>
       <c r="G9" s="52"/>
       <c r="H9" s="55"/>
@@ -14929,18 +14982,18 @@
       <c r="A10" s="52">
         <v>8</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="47" t="s">
-        <v>1202</v>
-      </c>
-      <c r="D10" s="48">
+      <c r="B10" s="85"/>
+      <c r="C10" s="56" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D10" s="57">
         <v>43664</v>
       </c>
-      <c r="E10" s="46" t="s">
-        <v>1209</v>
-      </c>
-      <c r="F10" s="52" t="s">
-        <v>1148</v>
+      <c r="E10" s="87" t="s">
+        <v>1205</v>
+      </c>
+      <c r="F10" s="88" t="s">
+        <v>1146</v>
       </c>
       <c r="G10" s="52"/>
       <c r="H10" s="55"/>
@@ -14952,18 +15005,18 @@
       <c r="A11" s="52">
         <v>10</v>
       </c>
-      <c r="B11" s="82"/>
+      <c r="B11" s="85"/>
       <c r="C11" s="47" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="D11" s="48">
         <v>43664</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>1210</v>
-      </c>
-      <c r="F11" s="52" t="s">
-        <v>1179</v>
+        <v>1206</v>
+      </c>
+      <c r="F11" s="67" t="s">
+        <v>1177</v>
       </c>
       <c r="G11" s="52"/>
       <c r="H11" s="55"/>
@@ -14975,18 +15028,18 @@
       <c r="A12" s="52">
         <v>11</v>
       </c>
-      <c r="B12" s="82"/>
+      <c r="B12" s="85"/>
       <c r="C12" s="47" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="D12" s="48">
         <v>43664</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>1211</v>
-      </c>
-      <c r="F12" s="52" t="s">
-        <v>1180</v>
+        <v>1207</v>
+      </c>
+      <c r="F12" s="67" t="s">
+        <v>1178</v>
       </c>
       <c r="G12" s="52"/>
       <c r="H12" s="55"/>
@@ -14998,18 +15051,18 @@
       <c r="A13" s="52">
         <v>13</v>
       </c>
-      <c r="B13" s="82"/>
+      <c r="B13" s="85"/>
       <c r="C13" s="47" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="D13" s="48">
         <v>43664</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>1212</v>
-      </c>
-      <c r="F13" s="52" t="s">
-        <v>1183</v>
+        <v>1208</v>
+      </c>
+      <c r="F13" s="67" t="s">
+        <v>1181</v>
       </c>
       <c r="G13" s="52"/>
       <c r="H13" s="55"/>
@@ -15021,18 +15074,18 @@
       <c r="A14" s="52">
         <v>14</v>
       </c>
-      <c r="B14" s="83"/>
-      <c r="C14" s="47" t="s">
-        <v>1202</v>
-      </c>
-      <c r="D14" s="48">
+      <c r="B14" s="86"/>
+      <c r="C14" s="56" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D14" s="57">
         <v>43664</v>
       </c>
-      <c r="E14" s="46" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F14" s="52" t="s">
-        <v>1184</v>
+      <c r="E14" s="87" t="s">
+        <v>1209</v>
+      </c>
+      <c r="F14" s="88" t="s">
+        <v>1182</v>
       </c>
       <c r="G14" s="52"/>
       <c r="H14" s="55"/>
@@ -15045,10 +15098,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="54" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="D15" s="48">
         <v>43670</v>
@@ -15056,8 +15109,8 @@
       <c r="E15" s="54" t="s">
         <v>1126</v>
       </c>
-      <c r="F15" s="52" t="s">
-        <v>1158</v>
+      <c r="F15" s="67" t="s">
+        <v>1156</v>
       </c>
       <c r="G15" s="52"/>
       <c r="H15" s="55"/>
@@ -15070,19 +15123,19 @@
         <v>16</v>
       </c>
       <c r="B16" s="54" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="C16" s="59" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D16" s="57">
         <v>43654</v>
       </c>
       <c r="E16" s="58" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="F16" s="59" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="G16" s="52"/>
       <c r="H16" s="55"/>
@@ -15095,19 +15148,19 @@
         <v>17</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="D17" s="48">
         <v>43670</v>
       </c>
       <c r="E17" s="54" t="s">
-        <v>1136</v>
-      </c>
-      <c r="F17" s="52" t="s">
-        <v>1172</v>
+        <v>1134</v>
+      </c>
+      <c r="F17" s="67" t="s">
+        <v>1170</v>
       </c>
       <c r="G17" s="52"/>
       <c r="H17" s="55"/>
@@ -15123,7 +15176,7 @@
         <v>448</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="D18" s="48">
         <v>43664</v>
@@ -15131,8 +15184,8 @@
       <c r="E18" s="54" t="s">
         <v>1125</v>
       </c>
-      <c r="F18" s="52" t="s">
-        <v>1157</v>
+      <c r="F18" s="67" t="s">
+        <v>1155</v>
       </c>
       <c r="G18" s="52"/>
       <c r="H18" s="55"/>
@@ -15144,11 +15197,11 @@
       <c r="A19" s="52">
         <v>19</v>
       </c>
-      <c r="B19" s="81" t="s">
-        <v>1188</v>
+      <c r="B19" s="84" t="s">
+        <v>1186</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D19" s="57">
         <v>43664</v>
@@ -15156,8 +15209,8 @@
       <c r="E19" s="58" t="s">
         <v>1116</v>
       </c>
-      <c r="F19" s="85" t="s">
-        <v>1143</v>
+      <c r="F19" s="68" t="s">
+        <v>1141</v>
       </c>
       <c r="G19" s="52"/>
       <c r="H19" s="55"/>
@@ -15169,9 +15222,9 @@
       <c r="A20" s="52">
         <v>20</v>
       </c>
-      <c r="B20" s="82"/>
+      <c r="B20" s="85"/>
       <c r="C20" s="60" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D20" s="57">
         <v>43664</v>
@@ -15179,8 +15232,8 @@
       <c r="E20" s="58" t="s">
         <v>1117</v>
       </c>
-      <c r="F20" s="85" t="s">
-        <v>1149</v>
+      <c r="F20" s="68" t="s">
+        <v>1147</v>
       </c>
       <c r="G20" s="52"/>
       <c r="H20" s="55"/>
@@ -15192,9 +15245,9 @@
       <c r="A21" s="52">
         <v>21</v>
       </c>
-      <c r="B21" s="82"/>
+      <c r="B21" s="85"/>
       <c r="C21" s="60" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D21" s="57">
         <v>43657</v>
@@ -15202,8 +15255,8 @@
       <c r="E21" s="58" t="s">
         <v>1118</v>
       </c>
-      <c r="F21" s="85" t="s">
-        <v>1150</v>
+      <c r="F21" s="68" t="s">
+        <v>1148</v>
       </c>
       <c r="G21" s="52"/>
       <c r="H21" s="55"/>
@@ -15215,9 +15268,9 @@
       <c r="A22" s="52">
         <v>22</v>
       </c>
-      <c r="B22" s="82"/>
+      <c r="B22" s="85"/>
       <c r="C22" s="60" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D22" s="57">
         <v>43657</v>
@@ -15225,8 +15278,8 @@
       <c r="E22" s="58" t="s">
         <v>1119</v>
       </c>
-      <c r="F22" s="85" t="s">
-        <v>1151</v>
+      <c r="F22" s="68" t="s">
+        <v>1149</v>
       </c>
       <c r="G22" s="52"/>
       <c r="H22" s="55"/>
@@ -15238,18 +15291,18 @@
       <c r="A23" s="52">
         <v>23</v>
       </c>
-      <c r="B23" s="82"/>
+      <c r="B23" s="85"/>
       <c r="C23" s="60" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D23" s="57">
         <v>43657</v>
       </c>
       <c r="E23" s="58" t="s">
-        <v>1194</v>
-      </c>
-      <c r="F23" s="85" t="s">
-        <v>1162</v>
+        <v>1192</v>
+      </c>
+      <c r="F23" s="68" t="s">
+        <v>1160</v>
       </c>
       <c r="G23" s="52"/>
       <c r="H23" s="55"/>
@@ -15259,18 +15312,18 @@
     </row>
     <row r="24" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="52"/>
-      <c r="B24" s="82"/>
+      <c r="B24" s="85"/>
       <c r="C24" s="60" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D24" s="57">
         <v>43657</v>
       </c>
-      <c r="E24" s="86" t="s">
-        <v>1220</v>
-      </c>
-      <c r="F24" s="85" t="s">
-        <v>1219</v>
+      <c r="E24" s="69" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F24" s="68" t="s">
+        <v>1215</v>
       </c>
       <c r="G24" s="52"/>
       <c r="H24" s="55"/>
@@ -15282,18 +15335,18 @@
       <c r="A25" s="52">
         <v>24</v>
       </c>
-      <c r="B25" s="83"/>
+      <c r="B25" s="86"/>
       <c r="C25" s="59" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D25" s="57">
         <v>43657</v>
       </c>
       <c r="E25" s="58" t="s">
-        <v>1195</v>
-      </c>
-      <c r="F25" s="85" t="s">
-        <v>1163</v>
+        <v>1193</v>
+      </c>
+      <c r="F25" s="68" t="s">
+        <v>1161</v>
       </c>
       <c r="G25" s="52"/>
       <c r="H25" s="55"/>
@@ -15305,20 +15358,20 @@
       <c r="A26" s="52">
         <v>25</v>
       </c>
-      <c r="B26" s="81" t="s">
-        <v>1196</v>
-      </c>
-      <c r="C26" s="53" t="s">
-        <v>1202</v>
-      </c>
-      <c r="D26" s="48">
+      <c r="B26" s="84" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D26" s="57">
         <v>43664</v>
       </c>
-      <c r="E26" s="33" t="s">
-        <v>1137</v>
-      </c>
-      <c r="F26" s="52" t="s">
-        <v>1164</v>
+      <c r="E26" s="89" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F26" s="88" t="s">
+        <v>1162</v>
       </c>
       <c r="G26" s="52"/>
       <c r="H26" s="55"/>
@@ -15330,18 +15383,18 @@
       <c r="A27" s="52">
         <v>26</v>
       </c>
-      <c r="B27" s="83"/>
-      <c r="C27" s="47" t="s">
-        <v>1202</v>
-      </c>
-      <c r="D27" s="48">
+      <c r="B27" s="86"/>
+      <c r="C27" s="56" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D27" s="57">
         <v>43664</v>
       </c>
-      <c r="E27" s="33" t="s">
-        <v>1221</v>
-      </c>
-      <c r="F27" s="84" t="s">
-        <v>1173</v>
+      <c r="E27" s="89" t="s">
+        <v>1217</v>
+      </c>
+      <c r="F27" s="88" t="s">
+        <v>1171</v>
       </c>
       <c r="G27" s="52"/>
       <c r="H27" s="55"/>
@@ -15353,11 +15406,11 @@
       <c r="A28" s="52">
         <v>27</v>
       </c>
-      <c r="B28" s="81" t="s">
-        <v>1189</v>
+      <c r="B28" s="84" t="s">
+        <v>1187</v>
       </c>
       <c r="C28" s="60" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D28" s="57">
         <v>43657</v>
@@ -15365,8 +15418,8 @@
       <c r="E28" s="58" t="s">
         <v>1120</v>
       </c>
-      <c r="F28" s="85" t="s">
-        <v>1152</v>
+      <c r="F28" s="68" t="s">
+        <v>1150</v>
       </c>
       <c r="G28" s="52"/>
       <c r="H28" s="55"/>
@@ -15378,18 +15431,18 @@
       <c r="A29" s="52">
         <v>28</v>
       </c>
-      <c r="B29" s="83"/>
+      <c r="B29" s="86"/>
       <c r="C29" s="59" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D29" s="57">
         <v>43657</v>
       </c>
       <c r="E29" s="58" t="s">
-        <v>1129</v>
-      </c>
-      <c r="F29" s="85" t="s">
-        <v>1165</v>
+        <v>1127</v>
+      </c>
+      <c r="F29" s="68" t="s">
+        <v>1163</v>
       </c>
       <c r="G29" s="52"/>
       <c r="H29" s="55"/>
@@ -15401,11 +15454,11 @@
       <c r="A30" s="52">
         <v>29</v>
       </c>
-      <c r="B30" s="81" t="s">
-        <v>1190</v>
+      <c r="B30" s="84" t="s">
+        <v>1188</v>
       </c>
       <c r="C30" s="60" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D30" s="57">
         <v>43654</v>
@@ -15414,7 +15467,7 @@
         <v>1121</v>
       </c>
       <c r="F30" s="59" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="G30" s="52"/>
       <c r="H30" s="55"/>
@@ -15426,9 +15479,9 @@
       <c r="A31" s="52">
         <v>30</v>
       </c>
-      <c r="B31" s="82"/>
+      <c r="B31" s="85"/>
       <c r="C31" s="61" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D31" s="57">
         <v>43654</v>
@@ -15437,7 +15490,7 @@
         <v>1122</v>
       </c>
       <c r="F31" s="59" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="G31" s="52"/>
       <c r="H31" s="55"/>
@@ -15449,18 +15502,18 @@
       <c r="A32" s="52">
         <v>31</v>
       </c>
-      <c r="B32" s="82"/>
+      <c r="B32" s="85"/>
       <c r="C32" s="61" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D32" s="57">
         <v>43654</v>
       </c>
       <c r="E32" s="58" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="F32" s="59" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="G32" s="52"/>
       <c r="H32" s="55"/>
@@ -15472,18 +15525,18 @@
       <c r="A33" s="52">
         <v>32</v>
       </c>
-      <c r="B33" s="82"/>
+      <c r="B33" s="85"/>
       <c r="C33" s="61" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D33" s="57">
         <v>43654</v>
       </c>
       <c r="E33" s="58" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="F33" s="59" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="G33" s="52"/>
       <c r="H33" s="55"/>
@@ -15493,18 +15546,18 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="52"/>
-      <c r="B34" s="82"/>
+      <c r="B34" s="85"/>
       <c r="C34" s="62" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D34" s="63">
         <v>43654</v>
       </c>
       <c r="E34" s="64" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="F34" s="65" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="G34" s="52"/>
       <c r="H34" s="55"/>
@@ -15516,18 +15569,18 @@
       <c r="A35" s="52">
         <v>33</v>
       </c>
-      <c r="B35" s="83"/>
+      <c r="B35" s="86"/>
       <c r="C35" s="61" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D35" s="57">
         <v>43654</v>
       </c>
       <c r="E35" s="58" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="F35" s="59" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="G35" s="52"/>
       <c r="H35" s="55"/>
@@ -15539,11 +15592,11 @@
       <c r="A36" s="52">
         <v>34</v>
       </c>
-      <c r="B36" s="81" t="s">
-        <v>1191</v>
+      <c r="B36" s="84" t="s">
+        <v>1189</v>
       </c>
       <c r="C36" s="56" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="D36" s="57">
         <v>43647</v>
@@ -15552,7 +15605,7 @@
         <v>1123</v>
       </c>
       <c r="F36" s="59" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="G36" s="52"/>
       <c r="H36" s="55"/>
@@ -15564,9 +15617,9 @@
       <c r="A37" s="52">
         <v>35</v>
       </c>
-      <c r="B37" s="82"/>
+      <c r="B37" s="85"/>
       <c r="C37" s="56" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="D37" s="57">
         <v>43647</v>
@@ -15575,7 +15628,7 @@
         <v>1124</v>
       </c>
       <c r="F37" s="59" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="G37" s="52"/>
       <c r="H37" s="55"/>
@@ -15587,18 +15640,18 @@
       <c r="A38" s="52">
         <v>36</v>
       </c>
-      <c r="B38" s="82"/>
+      <c r="B38" s="85"/>
       <c r="C38" s="56" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="D38" s="57">
         <v>43647</v>
       </c>
       <c r="E38" s="58" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="F38" s="59" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="G38" s="52"/>
       <c r="H38" s="55"/>
@@ -15610,18 +15663,18 @@
       <c r="A39" s="52">
         <v>37</v>
       </c>
-      <c r="B39" s="83"/>
+      <c r="B39" s="86"/>
       <c r="C39" s="56" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="D39" s="57">
         <v>43647</v>
       </c>
       <c r="E39" s="58" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="F39" s="59" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="G39" s="52"/>
       <c r="H39" s="55"/>
@@ -15633,20 +15686,20 @@
       <c r="A40" s="52">
         <v>38</v>
       </c>
-      <c r="B40" s="81" t="s">
-        <v>1193</v>
+      <c r="B40" s="84" t="s">
+        <v>1191</v>
       </c>
       <c r="C40" s="53" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D40" s="48">
         <v>43657</v>
       </c>
       <c r="E40" s="54" t="s">
-        <v>1127</v>
+        <v>1220</v>
       </c>
       <c r="F40" s="52" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="G40" s="52"/>
       <c r="H40" s="55"/>
@@ -15658,18 +15711,18 @@
       <c r="A41" s="52">
         <v>39</v>
       </c>
-      <c r="B41" s="83"/>
+      <c r="B41" s="86"/>
       <c r="C41" s="47" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D41" s="48">
         <v>43657</v>
       </c>
       <c r="E41" s="54" t="s">
-        <v>1128</v>
+        <v>1221</v>
       </c>
       <c r="F41" s="52" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="G41" s="52"/>
       <c r="H41" s="55"/>
@@ -15682,19 +15735,19 @@
         <v>40</v>
       </c>
       <c r="B42" s="52" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="C42" s="61" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D42" s="57">
         <v>43654</v>
       </c>
       <c r="E42" s="58" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="F42" s="59" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="G42" s="52"/>
       <c r="H42" s="55"/>
@@ -15706,18 +15759,18 @@
       <c r="A43" s="52">
         <v>49</v>
       </c>
-      <c r="B43" s="82"/>
+      <c r="B43" s="85"/>
       <c r="C43" s="56" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="D43" s="57">
         <v>43647</v>
       </c>
       <c r="E43" s="58" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="F43" s="59" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="G43" s="52"/>
       <c r="H43" s="55"/>
@@ -15729,18 +15782,18 @@
       <c r="A44" s="52">
         <v>50</v>
       </c>
-      <c r="B44" s="82"/>
+      <c r="B44" s="85"/>
       <c r="C44" s="56" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="D44" s="57">
         <v>43647</v>
       </c>
       <c r="E44" s="58" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="F44" s="59" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="G44" s="52"/>
       <c r="H44" s="55"/>
@@ -15752,18 +15805,18 @@
       <c r="A45" s="52">
         <v>51</v>
       </c>
-      <c r="B45" s="82"/>
+      <c r="B45" s="85"/>
       <c r="C45" s="56" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="D45" s="57">
         <v>43647</v>
       </c>
       <c r="E45" s="58" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="F45" s="59" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="G45" s="52"/>
       <c r="H45" s="55"/>
@@ -15775,18 +15828,18 @@
       <c r="A46" s="52">
         <v>52</v>
       </c>
-      <c r="B46" s="83"/>
+      <c r="B46" s="86"/>
       <c r="C46" s="56" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="D46" s="57">
         <v>43647</v>
       </c>
       <c r="E46" s="58" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="F46" s="59" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="G46" s="52"/>
       <c r="H46" s="55"/>
@@ -15820,41 +15873,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16061,32 +16079,42 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7F7E23-FE37-4AB8-A4B3-5025B5D9E450}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16103,4 +16131,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating status for Partner Management
</commit_message>
<xml_diff>
--- a/_files/requirements/requirements_detailing_references/Partner Management/Pending_Backlog_Stories_Status Tracking.xlsx
+++ b/_files/requirements/requirements_detailing_references/Partner Management/Pending_Backlog_Stories_Status Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP wiki Open Source\Requirements\_files\requirements\requirements_detailing_references\Partner Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CA984C9F-169D-4C46-A306-4CBB4E669A3D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{93D8F3A2-19EB-487D-95FD-C6EA67FDBE93}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4840,6 +4840,15 @@
     <xf numFmtId="0" fontId="5" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4890,15 +4899,6 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -5278,12 +5278,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="73" t="s">
         <v>984</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="72"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="75"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -5832,17 +5832,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="72"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="75"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -5877,7 +5877,7 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="76" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -5904,7 +5904,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="74"/>
+      <c r="B4" s="77"/>
       <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
@@ -5929,7 +5929,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="74"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
@@ -5954,7 +5954,7 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="74"/>
+      <c r="B6" s="77"/>
       <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
@@ -5979,7 +5979,7 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="74"/>
+      <c r="B7" s="77"/>
       <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
@@ -6006,7 +6006,7 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="75"/>
+      <c r="B8" s="78"/>
       <c r="C8" s="6" t="s">
         <v>30</v>
       </c>
@@ -6234,7 +6234,7 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="76" t="s">
         <v>67</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -6261,7 +6261,7 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="75"/>
+      <c r="B17" s="78"/>
       <c r="C17" s="6" t="s">
         <v>71</v>
       </c>
@@ -6286,7 +6286,7 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="76" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -6313,7 +6313,7 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="75"/>
+      <c r="B19" s="78"/>
       <c r="C19" s="6" t="s">
         <v>64</v>
       </c>
@@ -6435,17 +6435,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="72"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="75"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -6507,7 +6507,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="79" t="s">
         <v>1020</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -6534,7 +6534,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="77"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="6" t="s">
         <v>92</v>
       </c>
@@ -6783,7 +6783,7 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="76" t="s">
+      <c r="B14" s="79" t="s">
         <v>1055</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -6812,7 +6812,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="77"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="6" t="s">
         <v>121</v>
       </c>
@@ -7001,7 +7001,7 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="79" t="s">
         <v>1038</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -7028,7 +7028,7 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="78"/>
+      <c r="B23" s="81"/>
       <c r="C23" s="6" t="s">
         <v>185</v>
       </c>
@@ -7053,7 +7053,7 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="77"/>
+      <c r="B24" s="80"/>
       <c r="C24" s="6" t="s">
         <v>188</v>
       </c>
@@ -7217,7 +7217,7 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="76" t="s">
+      <c r="B30" s="79" t="s">
         <v>1057</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -7246,7 +7246,7 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="77"/>
+      <c r="B31" s="80"/>
       <c r="C31" s="6" t="s">
         <v>142</v>
       </c>
@@ -7273,7 +7273,7 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="76" t="s">
+      <c r="B32" s="79" t="s">
         <v>1058</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -7302,7 +7302,7 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="77"/>
+      <c r="B33" s="80"/>
       <c r="C33" s="6" t="s">
         <v>147</v>
       </c>
@@ -7526,7 +7526,7 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="76" t="s">
+      <c r="B41" s="79" t="s">
         <v>194</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -7555,7 +7555,7 @@
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="77"/>
+      <c r="B42" s="80"/>
       <c r="C42" s="6" t="s">
         <v>197</v>
       </c>
@@ -7609,7 +7609,7 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="76" t="s">
+      <c r="B44" s="79" t="s">
         <v>1034</v>
       </c>
       <c r="C44" s="6" t="s">
@@ -7638,7 +7638,7 @@
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" s="77"/>
+      <c r="B45" s="80"/>
       <c r="C45" s="6" t="s">
         <v>208</v>
       </c>
@@ -7721,7 +7721,7 @@
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="76" t="s">
+      <c r="B48" s="79" t="s">
         <v>222</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -7742,7 +7742,7 @@
       <c r="H48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I48" s="73" t="s">
+      <c r="I48" s="76" t="s">
         <v>1000</v>
       </c>
     </row>
@@ -7750,7 +7750,7 @@
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" s="78"/>
+      <c r="B49" s="81"/>
       <c r="C49" s="6" t="s">
         <v>226</v>
       </c>
@@ -7769,13 +7769,13 @@
       <c r="H49" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I49" s="74"/>
+      <c r="I49" s="77"/>
     </row>
     <row r="50" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="78"/>
+      <c r="B50" s="81"/>
       <c r="C50" s="6" t="s">
         <v>229</v>
       </c>
@@ -7794,13 +7794,13 @@
       <c r="H50" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I50" s="74"/>
+      <c r="I50" s="77"/>
     </row>
     <row r="51" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" s="78"/>
+      <c r="B51" s="81"/>
       <c r="C51" s="6" t="s">
         <v>232</v>
       </c>
@@ -7819,13 +7819,13 @@
       <c r="H51" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I51" s="74"/>
+      <c r="I51" s="77"/>
     </row>
     <row r="52" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" s="78"/>
+      <c r="B52" s="81"/>
       <c r="C52" s="6" t="s">
         <v>235</v>
       </c>
@@ -7844,13 +7844,13 @@
       <c r="H52" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I52" s="74"/>
+      <c r="I52" s="77"/>
     </row>
     <row r="53" spans="1:9" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="B53" s="78"/>
+      <c r="B53" s="81"/>
       <c r="C53" s="6" t="s">
         <v>238</v>
       </c>
@@ -7869,13 +7869,13 @@
       <c r="H53" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I53" s="74"/>
+      <c r="I53" s="77"/>
     </row>
     <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54" s="78"/>
+      <c r="B54" s="81"/>
       <c r="C54" s="6" t="s">
         <v>241</v>
       </c>
@@ -7894,13 +7894,13 @@
       <c r="H54" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I54" s="74"/>
+      <c r="I54" s="77"/>
     </row>
     <row r="55" spans="1:9" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55" s="78"/>
+      <c r="B55" s="81"/>
       <c r="C55" s="6" t="s">
         <v>244</v>
       </c>
@@ -7919,13 +7919,13 @@
       <c r="H55" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I55" s="74"/>
+      <c r="I55" s="77"/>
     </row>
     <row r="56" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56" s="78"/>
+      <c r="B56" s="81"/>
       <c r="C56" s="6" t="s">
         <v>1041</v>
       </c>
@@ -7940,13 +7940,13 @@
         <v>987</v>
       </c>
       <c r="H56" s="4"/>
-      <c r="I56" s="74"/>
+      <c r="I56" s="77"/>
     </row>
     <row r="57" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57" s="77"/>
+      <c r="B57" s="80"/>
       <c r="C57" s="6" t="s">
         <v>247</v>
       </c>
@@ -7965,13 +7965,13 @@
       <c r="H57" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I57" s="75"/>
+      <c r="I57" s="78"/>
     </row>
     <row r="58" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58" s="76" t="s">
+      <c r="B58" s="79" t="s">
         <v>222</v>
       </c>
       <c r="C58" s="6" t="s">
@@ -7992,7 +7992,7 @@
       <c r="H58" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I58" s="73" t="s">
+      <c r="I58" s="76" t="s">
         <v>1000</v>
       </c>
     </row>
@@ -8000,7 +8000,7 @@
       <c r="A59" s="1">
         <v>57</v>
       </c>
-      <c r="B59" s="78"/>
+      <c r="B59" s="81"/>
       <c r="C59" s="6" t="s">
         <v>253</v>
       </c>
@@ -8019,13 +8019,13 @@
       <c r="H59" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I59" s="74"/>
+      <c r="I59" s="77"/>
     </row>
     <row r="60" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
-      <c r="B60" s="78"/>
+      <c r="B60" s="81"/>
       <c r="C60" s="6" t="s">
         <v>256</v>
       </c>
@@ -8044,13 +8044,13 @@
       <c r="H60" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I60" s="74"/>
+      <c r="I60" s="77"/>
     </row>
     <row r="61" spans="1:9" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61" s="78"/>
+      <c r="B61" s="81"/>
       <c r="C61" s="6" t="s">
         <v>259</v>
       </c>
@@ -8069,13 +8069,13 @@
       <c r="H61" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I61" s="74"/>
+      <c r="I61" s="77"/>
     </row>
     <row r="62" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" s="78"/>
+      <c r="B62" s="81"/>
       <c r="C62" s="6" t="s">
         <v>262</v>
       </c>
@@ -8094,13 +8094,13 @@
       <c r="H62" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I62" s="74"/>
+      <c r="I62" s="77"/>
     </row>
     <row r="63" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" s="78"/>
+      <c r="B63" s="81"/>
       <c r="C63" s="6" t="s">
         <v>264</v>
       </c>
@@ -8119,13 +8119,13 @@
       <c r="H63" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I63" s="74"/>
+      <c r="I63" s="77"/>
     </row>
     <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" s="78"/>
+      <c r="B64" s="81"/>
       <c r="C64" s="6" t="s">
         <v>75</v>
       </c>
@@ -8144,13 +8144,13 @@
       <c r="H64" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I64" s="74"/>
+      <c r="I64" s="77"/>
     </row>
     <row r="65" spans="1:9" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" s="78"/>
+      <c r="B65" s="81"/>
       <c r="C65" s="6" t="s">
         <v>268</v>
       </c>
@@ -8169,13 +8169,13 @@
       <c r="H65" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I65" s="74"/>
+      <c r="I65" s="77"/>
     </row>
     <row r="66" spans="1:9" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" s="78"/>
+      <c r="B66" s="81"/>
       <c r="C66" s="6" t="s">
         <v>271</v>
       </c>
@@ -8194,13 +8194,13 @@
       <c r="H66" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I66" s="74"/>
+      <c r="I66" s="77"/>
     </row>
     <row r="67" spans="1:9" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" s="78"/>
+      <c r="B67" s="81"/>
       <c r="C67" s="6" t="s">
         <v>274</v>
       </c>
@@ -8219,13 +8219,13 @@
       <c r="H67" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I67" s="74"/>
+      <c r="I67" s="77"/>
     </row>
     <row r="68" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" s="78"/>
+      <c r="B68" s="81"/>
       <c r="C68" s="6" t="s">
         <v>277</v>
       </c>
@@ -8244,13 +8244,13 @@
       <c r="H68" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I68" s="74"/>
+      <c r="I68" s="77"/>
     </row>
     <row r="69" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69" s="78"/>
+      <c r="B69" s="81"/>
       <c r="C69" s="6" t="s">
         <v>280</v>
       </c>
@@ -8269,13 +8269,13 @@
       <c r="H69" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I69" s="74"/>
+      <c r="I69" s="77"/>
     </row>
     <row r="70" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
-      <c r="B70" s="78"/>
+      <c r="B70" s="81"/>
       <c r="C70" s="6" t="s">
         <v>283</v>
       </c>
@@ -8294,13 +8294,13 @@
       <c r="H70" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I70" s="74"/>
+      <c r="I70" s="77"/>
     </row>
     <row r="71" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" s="77"/>
+      <c r="B71" s="80"/>
       <c r="C71" s="6" t="s">
         <v>285</v>
       </c>
@@ -8319,7 +8319,7 @@
       <c r="H71" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I71" s="75"/>
+      <c r="I71" s="78"/>
     </row>
     <row r="72" spans="1:9" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
@@ -8514,17 +8514,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="73" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="72"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="75"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -9375,17 +9375,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="73" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="72"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="75"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -9530,7 +9530,7 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="79" t="s">
         <v>398</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -9557,7 +9557,7 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="79"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="6" t="s">
         <v>402</v>
       </c>
@@ -9582,7 +9582,7 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="79"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="6" t="s">
         <v>405</v>
       </c>
@@ -9607,7 +9607,7 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="79"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="6" t="s">
         <v>408</v>
       </c>
@@ -9632,7 +9632,7 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="79"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="6" t="s">
         <v>411</v>
       </c>
@@ -9657,7 +9657,7 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="79"/>
+      <c r="B12" s="82"/>
       <c r="C12" s="6" t="s">
         <v>414</v>
       </c>
@@ -9682,7 +9682,7 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="79"/>
+      <c r="B13" s="82"/>
       <c r="C13" s="6" t="s">
         <v>417</v>
       </c>
@@ -9707,7 +9707,7 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="80"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="6" t="s">
         <v>420</v>
       </c>
@@ -9927,7 +9927,7 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="79" t="s">
         <v>448</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -9954,7 +9954,7 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="79"/>
+      <c r="B23" s="82"/>
       <c r="C23" s="38" t="s">
         <v>452</v>
       </c>
@@ -9981,7 +9981,7 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="79"/>
+      <c r="B24" s="82"/>
       <c r="C24" s="6" t="s">
         <v>455</v>
       </c>
@@ -10006,7 +10006,7 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="79"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="6" t="s">
         <v>457</v>
       </c>
@@ -10031,7 +10031,7 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="79"/>
+      <c r="B26" s="82"/>
       <c r="C26" s="38" t="s">
         <v>459</v>
       </c>
@@ -10058,7 +10058,7 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="80"/>
+      <c r="B27" s="83"/>
       <c r="C27" s="6" t="s">
         <v>462</v>
       </c>
@@ -10137,7 +10137,7 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="76" t="s">
+      <c r="B30" s="79" t="s">
         <v>471</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -10164,7 +10164,7 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="79"/>
+      <c r="B31" s="82"/>
       <c r="C31" s="6" t="s">
         <v>475</v>
       </c>
@@ -10189,7 +10189,7 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="79"/>
+      <c r="B32" s="82"/>
       <c r="C32" s="6" t="s">
         <v>478</v>
       </c>
@@ -10214,7 +10214,7 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="80"/>
+      <c r="B33" s="83"/>
       <c r="C33" s="6" t="s">
         <v>481</v>
       </c>
@@ -10378,7 +10378,7 @@
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="76" t="s">
+      <c r="B39" s="79" t="s">
         <v>502</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -10405,7 +10405,7 @@
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="79"/>
+      <c r="B40" s="82"/>
       <c r="C40" s="6" t="s">
         <v>506</v>
       </c>
@@ -10430,7 +10430,7 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="80"/>
+      <c r="B41" s="83"/>
       <c r="C41" s="6" t="s">
         <v>509</v>
       </c>
@@ -10455,7 +10455,7 @@
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="76" t="s">
+      <c r="B42" s="79" t="s">
         <v>512</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -10480,7 +10480,7 @@
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" s="79"/>
+      <c r="B43" s="82"/>
       <c r="C43" s="6" t="s">
         <v>516</v>
       </c>
@@ -10503,7 +10503,7 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="80"/>
+      <c r="B44" s="83"/>
       <c r="C44" s="6" t="s">
         <v>519</v>
       </c>
@@ -10573,17 +10573,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="73" t="s">
         <v>522</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="72"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="75"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -10950,17 +10950,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="73" t="s">
         <v>550</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="72"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="75"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -11291,7 +11291,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="76" t="s">
         <v>601</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -11316,7 +11316,7 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="75"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="6" t="s">
         <v>605</v>
       </c>
@@ -11455,18 +11455,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="73" t="s">
         <v>616</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="72"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="75"/>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -11504,7 +11504,7 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="79" t="s">
         <v>618</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -11528,7 +11528,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="77"/>
+      <c r="B4" s="80"/>
       <c r="C4" s="8" t="s">
         <v>621</v>
       </c>
@@ -11550,7 +11550,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="79" t="s">
         <v>623</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -11574,7 +11574,7 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="77"/>
+      <c r="B6" s="80"/>
       <c r="C6" s="8" t="s">
         <v>626</v>
       </c>
@@ -11620,7 +11620,7 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="79" t="s">
         <v>631</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -11644,7 +11644,7 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="77"/>
+      <c r="B9" s="80"/>
       <c r="C9" s="8" t="s">
         <v>634</v>
       </c>
@@ -11692,7 +11692,7 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="79" t="s">
         <v>640</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -11718,7 +11718,7 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="77"/>
+      <c r="B12" s="80"/>
       <c r="C12" s="8" t="s">
         <v>643</v>
       </c>
@@ -11764,7 +11764,7 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="76" t="s">
+      <c r="B14" s="79" t="s">
         <v>648</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -11788,7 +11788,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="77"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="8" t="s">
         <v>651</v>
       </c>
@@ -11808,7 +11808,7 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="76" t="s">
+      <c r="B16" s="79" t="s">
         <v>653</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -11832,7 +11832,7 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="78"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="8" t="s">
         <v>656</v>
       </c>
@@ -11856,7 +11856,7 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="77"/>
+      <c r="B18" s="80"/>
       <c r="C18" s="8" t="s">
         <v>658</v>
       </c>
@@ -11900,7 +11900,7 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="76" t="s">
+      <c r="B20" s="79" t="s">
         <v>663</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -11922,7 +11922,7 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="77"/>
+      <c r="B21" s="80"/>
       <c r="C21" s="8" t="s">
         <v>666</v>
       </c>
@@ -11966,7 +11966,7 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="79" t="s">
         <v>671</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -11990,7 +11990,7 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="77"/>
+      <c r="B24" s="80"/>
       <c r="C24" s="8" t="s">
         <v>674</v>
       </c>
@@ -12036,7 +12036,7 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="79" t="s">
         <v>679</v>
       </c>
       <c r="C26" s="8" t="s">
@@ -12060,7 +12060,7 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="78"/>
+      <c r="B27" s="81"/>
       <c r="C27" s="8" t="s">
         <v>682</v>
       </c>
@@ -12084,7 +12084,7 @@
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="77"/>
+      <c r="B28" s="80"/>
       <c r="C28" s="8" t="s">
         <v>684</v>
       </c>
@@ -12104,7 +12104,7 @@
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="76" t="s">
+      <c r="B29" s="79" t="s">
         <v>686</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -12128,7 +12128,7 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="77"/>
+      <c r="B30" s="80"/>
       <c r="C30" s="8" t="s">
         <v>689</v>
       </c>
@@ -12174,7 +12174,7 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="76" t="s">
+      <c r="B32" s="79" t="s">
         <v>694</v>
       </c>
       <c r="C32" s="8" t="s">
@@ -12198,7 +12198,7 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="77"/>
+      <c r="B33" s="80"/>
       <c r="C33" s="8" t="s">
         <v>697</v>
       </c>
@@ -12220,7 +12220,7 @@
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="76" t="s">
+      <c r="B34" s="79" t="s">
         <v>699</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -12244,7 +12244,7 @@
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" s="77"/>
+      <c r="B35" s="80"/>
       <c r="C35" s="8" t="s">
         <v>702</v>
       </c>
@@ -12312,7 +12312,7 @@
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" s="76" t="s">
+      <c r="B38" s="79" t="s">
         <v>710</v>
       </c>
       <c r="C38" s="8" t="s">
@@ -12336,7 +12336,7 @@
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="77"/>
+      <c r="B39" s="80"/>
       <c r="C39" s="8" t="s">
         <v>713</v>
       </c>
@@ -12358,7 +12358,7 @@
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="76" t="s">
+      <c r="B40" s="79" t="s">
         <v>715</v>
       </c>
       <c r="C40" s="8" t="s">
@@ -12382,7 +12382,7 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="77"/>
+      <c r="B41" s="80"/>
       <c r="C41" s="8" t="s">
         <v>718</v>
       </c>
@@ -12428,7 +12428,7 @@
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" s="76" t="s">
+      <c r="B43" s="79" t="s">
         <v>723</v>
       </c>
       <c r="C43" s="8" t="s">
@@ -12452,7 +12452,7 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="77"/>
+      <c r="B44" s="80"/>
       <c r="C44" s="8" t="s">
         <v>726</v>
       </c>
@@ -12474,7 +12474,7 @@
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" s="76" t="s">
+      <c r="B45" s="79" t="s">
         <v>728</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -12498,7 +12498,7 @@
       <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="B46" s="77"/>
+      <c r="B46" s="80"/>
       <c r="C46" s="8" t="s">
         <v>731</v>
       </c>
@@ -12522,7 +12522,7 @@
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" s="76" t="s">
+      <c r="B47" s="79" t="s">
         <v>733</v>
       </c>
       <c r="C47" s="8" t="s">
@@ -12546,7 +12546,7 @@
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="77"/>
+      <c r="B48" s="80"/>
       <c r="C48" s="8" t="s">
         <v>736</v>
       </c>
@@ -12566,7 +12566,7 @@
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" s="76" t="s">
+      <c r="B49" s="79" t="s">
         <v>738</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -12590,7 +12590,7 @@
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="77"/>
+      <c r="B50" s="80"/>
       <c r="C50" s="8" t="s">
         <v>741</v>
       </c>
@@ -12614,7 +12614,7 @@
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" s="76" t="s">
+      <c r="B51" s="79" t="s">
         <v>743</v>
       </c>
       <c r="C51" s="8" t="s">
@@ -12636,7 +12636,7 @@
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" s="77"/>
+      <c r="B52" s="80"/>
       <c r="C52" s="8" t="s">
         <v>746</v>
       </c>
@@ -12680,7 +12680,7 @@
       <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54" s="76" t="s">
+      <c r="B54" s="79" t="s">
         <v>751</v>
       </c>
       <c r="C54" s="8" t="s">
@@ -12704,7 +12704,7 @@
       <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55" s="78"/>
+      <c r="B55" s="81"/>
       <c r="C55" s="8" t="s">
         <v>754</v>
       </c>
@@ -12728,7 +12728,7 @@
       <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56" s="77"/>
+      <c r="B56" s="80"/>
       <c r="C56" s="8" t="s">
         <v>756</v>
       </c>
@@ -12748,7 +12748,7 @@
       <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57" s="76" t="s">
+      <c r="B57" s="79" t="s">
         <v>758</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -12772,7 +12772,7 @@
       <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58" s="77"/>
+      <c r="B58" s="80"/>
       <c r="C58" s="8" t="s">
         <v>761</v>
       </c>
@@ -12844,7 +12844,7 @@
       <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61" s="76" t="s">
+      <c r="B61" s="79" t="s">
         <v>769</v>
       </c>
       <c r="C61" s="8" t="s">
@@ -12868,7 +12868,7 @@
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" s="77"/>
+      <c r="B62" s="80"/>
       <c r="C62" s="8" t="s">
         <v>772</v>
       </c>
@@ -12892,7 +12892,7 @@
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" s="76" t="s">
+      <c r="B63" s="79" t="s">
         <v>774</v>
       </c>
       <c r="C63" s="8" t="s">
@@ -12916,7 +12916,7 @@
       <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" s="77"/>
+      <c r="B64" s="80"/>
       <c r="C64" s="8" t="s">
         <v>777</v>
       </c>
@@ -12942,7 +12942,7 @@
       <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" s="76" t="s">
+      <c r="B65" s="79" t="s">
         <v>780</v>
       </c>
       <c r="C65" s="8" t="s">
@@ -12966,7 +12966,7 @@
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" s="78"/>
+      <c r="B66" s="81"/>
       <c r="C66" s="8" t="s">
         <v>783</v>
       </c>
@@ -12988,7 +12988,7 @@
       <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" s="78"/>
+      <c r="B67" s="81"/>
       <c r="C67" s="8" t="s">
         <v>785</v>
       </c>
@@ -13010,7 +13010,7 @@
       <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" s="78"/>
+      <c r="B68" s="81"/>
       <c r="C68" s="8" t="s">
         <v>787</v>
       </c>
@@ -13032,7 +13032,7 @@
       <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69" s="77"/>
+      <c r="B69" s="80"/>
       <c r="C69" s="8" t="s">
         <v>789</v>
       </c>
@@ -13078,7 +13078,7 @@
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" s="76" t="s">
+      <c r="B71" s="79" t="s">
         <v>794</v>
       </c>
       <c r="C71" s="8" t="s">
@@ -13102,7 +13102,7 @@
       <c r="A72" s="1">
         <v>70</v>
       </c>
-      <c r="B72" s="77"/>
+      <c r="B72" s="80"/>
       <c r="C72" s="8" t="s">
         <v>797</v>
       </c>
@@ -13146,7 +13146,7 @@
       <c r="A74" s="1">
         <v>72</v>
       </c>
-      <c r="B74" s="76" t="s">
+      <c r="B74" s="79" t="s">
         <v>802</v>
       </c>
       <c r="C74" s="8" t="s">
@@ -13170,7 +13170,7 @@
       <c r="A75" s="1">
         <v>73</v>
       </c>
-      <c r="B75" s="77"/>
+      <c r="B75" s="80"/>
       <c r="C75" s="8" t="s">
         <v>805</v>
       </c>
@@ -13240,7 +13240,7 @@
       <c r="A78" s="1">
         <v>76</v>
       </c>
-      <c r="B78" s="76" t="s">
+      <c r="B78" s="79" t="s">
         <v>813</v>
       </c>
       <c r="C78" s="8" t="s">
@@ -13264,7 +13264,7 @@
       <c r="A79" s="1">
         <v>77</v>
       </c>
-      <c r="B79" s="77"/>
+      <c r="B79" s="80"/>
       <c r="C79" s="8" t="s">
         <v>816</v>
       </c>
@@ -13288,7 +13288,7 @@
       <c r="A80" s="1">
         <v>78</v>
       </c>
-      <c r="B80" s="76" t="s">
+      <c r="B80" s="79" t="s">
         <v>818</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -13312,7 +13312,7 @@
       <c r="A81" s="1">
         <v>79</v>
       </c>
-      <c r="B81" s="77"/>
+      <c r="B81" s="80"/>
       <c r="C81" s="8" t="s">
         <v>821</v>
       </c>
@@ -13336,7 +13336,7 @@
       <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B82" s="76" t="s">
+      <c r="B82" s="79" t="s">
         <v>823</v>
       </c>
       <c r="C82" s="8" t="s">
@@ -13360,7 +13360,7 @@
       <c r="A83" s="1">
         <v>81</v>
       </c>
-      <c r="B83" s="78"/>
+      <c r="B83" s="81"/>
       <c r="C83" s="8" t="s">
         <v>826</v>
       </c>
@@ -13382,7 +13382,7 @@
       <c r="A84" s="1">
         <v>82</v>
       </c>
-      <c r="B84" s="78"/>
+      <c r="B84" s="81"/>
       <c r="C84" s="8" t="s">
         <v>828</v>
       </c>
@@ -13404,7 +13404,7 @@
       <c r="A85" s="1">
         <v>83</v>
       </c>
-      <c r="B85" s="77"/>
+      <c r="B85" s="80"/>
       <c r="C85" s="8" t="s">
         <v>830</v>
       </c>
@@ -13448,7 +13448,7 @@
       <c r="A87" s="1">
         <v>85</v>
       </c>
-      <c r="B87" s="76" t="s">
+      <c r="B87" s="79" t="s">
         <v>834</v>
       </c>
       <c r="C87" s="8" t="s">
@@ -13472,7 +13472,7 @@
       <c r="A88" s="1">
         <v>86</v>
       </c>
-      <c r="B88" s="78"/>
+      <c r="B88" s="81"/>
       <c r="C88" s="8" t="s">
         <v>837</v>
       </c>
@@ -13494,7 +13494,7 @@
       <c r="A89" s="1">
         <v>87</v>
       </c>
-      <c r="B89" s="77"/>
+      <c r="B89" s="80"/>
       <c r="C89" s="8" t="s">
         <v>839</v>
       </c>
@@ -13516,7 +13516,7 @@
       <c r="A90" s="1">
         <v>88</v>
       </c>
-      <c r="B90" s="76" t="s">
+      <c r="B90" s="79" t="s">
         <v>841</v>
       </c>
       <c r="C90" s="8" t="s">
@@ -13540,7 +13540,7 @@
       <c r="A91" s="1">
         <v>89</v>
       </c>
-      <c r="B91" s="78"/>
+      <c r="B91" s="81"/>
       <c r="C91" s="8" t="s">
         <v>844</v>
       </c>
@@ -13560,7 +13560,7 @@
       <c r="A92" s="1">
         <v>90</v>
       </c>
-      <c r="B92" s="77"/>
+      <c r="B92" s="80"/>
       <c r="C92" s="8" t="s">
         <v>846</v>
       </c>
@@ -13580,7 +13580,7 @@
       <c r="A93" s="1">
         <v>91</v>
       </c>
-      <c r="B93" s="76" t="s">
+      <c r="B93" s="79" t="s">
         <v>848</v>
       </c>
       <c r="C93" s="8" t="s">
@@ -13604,7 +13604,7 @@
       <c r="A94" s="1">
         <v>92</v>
       </c>
-      <c r="B94" s="77"/>
+      <c r="B94" s="80"/>
       <c r="C94" s="8" t="s">
         <v>851</v>
       </c>
@@ -13628,7 +13628,7 @@
       <c r="A95" s="1">
         <v>93</v>
       </c>
-      <c r="B95" s="76" t="s">
+      <c r="B95" s="79" t="s">
         <v>853</v>
       </c>
       <c r="C95" s="8" t="s">
@@ -13650,7 +13650,7 @@
       <c r="A96" s="1">
         <v>94</v>
       </c>
-      <c r="B96" s="77"/>
+      <c r="B96" s="80"/>
       <c r="C96" s="8" t="s">
         <v>856</v>
       </c>
@@ -13694,7 +13694,7 @@
       <c r="A98" s="1">
         <v>96</v>
       </c>
-      <c r="B98" s="76" t="s">
+      <c r="B98" s="79" t="s">
         <v>861</v>
       </c>
       <c r="C98" s="8" t="s">
@@ -13718,7 +13718,7 @@
       <c r="A99" s="1">
         <v>97</v>
       </c>
-      <c r="B99" s="78"/>
+      <c r="B99" s="81"/>
       <c r="C99" s="8" t="s">
         <v>864</v>
       </c>
@@ -13742,7 +13742,7 @@
       <c r="A100" s="1">
         <v>98</v>
       </c>
-      <c r="B100" s="77"/>
+      <c r="B100" s="80"/>
       <c r="C100" s="8" t="s">
         <v>866</v>
       </c>
@@ -13762,7 +13762,7 @@
       <c r="A101" s="1">
         <v>99</v>
       </c>
-      <c r="B101" s="76" t="s">
+      <c r="B101" s="79" t="s">
         <v>868</v>
       </c>
       <c r="C101" s="8" t="s">
@@ -13786,7 +13786,7 @@
       <c r="A102" s="1">
         <v>100</v>
       </c>
-      <c r="B102" s="77"/>
+      <c r="B102" s="80"/>
       <c r="C102" s="8" t="s">
         <v>871</v>
       </c>
@@ -13834,7 +13834,7 @@
       <c r="A104" s="1">
         <v>102</v>
       </c>
-      <c r="B104" s="76" t="s">
+      <c r="B104" s="79" t="s">
         <v>876</v>
       </c>
       <c r="C104" s="8" t="s">
@@ -13858,7 +13858,7 @@
       <c r="A105" s="1">
         <v>103</v>
       </c>
-      <c r="B105" s="78"/>
+      <c r="B105" s="81"/>
       <c r="C105" s="8" t="s">
         <v>879</v>
       </c>
@@ -13880,7 +13880,7 @@
       <c r="A106" s="1">
         <v>104</v>
       </c>
-      <c r="B106" s="78"/>
+      <c r="B106" s="81"/>
       <c r="C106" s="8" t="s">
         <v>881</v>
       </c>
@@ -13902,7 +13902,7 @@
       <c r="A107" s="1">
         <v>105</v>
       </c>
-      <c r="B107" s="77"/>
+      <c r="B107" s="80"/>
       <c r="C107" s="8" t="s">
         <v>883</v>
       </c>
@@ -13952,7 +13952,7 @@
       <c r="A109" s="1">
         <v>107</v>
       </c>
-      <c r="B109" s="76" t="s">
+      <c r="B109" s="79" t="s">
         <v>888</v>
       </c>
       <c r="C109" s="8" t="s">
@@ -13974,7 +13974,7 @@
       <c r="A110" s="1">
         <v>108</v>
       </c>
-      <c r="B110" s="77"/>
+      <c r="B110" s="80"/>
       <c r="C110" s="8" t="s">
         <v>891</v>
       </c>
@@ -13994,7 +13994,7 @@
       <c r="A111" s="1">
         <v>109</v>
       </c>
-      <c r="B111" s="76" t="s">
+      <c r="B111" s="79" t="s">
         <v>893</v>
       </c>
       <c r="C111" s="8" t="s">
@@ -14018,7 +14018,7 @@
       <c r="A112" s="1">
         <v>110</v>
       </c>
-      <c r="B112" s="77"/>
+      <c r="B112" s="80"/>
       <c r="C112" s="8" t="s">
         <v>896</v>
       </c>
@@ -14064,7 +14064,7 @@
       <c r="A114" s="1">
         <v>112</v>
       </c>
-      <c r="B114" s="76" t="s">
+      <c r="B114" s="79" t="s">
         <v>901</v>
       </c>
       <c r="C114" s="8" t="s">
@@ -14088,7 +14088,7 @@
       <c r="A115" s="1">
         <v>113</v>
       </c>
-      <c r="B115" s="77"/>
+      <c r="B115" s="80"/>
       <c r="C115" s="8" t="s">
         <v>904</v>
       </c>
@@ -14132,7 +14132,7 @@
       <c r="A117" s="1">
         <v>115</v>
       </c>
-      <c r="B117" s="76" t="s">
+      <c r="B117" s="79" t="s">
         <v>909</v>
       </c>
       <c r="C117" s="8" t="s">
@@ -14154,7 +14154,7 @@
       <c r="A118" s="1">
         <v>116</v>
       </c>
-      <c r="B118" s="78"/>
+      <c r="B118" s="81"/>
       <c r="C118" s="8" t="s">
         <v>912</v>
       </c>
@@ -14174,7 +14174,7 @@
       <c r="A119" s="1">
         <v>117</v>
       </c>
-      <c r="B119" s="78"/>
+      <c r="B119" s="81"/>
       <c r="C119" s="8" t="s">
         <v>914</v>
       </c>
@@ -14194,7 +14194,7 @@
       <c r="A120" s="1">
         <v>118</v>
       </c>
-      <c r="B120" s="77"/>
+      <c r="B120" s="80"/>
       <c r="C120" s="8" t="s">
         <v>916</v>
       </c>
@@ -14214,7 +14214,7 @@
       <c r="A121" s="1">
         <v>119</v>
       </c>
-      <c r="B121" s="76" t="s">
+      <c r="B121" s="79" t="s">
         <v>918</v>
       </c>
       <c r="C121" s="8" t="s">
@@ -14238,7 +14238,7 @@
       <c r="A122" s="1">
         <v>120</v>
       </c>
-      <c r="B122" s="78"/>
+      <c r="B122" s="81"/>
       <c r="C122" s="8" t="s">
         <v>921</v>
       </c>
@@ -14260,7 +14260,7 @@
       <c r="A123" s="1">
         <v>121</v>
       </c>
-      <c r="B123" s="77"/>
+      <c r="B123" s="80"/>
       <c r="C123" s="8" t="s">
         <v>923</v>
       </c>
@@ -14306,7 +14306,7 @@
       <c r="A125" s="1">
         <v>123</v>
       </c>
-      <c r="B125" s="76" t="s">
+      <c r="B125" s="79" t="s">
         <v>928</v>
       </c>
       <c r="C125" s="8" t="s">
@@ -14330,7 +14330,7 @@
       <c r="A126" s="1">
         <v>124</v>
       </c>
-      <c r="B126" s="78"/>
+      <c r="B126" s="81"/>
       <c r="C126" s="8" t="s">
         <v>931</v>
       </c>
@@ -14352,7 +14352,7 @@
       <c r="A127" s="1">
         <v>125</v>
       </c>
-      <c r="B127" s="78"/>
+      <c r="B127" s="81"/>
       <c r="C127" s="8" t="s">
         <v>933</v>
       </c>
@@ -14376,7 +14376,7 @@
       <c r="A128" s="1">
         <v>126</v>
       </c>
-      <c r="B128" s="78"/>
+      <c r="B128" s="81"/>
       <c r="C128" s="8" t="s">
         <v>935</v>
       </c>
@@ -14398,7 +14398,7 @@
       <c r="A129" s="1">
         <v>127</v>
       </c>
-      <c r="B129" s="78"/>
+      <c r="B129" s="81"/>
       <c r="C129" s="8" t="s">
         <v>937</v>
       </c>
@@ -14420,7 +14420,7 @@
       <c r="A130" s="1">
         <v>128</v>
       </c>
-      <c r="B130" s="77"/>
+      <c r="B130" s="80"/>
       <c r="C130" s="8" t="s">
         <v>939</v>
       </c>
@@ -14466,7 +14466,7 @@
       <c r="A132" s="1">
         <v>130</v>
       </c>
-      <c r="B132" s="76" t="s">
+      <c r="B132" s="79" t="s">
         <v>944</v>
       </c>
       <c r="C132" s="8" t="s">
@@ -14490,7 +14490,7 @@
       <c r="A133" s="1">
         <v>131</v>
       </c>
-      <c r="B133" s="77"/>
+      <c r="B133" s="80"/>
       <c r="C133" s="8" t="s">
         <v>947</v>
       </c>
@@ -14636,7 +14636,7 @@
       <c r="A139" s="1">
         <v>137</v>
       </c>
-      <c r="B139" s="76" t="s">
+      <c r="B139" s="79" t="s">
         <v>964</v>
       </c>
       <c r="C139" s="8" t="s">
@@ -14660,7 +14660,7 @@
       <c r="A140" s="1">
         <v>138</v>
       </c>
-      <c r="B140" s="77"/>
+      <c r="B140" s="80"/>
       <c r="C140" s="8" t="s">
         <v>967</v>
       </c>
@@ -14685,6 +14685,41 @@
     </sortState>
   </autoFilter>
   <mergeCells count="45">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="B90:B92"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="B98:B100"/>
     <mergeCell ref="B101:B102"/>
     <mergeCell ref="B104:B107"/>
     <mergeCell ref="B109:B110"/>
@@ -14695,41 +14730,6 @@
     <mergeCell ref="B121:B123"/>
     <mergeCell ref="B125:B130"/>
     <mergeCell ref="B132:B133"/>
-    <mergeCell ref="B87:B89"/>
-    <mergeCell ref="B90:B92"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B65:B69"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -14744,7 +14744,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14764,19 +14764,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="84" t="s">
         <v>969</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="83"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="86"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
@@ -14817,7 +14817,7 @@
       <c r="A3" s="52">
         <v>1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="87" t="s">
         <v>1184</v>
       </c>
       <c r="C3" s="53" t="s">
@@ -14842,7 +14842,7 @@
       <c r="A4" s="52">
         <v>2</v>
       </c>
-      <c r="B4" s="86"/>
+      <c r="B4" s="89"/>
       <c r="C4" s="47" t="s">
         <v>1199</v>
       </c>
@@ -14865,7 +14865,7 @@
       <c r="A5" s="52">
         <v>3</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="87" t="s">
         <v>1183</v>
       </c>
       <c r="C5" s="56" t="s">
@@ -14874,10 +14874,10 @@
       <c r="D5" s="57">
         <v>43664</v>
       </c>
-      <c r="E5" s="87" t="s">
+      <c r="E5" s="70" t="s">
         <v>1210</v>
       </c>
-      <c r="F5" s="88" t="s">
+      <c r="F5" s="71" t="s">
         <v>1179</v>
       </c>
       <c r="G5" s="52"/>
@@ -14890,7 +14890,7 @@
       <c r="A6" s="52">
         <v>4</v>
       </c>
-      <c r="B6" s="85"/>
+      <c r="B6" s="88"/>
       <c r="C6" s="47" t="s">
         <v>1200</v>
       </c>
@@ -14913,17 +14913,17 @@
       <c r="A7" s="52">
         <v>5</v>
       </c>
-      <c r="B7" s="85"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="56" t="s">
         <v>1200</v>
       </c>
       <c r="D7" s="57">
         <v>43664</v>
       </c>
-      <c r="E7" s="87" t="s">
+      <c r="E7" s="70" t="s">
         <v>1204</v>
       </c>
-      <c r="F7" s="88" t="s">
+      <c r="F7" s="71" t="s">
         <v>1143</v>
       </c>
       <c r="G7" s="52"/>
@@ -14936,17 +14936,17 @@
       <c r="A8" s="52">
         <v>6</v>
       </c>
-      <c r="B8" s="85"/>
+      <c r="B8" s="88"/>
       <c r="C8" s="56" t="s">
         <v>1200</v>
       </c>
       <c r="D8" s="57">
         <v>43664</v>
       </c>
-      <c r="E8" s="87" t="s">
+      <c r="E8" s="70" t="s">
         <v>1219</v>
       </c>
-      <c r="F8" s="88" t="s">
+      <c r="F8" s="71" t="s">
         <v>1144</v>
       </c>
       <c r="G8" s="52"/>
@@ -14959,17 +14959,17 @@
       <c r="A9" s="52">
         <v>7</v>
       </c>
-      <c r="B9" s="85"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="56" t="s">
         <v>1200</v>
       </c>
       <c r="D9" s="57">
         <v>43664</v>
       </c>
-      <c r="E9" s="87" t="s">
+      <c r="E9" s="70" t="s">
         <v>1218</v>
       </c>
-      <c r="F9" s="88" t="s">
+      <c r="F9" s="71" t="s">
         <v>1145</v>
       </c>
       <c r="G9" s="52"/>
@@ -14982,17 +14982,17 @@
       <c r="A10" s="52">
         <v>8</v>
       </c>
-      <c r="B10" s="85"/>
+      <c r="B10" s="88"/>
       <c r="C10" s="56" t="s">
         <v>1200</v>
       </c>
       <c r="D10" s="57">
         <v>43664</v>
       </c>
-      <c r="E10" s="87" t="s">
+      <c r="E10" s="70" t="s">
         <v>1205</v>
       </c>
-      <c r="F10" s="88" t="s">
+      <c r="F10" s="71" t="s">
         <v>1146</v>
       </c>
       <c r="G10" s="52"/>
@@ -15005,7 +15005,7 @@
       <c r="A11" s="52">
         <v>10</v>
       </c>
-      <c r="B11" s="85"/>
+      <c r="B11" s="88"/>
       <c r="C11" s="47" t="s">
         <v>1200</v>
       </c>
@@ -15028,7 +15028,7 @@
       <c r="A12" s="52">
         <v>11</v>
       </c>
-      <c r="B12" s="85"/>
+      <c r="B12" s="88"/>
       <c r="C12" s="47" t="s">
         <v>1200</v>
       </c>
@@ -15051,7 +15051,7 @@
       <c r="A13" s="52">
         <v>13</v>
       </c>
-      <c r="B13" s="85"/>
+      <c r="B13" s="88"/>
       <c r="C13" s="47" t="s">
         <v>1200</v>
       </c>
@@ -15074,17 +15074,17 @@
       <c r="A14" s="52">
         <v>14</v>
       </c>
-      <c r="B14" s="86"/>
+      <c r="B14" s="89"/>
       <c r="C14" s="56" t="s">
         <v>1200</v>
       </c>
       <c r="D14" s="57">
         <v>43664</v>
       </c>
-      <c r="E14" s="87" t="s">
+      <c r="E14" s="70" t="s">
         <v>1209</v>
       </c>
-      <c r="F14" s="88" t="s">
+      <c r="F14" s="71" t="s">
         <v>1182</v>
       </c>
       <c r="G14" s="52"/>
@@ -15197,7 +15197,7 @@
       <c r="A19" s="52">
         <v>19</v>
       </c>
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="87" t="s">
         <v>1186</v>
       </c>
       <c r="C19" s="60" t="s">
@@ -15222,7 +15222,7 @@
       <c r="A20" s="52">
         <v>20</v>
       </c>
-      <c r="B20" s="85"/>
+      <c r="B20" s="88"/>
       <c r="C20" s="60" t="s">
         <v>1199</v>
       </c>
@@ -15245,7 +15245,7 @@
       <c r="A21" s="52">
         <v>21</v>
       </c>
-      <c r="B21" s="85"/>
+      <c r="B21" s="88"/>
       <c r="C21" s="60" t="s">
         <v>1199</v>
       </c>
@@ -15268,7 +15268,7 @@
       <c r="A22" s="52">
         <v>22</v>
       </c>
-      <c r="B22" s="85"/>
+      <c r="B22" s="88"/>
       <c r="C22" s="60" t="s">
         <v>1199</v>
       </c>
@@ -15291,7 +15291,7 @@
       <c r="A23" s="52">
         <v>23</v>
       </c>
-      <c r="B23" s="85"/>
+      <c r="B23" s="88"/>
       <c r="C23" s="60" t="s">
         <v>1199</v>
       </c>
@@ -15312,7 +15312,7 @@
     </row>
     <row r="24" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="52"/>
-      <c r="B24" s="85"/>
+      <c r="B24" s="88"/>
       <c r="C24" s="60" t="s">
         <v>1199</v>
       </c>
@@ -15335,7 +15335,7 @@
       <c r="A25" s="52">
         <v>24</v>
       </c>
-      <c r="B25" s="86"/>
+      <c r="B25" s="89"/>
       <c r="C25" s="59" t="s">
         <v>1199</v>
       </c>
@@ -15358,7 +15358,7 @@
       <c r="A26" s="52">
         <v>25</v>
       </c>
-      <c r="B26" s="84" t="s">
+      <c r="B26" s="87" t="s">
         <v>1194</v>
       </c>
       <c r="C26" s="60" t="s">
@@ -15367,10 +15367,10 @@
       <c r="D26" s="57">
         <v>43664</v>
       </c>
-      <c r="E26" s="89" t="s">
+      <c r="E26" s="72" t="s">
         <v>1135</v>
       </c>
-      <c r="F26" s="88" t="s">
+      <c r="F26" s="71" t="s">
         <v>1162</v>
       </c>
       <c r="G26" s="52"/>
@@ -15383,17 +15383,17 @@
       <c r="A27" s="52">
         <v>26</v>
       </c>
-      <c r="B27" s="86"/>
+      <c r="B27" s="89"/>
       <c r="C27" s="56" t="s">
         <v>1200</v>
       </c>
       <c r="D27" s="57">
         <v>43664</v>
       </c>
-      <c r="E27" s="89" t="s">
+      <c r="E27" s="72" t="s">
         <v>1217</v>
       </c>
-      <c r="F27" s="88" t="s">
+      <c r="F27" s="71" t="s">
         <v>1171</v>
       </c>
       <c r="G27" s="52"/>
@@ -15406,7 +15406,7 @@
       <c r="A28" s="52">
         <v>27</v>
       </c>
-      <c r="B28" s="84" t="s">
+      <c r="B28" s="87" t="s">
         <v>1187</v>
       </c>
       <c r="C28" s="60" t="s">
@@ -15431,7 +15431,7 @@
       <c r="A29" s="52">
         <v>28</v>
       </c>
-      <c r="B29" s="86"/>
+      <c r="B29" s="89"/>
       <c r="C29" s="59" t="s">
         <v>1199</v>
       </c>
@@ -15454,7 +15454,7 @@
       <c r="A30" s="52">
         <v>29</v>
       </c>
-      <c r="B30" s="84" t="s">
+      <c r="B30" s="87" t="s">
         <v>1188</v>
       </c>
       <c r="C30" s="60" t="s">
@@ -15479,7 +15479,7 @@
       <c r="A31" s="52">
         <v>30</v>
       </c>
-      <c r="B31" s="85"/>
+      <c r="B31" s="88"/>
       <c r="C31" s="61" t="s">
         <v>1198</v>
       </c>
@@ -15502,7 +15502,7 @@
       <c r="A32" s="52">
         <v>31</v>
       </c>
-      <c r="B32" s="85"/>
+      <c r="B32" s="88"/>
       <c r="C32" s="61" t="s">
         <v>1198</v>
       </c>
@@ -15525,7 +15525,7 @@
       <c r="A33" s="52">
         <v>32</v>
       </c>
-      <c r="B33" s="85"/>
+      <c r="B33" s="88"/>
       <c r="C33" s="61" t="s">
         <v>1198</v>
       </c>
@@ -15546,7 +15546,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="52"/>
-      <c r="B34" s="85"/>
+      <c r="B34" s="88"/>
       <c r="C34" s="62" t="s">
         <v>1198</v>
       </c>
@@ -15569,7 +15569,7 @@
       <c r="A35" s="52">
         <v>33</v>
       </c>
-      <c r="B35" s="86"/>
+      <c r="B35" s="89"/>
       <c r="C35" s="61" t="s">
         <v>1198</v>
       </c>
@@ -15592,7 +15592,7 @@
       <c r="A36" s="52">
         <v>34</v>
       </c>
-      <c r="B36" s="84" t="s">
+      <c r="B36" s="87" t="s">
         <v>1189</v>
       </c>
       <c r="C36" s="56" t="s">
@@ -15617,7 +15617,7 @@
       <c r="A37" s="52">
         <v>35</v>
       </c>
-      <c r="B37" s="85"/>
+      <c r="B37" s="88"/>
       <c r="C37" s="56" t="s">
         <v>1197</v>
       </c>
@@ -15640,7 +15640,7 @@
       <c r="A38" s="52">
         <v>36</v>
       </c>
-      <c r="B38" s="85"/>
+      <c r="B38" s="88"/>
       <c r="C38" s="56" t="s">
         <v>1197</v>
       </c>
@@ -15663,7 +15663,7 @@
       <c r="A39" s="52">
         <v>37</v>
       </c>
-      <c r="B39" s="86"/>
+      <c r="B39" s="89"/>
       <c r="C39" s="56" t="s">
         <v>1197</v>
       </c>
@@ -15686,7 +15686,7 @@
       <c r="A40" s="52">
         <v>38</v>
       </c>
-      <c r="B40" s="84" t="s">
+      <c r="B40" s="87" t="s">
         <v>1191</v>
       </c>
       <c r="C40" s="53" t="s">
@@ -15711,7 +15711,7 @@
       <c r="A41" s="52">
         <v>39</v>
       </c>
-      <c r="B41" s="86"/>
+      <c r="B41" s="89"/>
       <c r="C41" s="47" t="s">
         <v>1199</v>
       </c>
@@ -15759,7 +15759,7 @@
       <c r="A43" s="52">
         <v>49</v>
       </c>
-      <c r="B43" s="85"/>
+      <c r="B43" s="88"/>
       <c r="C43" s="56" t="s">
         <v>1197</v>
       </c>
@@ -15782,7 +15782,7 @@
       <c r="A44" s="52">
         <v>50</v>
       </c>
-      <c r="B44" s="85"/>
+      <c r="B44" s="88"/>
       <c r="C44" s="56" t="s">
         <v>1197</v>
       </c>
@@ -15805,7 +15805,7 @@
       <c r="A45" s="52">
         <v>51</v>
       </c>
-      <c r="B45" s="85"/>
+      <c r="B45" s="88"/>
       <c r="C45" s="56" t="s">
         <v>1197</v>
       </c>
@@ -15828,7 +15828,7 @@
       <c r="A46" s="52">
         <v>52</v>
       </c>
-      <c r="B46" s="86"/>
+      <c r="B46" s="89"/>
       <c r="C46" s="56" t="s">
         <v>1197</v>
       </c>
@@ -15873,6 +15873,41 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16079,42 +16114,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7F7E23-FE37-4AB8-A4B3-5025B5D9E450}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16131,29 +16156,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Partner Management status file
</commit_message>
<xml_diff>
--- a/_files/requirements/requirements_detailing_references/Partner Management/Pending_Backlog_Stories_Status Tracking.xlsx
+++ b/_files/requirements/requirements_detailing_references/Partner Management/Pending_Backlog_Stories_Status Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP wiki Open Source\Requirements\_files\requirements\requirements_detailing_references\Partner Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{93D8F3A2-19EB-487D-95FD-C6EA67FDBE93}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{88804382-E626-49E1-800F-3FA2714F6E16}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14685,41 +14685,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="45">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B65:B69"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B87:B89"/>
-    <mergeCell ref="B90:B92"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="B98:B100"/>
     <mergeCell ref="B101:B102"/>
     <mergeCell ref="B104:B107"/>
     <mergeCell ref="B109:B110"/>
@@ -14730,6 +14695,41 @@
     <mergeCell ref="B121:B123"/>
     <mergeCell ref="B125:B130"/>
     <mergeCell ref="B132:B133"/>
+    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="B90:B92"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -15873,41 +15873,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16114,32 +16079,42 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7F7E23-FE37-4AB8-A4B3-5025B5D9E450}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16156,4 +16131,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating status file for Partner Management
</commit_message>
<xml_diff>
--- a/_files/requirements/requirements_detailing_references/Partner Management/Pending_Backlog_Stories_Status Tracking.xlsx
+++ b/_files/requirements/requirements_detailing_references/Partner Management/Pending_Backlog_Stories_Status Tracking.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP wiki Open Source\Requirements\_files\requirements\requirements_detailing_references\Partner Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\Project\PMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{88804382-E626-49E1-800F-3FA2714F6E16}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C63D6701-41E3-42A9-B38A-51343EFFDAB3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4643,7 +4643,7 @@
     <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4898,6 +4898,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -14685,6 +14688,41 @@
     </sortState>
   </autoFilter>
   <mergeCells count="45">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="B90:B92"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="B98:B100"/>
     <mergeCell ref="B101:B102"/>
     <mergeCell ref="B104:B107"/>
     <mergeCell ref="B109:B110"/>
@@ -14695,41 +14733,6 @@
     <mergeCell ref="B121:B123"/>
     <mergeCell ref="B125:B130"/>
     <mergeCell ref="B132:B133"/>
-    <mergeCell ref="B87:B89"/>
-    <mergeCell ref="B90:B92"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B65:B69"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -14744,7 +14747,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14900,7 +14903,7 @@
       <c r="E6" s="46" t="s">
         <v>1203</v>
       </c>
-      <c r="F6" s="67" t="s">
+      <c r="F6" s="90" t="s">
         <v>1142</v>
       </c>
       <c r="G6" s="52"/>
@@ -15038,7 +15041,7 @@
       <c r="E12" s="46" t="s">
         <v>1207</v>
       </c>
-      <c r="F12" s="67" t="s">
+      <c r="F12" s="90" t="s">
         <v>1178</v>
       </c>
       <c r="G12" s="52"/>
@@ -15061,7 +15064,7 @@
       <c r="E13" s="46" t="s">
         <v>1208</v>
       </c>
-      <c r="F13" s="67" t="s">
+      <c r="F13" s="90" t="s">
         <v>1181</v>
       </c>
       <c r="G13" s="52"/>
@@ -15109,7 +15112,7 @@
       <c r="E15" s="54" t="s">
         <v>1126</v>
       </c>
-      <c r="F15" s="67" t="s">
+      <c r="F15" s="90" t="s">
         <v>1156</v>
       </c>
       <c r="G15" s="52"/>
@@ -15159,7 +15162,7 @@
       <c r="E17" s="54" t="s">
         <v>1134</v>
       </c>
-      <c r="F17" s="67" t="s">
+      <c r="F17" s="90" t="s">
         <v>1170</v>
       </c>
       <c r="G17" s="52"/>
@@ -15184,7 +15187,7 @@
       <c r="E18" s="54" t="s">
         <v>1125</v>
       </c>
-      <c r="F18" s="67" t="s">
+      <c r="F18" s="90" t="s">
         <v>1155</v>
       </c>
       <c r="G18" s="52"/>
@@ -15873,6 +15876,41 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16079,42 +16117,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7F7E23-FE37-4AB8-A4B3-5025B5D9E450}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16131,29 +16159,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update files for IDA/PM
</commit_message>
<xml_diff>
--- a/_files/requirements/requirements_detailing_references/Partner Management/Pending_Backlog_Stories_Status Tracking.xlsx
+++ b/_files/requirements/requirements_detailing_references/Partner Management/Pending_Backlog_Stories_Status Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\Project\PMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C63D6701-41E3-42A9-B38A-51343EFFDAB3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E1F4E65-FA01-4E10-92AB-8227AB6FCF58}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Admin!$A$2:$I$115</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ID-Authentication'!$A$2:$J$44</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Kernel!$A$2:$I$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Partner Management'!$A$2:$K$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Partner Management'!$A$2:$K$44</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Pre-registration'!$A$2:$I$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Registration Client'!$A$2:$I$73</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Registration Processor'!$A$2:$I$31</definedName>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2194" uniqueCount="1222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="1217">
   <si>
     <t>Story Backlog: Pre-registration</t>
   </si>
@@ -3724,12 +3724,6 @@
     <t>MOS-24503</t>
   </si>
   <si>
-    <t>MOS-24502</t>
-  </si>
-  <si>
-    <t>MOS-24501</t>
-  </si>
-  <si>
     <t>MOS-24500</t>
   </si>
   <si>
@@ -3824,9 +3818,6 @@
   </si>
   <si>
     <t>Integration with IDA for PM</t>
-  </si>
-  <si>
-    <t>Public Key Management</t>
   </si>
   <si>
     <t>As the Partner Manger, I should be able to retrieve Partner API key to Policy Mappings</t>
@@ -3950,18 +3941,12 @@
       <t xml:space="preserve"> Manager ID</t>
     </r>
   </si>
-  <si>
-    <t>As the MOSIP system, I should be able to retrieve Public key from Partners for encryption of e-kyc response [To be deleted]</t>
-  </si>
-  <si>
-    <t>As the MOSIP system, I should be able to distribute Public Key to Partners for Encryption of auth/KYC Request [To be deleted]</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4177,18 +4162,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF7030A0"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Cambria"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4389,6 +4368,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4643,7 +4628,7 @@
     <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4770,15 +4755,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4789,9 +4765,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4825,26 +4798,14 @@
     <xf numFmtId="0" fontId="28" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4900,7 +4861,16 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5281,12 +5251,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="65" t="s">
         <v>984</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="75"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -5835,17 +5805,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="75"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -5880,7 +5850,7 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="68" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -5907,7 +5877,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="77"/>
+      <c r="B4" s="69"/>
       <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
@@ -5932,7 +5902,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="77"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
@@ -5957,7 +5927,7 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="77"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
@@ -5982,7 +5952,7 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="77"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
@@ -6009,7 +5979,7 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="78"/>
+      <c r="B8" s="70"/>
       <c r="C8" s="6" t="s">
         <v>30</v>
       </c>
@@ -6237,7 +6207,7 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="76" t="s">
+      <c r="B16" s="68" t="s">
         <v>67</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -6264,7 +6234,7 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="78"/>
+      <c r="B17" s="70"/>
       <c r="C17" s="6" t="s">
         <v>71</v>
       </c>
@@ -6289,7 +6259,7 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="68" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -6316,7 +6286,7 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="78"/>
+      <c r="B19" s="70"/>
       <c r="C19" s="6" t="s">
         <v>64</v>
       </c>
@@ -6438,17 +6408,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="75"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -6510,7 +6480,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="71" t="s">
         <v>1020</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -6537,7 +6507,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="80"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="6" t="s">
         <v>92</v>
       </c>
@@ -6786,7 +6756,7 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="71" t="s">
         <v>1055</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -6815,7 +6785,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="80"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="6" t="s">
         <v>121</v>
       </c>
@@ -7004,7 +6974,7 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="79" t="s">
+      <c r="B22" s="71" t="s">
         <v>1038</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -7031,7 +7001,7 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="81"/>
+      <c r="B23" s="73"/>
       <c r="C23" s="6" t="s">
         <v>185</v>
       </c>
@@ -7056,7 +7026,7 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="80"/>
+      <c r="B24" s="72"/>
       <c r="C24" s="6" t="s">
         <v>188</v>
       </c>
@@ -7220,7 +7190,7 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="71" t="s">
         <v>1057</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -7249,7 +7219,7 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="80"/>
+      <c r="B31" s="72"/>
       <c r="C31" s="6" t="s">
         <v>142</v>
       </c>
@@ -7276,7 +7246,7 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="79" t="s">
+      <c r="B32" s="71" t="s">
         <v>1058</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -7305,7 +7275,7 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="80"/>
+      <c r="B33" s="72"/>
       <c r="C33" s="6" t="s">
         <v>147</v>
       </c>
@@ -7529,7 +7499,7 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="79" t="s">
+      <c r="B41" s="71" t="s">
         <v>194</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -7558,7 +7528,7 @@
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="80"/>
+      <c r="B42" s="72"/>
       <c r="C42" s="6" t="s">
         <v>197</v>
       </c>
@@ -7612,7 +7582,7 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="79" t="s">
+      <c r="B44" s="71" t="s">
         <v>1034</v>
       </c>
       <c r="C44" s="6" t="s">
@@ -7641,7 +7611,7 @@
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" s="80"/>
+      <c r="B45" s="72"/>
       <c r="C45" s="6" t="s">
         <v>208</v>
       </c>
@@ -7724,7 +7694,7 @@
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="79" t="s">
+      <c r="B48" s="71" t="s">
         <v>222</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -7745,7 +7715,7 @@
       <c r="H48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I48" s="76" t="s">
+      <c r="I48" s="68" t="s">
         <v>1000</v>
       </c>
     </row>
@@ -7753,7 +7723,7 @@
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" s="81"/>
+      <c r="B49" s="73"/>
       <c r="C49" s="6" t="s">
         <v>226</v>
       </c>
@@ -7772,13 +7742,13 @@
       <c r="H49" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I49" s="77"/>
+      <c r="I49" s="69"/>
     </row>
     <row r="50" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="81"/>
+      <c r="B50" s="73"/>
       <c r="C50" s="6" t="s">
         <v>229</v>
       </c>
@@ -7797,13 +7767,13 @@
       <c r="H50" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I50" s="77"/>
+      <c r="I50" s="69"/>
     </row>
     <row r="51" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" s="81"/>
+      <c r="B51" s="73"/>
       <c r="C51" s="6" t="s">
         <v>232</v>
       </c>
@@ -7822,13 +7792,13 @@
       <c r="H51" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I51" s="77"/>
+      <c r="I51" s="69"/>
     </row>
     <row r="52" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" s="81"/>
+      <c r="B52" s="73"/>
       <c r="C52" s="6" t="s">
         <v>235</v>
       </c>
@@ -7847,13 +7817,13 @@
       <c r="H52" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I52" s="77"/>
+      <c r="I52" s="69"/>
     </row>
     <row r="53" spans="1:9" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="B53" s="81"/>
+      <c r="B53" s="73"/>
       <c r="C53" s="6" t="s">
         <v>238</v>
       </c>
@@ -7872,13 +7842,13 @@
       <c r="H53" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I53" s="77"/>
+      <c r="I53" s="69"/>
     </row>
     <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54" s="81"/>
+      <c r="B54" s="73"/>
       <c r="C54" s="6" t="s">
         <v>241</v>
       </c>
@@ -7897,13 +7867,13 @@
       <c r="H54" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I54" s="77"/>
+      <c r="I54" s="69"/>
     </row>
     <row r="55" spans="1:9" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55" s="81"/>
+      <c r="B55" s="73"/>
       <c r="C55" s="6" t="s">
         <v>244</v>
       </c>
@@ -7922,13 +7892,13 @@
       <c r="H55" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I55" s="77"/>
+      <c r="I55" s="69"/>
     </row>
     <row r="56" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56" s="81"/>
+      <c r="B56" s="73"/>
       <c r="C56" s="6" t="s">
         <v>1041</v>
       </c>
@@ -7943,13 +7913,13 @@
         <v>987</v>
       </c>
       <c r="H56" s="4"/>
-      <c r="I56" s="77"/>
+      <c r="I56" s="69"/>
     </row>
     <row r="57" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57" s="80"/>
+      <c r="B57" s="72"/>
       <c r="C57" s="6" t="s">
         <v>247</v>
       </c>
@@ -7968,13 +7938,13 @@
       <c r="H57" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I57" s="78"/>
+      <c r="I57" s="70"/>
     </row>
     <row r="58" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58" s="79" t="s">
+      <c r="B58" s="71" t="s">
         <v>222</v>
       </c>
       <c r="C58" s="6" t="s">
@@ -7995,7 +7965,7 @@
       <c r="H58" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I58" s="76" t="s">
+      <c r="I58" s="68" t="s">
         <v>1000</v>
       </c>
     </row>
@@ -8003,7 +7973,7 @@
       <c r="A59" s="1">
         <v>57</v>
       </c>
-      <c r="B59" s="81"/>
+      <c r="B59" s="73"/>
       <c r="C59" s="6" t="s">
         <v>253</v>
       </c>
@@ -8022,13 +7992,13 @@
       <c r="H59" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I59" s="77"/>
+      <c r="I59" s="69"/>
     </row>
     <row r="60" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
-      <c r="B60" s="81"/>
+      <c r="B60" s="73"/>
       <c r="C60" s="6" t="s">
         <v>256</v>
       </c>
@@ -8047,13 +8017,13 @@
       <c r="H60" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I60" s="77"/>
+      <c r="I60" s="69"/>
     </row>
     <row r="61" spans="1:9" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61" s="81"/>
+      <c r="B61" s="73"/>
       <c r="C61" s="6" t="s">
         <v>259</v>
       </c>
@@ -8072,13 +8042,13 @@
       <c r="H61" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I61" s="77"/>
+      <c r="I61" s="69"/>
     </row>
     <row r="62" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" s="81"/>
+      <c r="B62" s="73"/>
       <c r="C62" s="6" t="s">
         <v>262</v>
       </c>
@@ -8097,13 +8067,13 @@
       <c r="H62" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I62" s="77"/>
+      <c r="I62" s="69"/>
     </row>
     <row r="63" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" s="81"/>
+      <c r="B63" s="73"/>
       <c r="C63" s="6" t="s">
         <v>264</v>
       </c>
@@ -8122,13 +8092,13 @@
       <c r="H63" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I63" s="77"/>
+      <c r="I63" s="69"/>
     </row>
     <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" s="81"/>
+      <c r="B64" s="73"/>
       <c r="C64" s="6" t="s">
         <v>75</v>
       </c>
@@ -8147,13 +8117,13 @@
       <c r="H64" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I64" s="77"/>
+      <c r="I64" s="69"/>
     </row>
     <row r="65" spans="1:9" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" s="81"/>
+      <c r="B65" s="73"/>
       <c r="C65" s="6" t="s">
         <v>268</v>
       </c>
@@ -8172,13 +8142,13 @@
       <c r="H65" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I65" s="77"/>
+      <c r="I65" s="69"/>
     </row>
     <row r="66" spans="1:9" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" s="81"/>
+      <c r="B66" s="73"/>
       <c r="C66" s="6" t="s">
         <v>271</v>
       </c>
@@ -8197,13 +8167,13 @@
       <c r="H66" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I66" s="77"/>
+      <c r="I66" s="69"/>
     </row>
     <row r="67" spans="1:9" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" s="81"/>
+      <c r="B67" s="73"/>
       <c r="C67" s="6" t="s">
         <v>274</v>
       </c>
@@ -8222,13 +8192,13 @@
       <c r="H67" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I67" s="77"/>
+      <c r="I67" s="69"/>
     </row>
     <row r="68" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" s="81"/>
+      <c r="B68" s="73"/>
       <c r="C68" s="6" t="s">
         <v>277</v>
       </c>
@@ -8247,13 +8217,13 @@
       <c r="H68" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I68" s="77"/>
+      <c r="I68" s="69"/>
     </row>
     <row r="69" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69" s="81"/>
+      <c r="B69" s="73"/>
       <c r="C69" s="6" t="s">
         <v>280</v>
       </c>
@@ -8272,13 +8242,13 @@
       <c r="H69" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I69" s="77"/>
+      <c r="I69" s="69"/>
     </row>
     <row r="70" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
-      <c r="B70" s="81"/>
+      <c r="B70" s="73"/>
       <c r="C70" s="6" t="s">
         <v>283</v>
       </c>
@@ -8297,13 +8267,13 @@
       <c r="H70" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I70" s="77"/>
+      <c r="I70" s="69"/>
     </row>
     <row r="71" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" s="80"/>
+      <c r="B71" s="72"/>
       <c r="C71" s="6" t="s">
         <v>285</v>
       </c>
@@ -8322,7 +8292,7 @@
       <c r="H71" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I71" s="78"/>
+      <c r="I71" s="70"/>
     </row>
     <row r="72" spans="1:9" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
@@ -8517,17 +8487,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="65" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="75"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -9378,17 +9348,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="65" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="75"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -9533,7 +9503,7 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="71" t="s">
         <v>398</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -9560,7 +9530,7 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="82"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="6" t="s">
         <v>402</v>
       </c>
@@ -9585,7 +9555,7 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="82"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="6" t="s">
         <v>405</v>
       </c>
@@ -9610,7 +9580,7 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="82"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="6" t="s">
         <v>408</v>
       </c>
@@ -9635,7 +9605,7 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="82"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="6" t="s">
         <v>411</v>
       </c>
@@ -9660,7 +9630,7 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="82"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="6" t="s">
         <v>414</v>
       </c>
@@ -9685,7 +9655,7 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="82"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="6" t="s">
         <v>417</v>
       </c>
@@ -9710,7 +9680,7 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="83"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="6" t="s">
         <v>420</v>
       </c>
@@ -9930,7 +9900,7 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="79" t="s">
+      <c r="B22" s="71" t="s">
         <v>448</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -9957,7 +9927,7 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="82"/>
+      <c r="B23" s="74"/>
       <c r="C23" s="38" t="s">
         <v>452</v>
       </c>
@@ -9984,7 +9954,7 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="82"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="6" t="s">
         <v>455</v>
       </c>
@@ -10009,7 +9979,7 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="82"/>
+      <c r="B25" s="74"/>
       <c r="C25" s="6" t="s">
         <v>457</v>
       </c>
@@ -10034,7 +10004,7 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="82"/>
+      <c r="B26" s="74"/>
       <c r="C26" s="38" t="s">
         <v>459</v>
       </c>
@@ -10061,7 +10031,7 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="83"/>
+      <c r="B27" s="75"/>
       <c r="C27" s="6" t="s">
         <v>462</v>
       </c>
@@ -10140,7 +10110,7 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="71" t="s">
         <v>471</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -10167,7 +10137,7 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="82"/>
+      <c r="B31" s="74"/>
       <c r="C31" s="6" t="s">
         <v>475</v>
       </c>
@@ -10192,7 +10162,7 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="82"/>
+      <c r="B32" s="74"/>
       <c r="C32" s="6" t="s">
         <v>478</v>
       </c>
@@ -10217,7 +10187,7 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="83"/>
+      <c r="B33" s="75"/>
       <c r="C33" s="6" t="s">
         <v>481</v>
       </c>
@@ -10381,7 +10351,7 @@
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="79" t="s">
+      <c r="B39" s="71" t="s">
         <v>502</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -10408,7 +10378,7 @@
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="82"/>
+      <c r="B40" s="74"/>
       <c r="C40" s="6" t="s">
         <v>506</v>
       </c>
@@ -10433,7 +10403,7 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="83"/>
+      <c r="B41" s="75"/>
       <c r="C41" s="6" t="s">
         <v>509</v>
       </c>
@@ -10458,7 +10428,7 @@
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="79" t="s">
+      <c r="B42" s="71" t="s">
         <v>512</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -10483,7 +10453,7 @@
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" s="82"/>
+      <c r="B43" s="74"/>
       <c r="C43" s="6" t="s">
         <v>516</v>
       </c>
@@ -10506,7 +10476,7 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="83"/>
+      <c r="B44" s="75"/>
       <c r="C44" s="6" t="s">
         <v>519</v>
       </c>
@@ -10576,17 +10546,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="65" t="s">
         <v>522</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="75"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -10953,17 +10923,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="65" t="s">
         <v>550</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="75"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -11294,7 +11264,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="68" t="s">
         <v>601</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -11319,7 +11289,7 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="78"/>
+      <c r="B16" s="70"/>
       <c r="C16" s="6" t="s">
         <v>605</v>
       </c>
@@ -11458,18 +11428,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="65" t="s">
         <v>616</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="75"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="67"/>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -11507,7 +11477,7 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="71" t="s">
         <v>618</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -11531,7 +11501,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="80"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="8" t="s">
         <v>621</v>
       </c>
@@ -11553,7 +11523,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="71" t="s">
         <v>623</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -11577,7 +11547,7 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="80"/>
+      <c r="B6" s="72"/>
       <c r="C6" s="8" t="s">
         <v>626</v>
       </c>
@@ -11623,7 +11593,7 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="79" t="s">
+      <c r="B8" s="71" t="s">
         <v>631</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -11647,7 +11617,7 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="80"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="8" t="s">
         <v>634</v>
       </c>
@@ -11695,7 +11665,7 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="71" t="s">
         <v>640</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -11721,7 +11691,7 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="80"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="8" t="s">
         <v>643</v>
       </c>
@@ -11767,7 +11737,7 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="71" t="s">
         <v>648</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -11791,7 +11761,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="80"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="8" t="s">
         <v>651</v>
       </c>
@@ -11811,7 +11781,7 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="79" t="s">
+      <c r="B16" s="71" t="s">
         <v>653</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -11835,7 +11805,7 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="81"/>
+      <c r="B17" s="73"/>
       <c r="C17" s="8" t="s">
         <v>656</v>
       </c>
@@ -11859,7 +11829,7 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="80"/>
+      <c r="B18" s="72"/>
       <c r="C18" s="8" t="s">
         <v>658</v>
       </c>
@@ -11903,7 +11873,7 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="71" t="s">
         <v>663</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -11925,7 +11895,7 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="80"/>
+      <c r="B21" s="72"/>
       <c r="C21" s="8" t="s">
         <v>666</v>
       </c>
@@ -11969,7 +11939,7 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="79" t="s">
+      <c r="B23" s="71" t="s">
         <v>671</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -11993,7 +11963,7 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="80"/>
+      <c r="B24" s="72"/>
       <c r="C24" s="8" t="s">
         <v>674</v>
       </c>
@@ -12039,7 +12009,7 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="79" t="s">
+      <c r="B26" s="71" t="s">
         <v>679</v>
       </c>
       <c r="C26" s="8" t="s">
@@ -12063,7 +12033,7 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="81"/>
+      <c r="B27" s="73"/>
       <c r="C27" s="8" t="s">
         <v>682</v>
       </c>
@@ -12087,7 +12057,7 @@
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="80"/>
+      <c r="B28" s="72"/>
       <c r="C28" s="8" t="s">
         <v>684</v>
       </c>
@@ -12107,7 +12077,7 @@
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="79" t="s">
+      <c r="B29" s="71" t="s">
         <v>686</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -12131,7 +12101,7 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="80"/>
+      <c r="B30" s="72"/>
       <c r="C30" s="8" t="s">
         <v>689</v>
       </c>
@@ -12177,7 +12147,7 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="79" t="s">
+      <c r="B32" s="71" t="s">
         <v>694</v>
       </c>
       <c r="C32" s="8" t="s">
@@ -12201,7 +12171,7 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="80"/>
+      <c r="B33" s="72"/>
       <c r="C33" s="8" t="s">
         <v>697</v>
       </c>
@@ -12223,7 +12193,7 @@
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="79" t="s">
+      <c r="B34" s="71" t="s">
         <v>699</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -12247,7 +12217,7 @@
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" s="80"/>
+      <c r="B35" s="72"/>
       <c r="C35" s="8" t="s">
         <v>702</v>
       </c>
@@ -12315,7 +12285,7 @@
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" s="79" t="s">
+      <c r="B38" s="71" t="s">
         <v>710</v>
       </c>
       <c r="C38" s="8" t="s">
@@ -12339,7 +12309,7 @@
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="80"/>
+      <c r="B39" s="72"/>
       <c r="C39" s="8" t="s">
         <v>713</v>
       </c>
@@ -12361,7 +12331,7 @@
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="79" t="s">
+      <c r="B40" s="71" t="s">
         <v>715</v>
       </c>
       <c r="C40" s="8" t="s">
@@ -12385,7 +12355,7 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="80"/>
+      <c r="B41" s="72"/>
       <c r="C41" s="8" t="s">
         <v>718</v>
       </c>
@@ -12431,7 +12401,7 @@
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" s="79" t="s">
+      <c r="B43" s="71" t="s">
         <v>723</v>
       </c>
       <c r="C43" s="8" t="s">
@@ -12455,7 +12425,7 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="80"/>
+      <c r="B44" s="72"/>
       <c r="C44" s="8" t="s">
         <v>726</v>
       </c>
@@ -12477,7 +12447,7 @@
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" s="79" t="s">
+      <c r="B45" s="71" t="s">
         <v>728</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -12501,7 +12471,7 @@
       <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="B46" s="80"/>
+      <c r="B46" s="72"/>
       <c r="C46" s="8" t="s">
         <v>731</v>
       </c>
@@ -12525,7 +12495,7 @@
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" s="79" t="s">
+      <c r="B47" s="71" t="s">
         <v>733</v>
       </c>
       <c r="C47" s="8" t="s">
@@ -12549,7 +12519,7 @@
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="80"/>
+      <c r="B48" s="72"/>
       <c r="C48" s="8" t="s">
         <v>736</v>
       </c>
@@ -12569,7 +12539,7 @@
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" s="79" t="s">
+      <c r="B49" s="71" t="s">
         <v>738</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -12593,7 +12563,7 @@
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="80"/>
+      <c r="B50" s="72"/>
       <c r="C50" s="8" t="s">
         <v>741</v>
       </c>
@@ -12617,7 +12587,7 @@
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" s="79" t="s">
+      <c r="B51" s="71" t="s">
         <v>743</v>
       </c>
       <c r="C51" s="8" t="s">
@@ -12639,7 +12609,7 @@
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" s="80"/>
+      <c r="B52" s="72"/>
       <c r="C52" s="8" t="s">
         <v>746</v>
       </c>
@@ -12683,7 +12653,7 @@
       <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54" s="79" t="s">
+      <c r="B54" s="71" t="s">
         <v>751</v>
       </c>
       <c r="C54" s="8" t="s">
@@ -12707,7 +12677,7 @@
       <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55" s="81"/>
+      <c r="B55" s="73"/>
       <c r="C55" s="8" t="s">
         <v>754</v>
       </c>
@@ -12731,7 +12701,7 @@
       <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56" s="80"/>
+      <c r="B56" s="72"/>
       <c r="C56" s="8" t="s">
         <v>756</v>
       </c>
@@ -12751,7 +12721,7 @@
       <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57" s="79" t="s">
+      <c r="B57" s="71" t="s">
         <v>758</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -12775,7 +12745,7 @@
       <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58" s="80"/>
+      <c r="B58" s="72"/>
       <c r="C58" s="8" t="s">
         <v>761</v>
       </c>
@@ -12847,7 +12817,7 @@
       <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61" s="79" t="s">
+      <c r="B61" s="71" t="s">
         <v>769</v>
       </c>
       <c r="C61" s="8" t="s">
@@ -12871,7 +12841,7 @@
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" s="80"/>
+      <c r="B62" s="72"/>
       <c r="C62" s="8" t="s">
         <v>772</v>
       </c>
@@ -12895,7 +12865,7 @@
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" s="79" t="s">
+      <c r="B63" s="71" t="s">
         <v>774</v>
       </c>
       <c r="C63" s="8" t="s">
@@ -12919,7 +12889,7 @@
       <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" s="80"/>
+      <c r="B64" s="72"/>
       <c r="C64" s="8" t="s">
         <v>777</v>
       </c>
@@ -12945,7 +12915,7 @@
       <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" s="79" t="s">
+      <c r="B65" s="71" t="s">
         <v>780</v>
       </c>
       <c r="C65" s="8" t="s">
@@ -12969,7 +12939,7 @@
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" s="81"/>
+      <c r="B66" s="73"/>
       <c r="C66" s="8" t="s">
         <v>783</v>
       </c>
@@ -12991,7 +12961,7 @@
       <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" s="81"/>
+      <c r="B67" s="73"/>
       <c r="C67" s="8" t="s">
         <v>785</v>
       </c>
@@ -13013,7 +12983,7 @@
       <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" s="81"/>
+      <c r="B68" s="73"/>
       <c r="C68" s="8" t="s">
         <v>787</v>
       </c>
@@ -13035,7 +13005,7 @@
       <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69" s="80"/>
+      <c r="B69" s="72"/>
       <c r="C69" s="8" t="s">
         <v>789</v>
       </c>
@@ -13081,7 +13051,7 @@
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" s="79" t="s">
+      <c r="B71" s="71" t="s">
         <v>794</v>
       </c>
       <c r="C71" s="8" t="s">
@@ -13105,7 +13075,7 @@
       <c r="A72" s="1">
         <v>70</v>
       </c>
-      <c r="B72" s="80"/>
+      <c r="B72" s="72"/>
       <c r="C72" s="8" t="s">
         <v>797</v>
       </c>
@@ -13149,7 +13119,7 @@
       <c r="A74" s="1">
         <v>72</v>
       </c>
-      <c r="B74" s="79" t="s">
+      <c r="B74" s="71" t="s">
         <v>802</v>
       </c>
       <c r="C74" s="8" t="s">
@@ -13173,7 +13143,7 @@
       <c r="A75" s="1">
         <v>73</v>
       </c>
-      <c r="B75" s="80"/>
+      <c r="B75" s="72"/>
       <c r="C75" s="8" t="s">
         <v>805</v>
       </c>
@@ -13243,7 +13213,7 @@
       <c r="A78" s="1">
         <v>76</v>
       </c>
-      <c r="B78" s="79" t="s">
+      <c r="B78" s="71" t="s">
         <v>813</v>
       </c>
       <c r="C78" s="8" t="s">
@@ -13267,7 +13237,7 @@
       <c r="A79" s="1">
         <v>77</v>
       </c>
-      <c r="B79" s="80"/>
+      <c r="B79" s="72"/>
       <c r="C79" s="8" t="s">
         <v>816</v>
       </c>
@@ -13291,7 +13261,7 @@
       <c r="A80" s="1">
         <v>78</v>
       </c>
-      <c r="B80" s="79" t="s">
+      <c r="B80" s="71" t="s">
         <v>818</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -13315,7 +13285,7 @@
       <c r="A81" s="1">
         <v>79</v>
       </c>
-      <c r="B81" s="80"/>
+      <c r="B81" s="72"/>
       <c r="C81" s="8" t="s">
         <v>821</v>
       </c>
@@ -13339,7 +13309,7 @@
       <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B82" s="79" t="s">
+      <c r="B82" s="71" t="s">
         <v>823</v>
       </c>
       <c r="C82" s="8" t="s">
@@ -13363,7 +13333,7 @@
       <c r="A83" s="1">
         <v>81</v>
       </c>
-      <c r="B83" s="81"/>
+      <c r="B83" s="73"/>
       <c r="C83" s="8" t="s">
         <v>826</v>
       </c>
@@ -13385,7 +13355,7 @@
       <c r="A84" s="1">
         <v>82</v>
       </c>
-      <c r="B84" s="81"/>
+      <c r="B84" s="73"/>
       <c r="C84" s="8" t="s">
         <v>828</v>
       </c>
@@ -13407,7 +13377,7 @@
       <c r="A85" s="1">
         <v>83</v>
       </c>
-      <c r="B85" s="80"/>
+      <c r="B85" s="72"/>
       <c r="C85" s="8" t="s">
         <v>830</v>
       </c>
@@ -13451,7 +13421,7 @@
       <c r="A87" s="1">
         <v>85</v>
       </c>
-      <c r="B87" s="79" t="s">
+      <c r="B87" s="71" t="s">
         <v>834</v>
       </c>
       <c r="C87" s="8" t="s">
@@ -13475,7 +13445,7 @@
       <c r="A88" s="1">
         <v>86</v>
       </c>
-      <c r="B88" s="81"/>
+      <c r="B88" s="73"/>
       <c r="C88" s="8" t="s">
         <v>837</v>
       </c>
@@ -13497,7 +13467,7 @@
       <c r="A89" s="1">
         <v>87</v>
       </c>
-      <c r="B89" s="80"/>
+      <c r="B89" s="72"/>
       <c r="C89" s="8" t="s">
         <v>839</v>
       </c>
@@ -13519,7 +13489,7 @@
       <c r="A90" s="1">
         <v>88</v>
       </c>
-      <c r="B90" s="79" t="s">
+      <c r="B90" s="71" t="s">
         <v>841</v>
       </c>
       <c r="C90" s="8" t="s">
@@ -13543,7 +13513,7 @@
       <c r="A91" s="1">
         <v>89</v>
       </c>
-      <c r="B91" s="81"/>
+      <c r="B91" s="73"/>
       <c r="C91" s="8" t="s">
         <v>844</v>
       </c>
@@ -13563,7 +13533,7 @@
       <c r="A92" s="1">
         <v>90</v>
       </c>
-      <c r="B92" s="80"/>
+      <c r="B92" s="72"/>
       <c r="C92" s="8" t="s">
         <v>846</v>
       </c>
@@ -13583,7 +13553,7 @@
       <c r="A93" s="1">
         <v>91</v>
       </c>
-      <c r="B93" s="79" t="s">
+      <c r="B93" s="71" t="s">
         <v>848</v>
       </c>
       <c r="C93" s="8" t="s">
@@ -13607,7 +13577,7 @@
       <c r="A94" s="1">
         <v>92</v>
       </c>
-      <c r="B94" s="80"/>
+      <c r="B94" s="72"/>
       <c r="C94" s="8" t="s">
         <v>851</v>
       </c>
@@ -13631,7 +13601,7 @@
       <c r="A95" s="1">
         <v>93</v>
       </c>
-      <c r="B95" s="79" t="s">
+      <c r="B95" s="71" t="s">
         <v>853</v>
       </c>
       <c r="C95" s="8" t="s">
@@ -13653,7 +13623,7 @@
       <c r="A96" s="1">
         <v>94</v>
       </c>
-      <c r="B96" s="80"/>
+      <c r="B96" s="72"/>
       <c r="C96" s="8" t="s">
         <v>856</v>
       </c>
@@ -13697,7 +13667,7 @@
       <c r="A98" s="1">
         <v>96</v>
       </c>
-      <c r="B98" s="79" t="s">
+      <c r="B98" s="71" t="s">
         <v>861</v>
       </c>
       <c r="C98" s="8" t="s">
@@ -13721,7 +13691,7 @@
       <c r="A99" s="1">
         <v>97</v>
       </c>
-      <c r="B99" s="81"/>
+      <c r="B99" s="73"/>
       <c r="C99" s="8" t="s">
         <v>864</v>
       </c>
@@ -13745,7 +13715,7 @@
       <c r="A100" s="1">
         <v>98</v>
       </c>
-      <c r="B100" s="80"/>
+      <c r="B100" s="72"/>
       <c r="C100" s="8" t="s">
         <v>866</v>
       </c>
@@ -13765,7 +13735,7 @@
       <c r="A101" s="1">
         <v>99</v>
       </c>
-      <c r="B101" s="79" t="s">
+      <c r="B101" s="71" t="s">
         <v>868</v>
       </c>
       <c r="C101" s="8" t="s">
@@ -13789,7 +13759,7 @@
       <c r="A102" s="1">
         <v>100</v>
       </c>
-      <c r="B102" s="80"/>
+      <c r="B102" s="72"/>
       <c r="C102" s="8" t="s">
         <v>871</v>
       </c>
@@ -13837,7 +13807,7 @@
       <c r="A104" s="1">
         <v>102</v>
       </c>
-      <c r="B104" s="79" t="s">
+      <c r="B104" s="71" t="s">
         <v>876</v>
       </c>
       <c r="C104" s="8" t="s">
@@ -13861,7 +13831,7 @@
       <c r="A105" s="1">
         <v>103</v>
       </c>
-      <c r="B105" s="81"/>
+      <c r="B105" s="73"/>
       <c r="C105" s="8" t="s">
         <v>879</v>
       </c>
@@ -13883,7 +13853,7 @@
       <c r="A106" s="1">
         <v>104</v>
       </c>
-      <c r="B106" s="81"/>
+      <c r="B106" s="73"/>
       <c r="C106" s="8" t="s">
         <v>881</v>
       </c>
@@ -13905,7 +13875,7 @@
       <c r="A107" s="1">
         <v>105</v>
       </c>
-      <c r="B107" s="80"/>
+      <c r="B107" s="72"/>
       <c r="C107" s="8" t="s">
         <v>883</v>
       </c>
@@ -13955,7 +13925,7 @@
       <c r="A109" s="1">
         <v>107</v>
       </c>
-      <c r="B109" s="79" t="s">
+      <c r="B109" s="71" t="s">
         <v>888</v>
       </c>
       <c r="C109" s="8" t="s">
@@ -13977,7 +13947,7 @@
       <c r="A110" s="1">
         <v>108</v>
       </c>
-      <c r="B110" s="80"/>
+      <c r="B110" s="72"/>
       <c r="C110" s="8" t="s">
         <v>891</v>
       </c>
@@ -13997,7 +13967,7 @@
       <c r="A111" s="1">
         <v>109</v>
       </c>
-      <c r="B111" s="79" t="s">
+      <c r="B111" s="71" t="s">
         <v>893</v>
       </c>
       <c r="C111" s="8" t="s">
@@ -14021,7 +13991,7 @@
       <c r="A112" s="1">
         <v>110</v>
       </c>
-      <c r="B112" s="80"/>
+      <c r="B112" s="72"/>
       <c r="C112" s="8" t="s">
         <v>896</v>
       </c>
@@ -14067,7 +14037,7 @@
       <c r="A114" s="1">
         <v>112</v>
       </c>
-      <c r="B114" s="79" t="s">
+      <c r="B114" s="71" t="s">
         <v>901</v>
       </c>
       <c r="C114" s="8" t="s">
@@ -14091,7 +14061,7 @@
       <c r="A115" s="1">
         <v>113</v>
       </c>
-      <c r="B115" s="80"/>
+      <c r="B115" s="72"/>
       <c r="C115" s="8" t="s">
         <v>904</v>
       </c>
@@ -14135,7 +14105,7 @@
       <c r="A117" s="1">
         <v>115</v>
       </c>
-      <c r="B117" s="79" t="s">
+      <c r="B117" s="71" t="s">
         <v>909</v>
       </c>
       <c r="C117" s="8" t="s">
@@ -14157,7 +14127,7 @@
       <c r="A118" s="1">
         <v>116</v>
       </c>
-      <c r="B118" s="81"/>
+      <c r="B118" s="73"/>
       <c r="C118" s="8" t="s">
         <v>912</v>
       </c>
@@ -14177,7 +14147,7 @@
       <c r="A119" s="1">
         <v>117</v>
       </c>
-      <c r="B119" s="81"/>
+      <c r="B119" s="73"/>
       <c r="C119" s="8" t="s">
         <v>914</v>
       </c>
@@ -14197,7 +14167,7 @@
       <c r="A120" s="1">
         <v>118</v>
       </c>
-      <c r="B120" s="80"/>
+      <c r="B120" s="72"/>
       <c r="C120" s="8" t="s">
         <v>916</v>
       </c>
@@ -14217,7 +14187,7 @@
       <c r="A121" s="1">
         <v>119</v>
       </c>
-      <c r="B121" s="79" t="s">
+      <c r="B121" s="71" t="s">
         <v>918</v>
       </c>
       <c r="C121" s="8" t="s">
@@ -14241,7 +14211,7 @@
       <c r="A122" s="1">
         <v>120</v>
       </c>
-      <c r="B122" s="81"/>
+      <c r="B122" s="73"/>
       <c r="C122" s="8" t="s">
         <v>921</v>
       </c>
@@ -14263,7 +14233,7 @@
       <c r="A123" s="1">
         <v>121</v>
       </c>
-      <c r="B123" s="80"/>
+      <c r="B123" s="72"/>
       <c r="C123" s="8" t="s">
         <v>923</v>
       </c>
@@ -14309,7 +14279,7 @@
       <c r="A125" s="1">
         <v>123</v>
       </c>
-      <c r="B125" s="79" t="s">
+      <c r="B125" s="71" t="s">
         <v>928</v>
       </c>
       <c r="C125" s="8" t="s">
@@ -14333,7 +14303,7 @@
       <c r="A126" s="1">
         <v>124</v>
       </c>
-      <c r="B126" s="81"/>
+      <c r="B126" s="73"/>
       <c r="C126" s="8" t="s">
         <v>931</v>
       </c>
@@ -14355,7 +14325,7 @@
       <c r="A127" s="1">
         <v>125</v>
       </c>
-      <c r="B127" s="81"/>
+      <c r="B127" s="73"/>
       <c r="C127" s="8" t="s">
         <v>933</v>
       </c>
@@ -14379,7 +14349,7 @@
       <c r="A128" s="1">
         <v>126</v>
       </c>
-      <c r="B128" s="81"/>
+      <c r="B128" s="73"/>
       <c r="C128" s="8" t="s">
         <v>935</v>
       </c>
@@ -14401,7 +14371,7 @@
       <c r="A129" s="1">
         <v>127</v>
       </c>
-      <c r="B129" s="81"/>
+      <c r="B129" s="73"/>
       <c r="C129" s="8" t="s">
         <v>937</v>
       </c>
@@ -14423,7 +14393,7 @@
       <c r="A130" s="1">
         <v>128</v>
       </c>
-      <c r="B130" s="80"/>
+      <c r="B130" s="72"/>
       <c r="C130" s="8" t="s">
         <v>939</v>
       </c>
@@ -14469,7 +14439,7 @@
       <c r="A132" s="1">
         <v>130</v>
       </c>
-      <c r="B132" s="79" t="s">
+      <c r="B132" s="71" t="s">
         <v>944</v>
       </c>
       <c r="C132" s="8" t="s">
@@ -14493,7 +14463,7 @@
       <c r="A133" s="1">
         <v>131</v>
       </c>
-      <c r="B133" s="80"/>
+      <c r="B133" s="72"/>
       <c r="C133" s="8" t="s">
         <v>947</v>
       </c>
@@ -14639,7 +14609,7 @@
       <c r="A139" s="1">
         <v>137</v>
       </c>
-      <c r="B139" s="79" t="s">
+      <c r="B139" s="71" t="s">
         <v>964</v>
       </c>
       <c r="C139" s="8" t="s">
@@ -14663,7 +14633,7 @@
       <c r="A140" s="1">
         <v>138</v>
       </c>
-      <c r="B140" s="80"/>
+      <c r="B140" s="72"/>
       <c r="C140" s="8" t="s">
         <v>967</v>
       </c>
@@ -14688,41 +14658,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="45">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B65:B69"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B87:B89"/>
-    <mergeCell ref="B90:B92"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="B98:B100"/>
     <mergeCell ref="B101:B102"/>
     <mergeCell ref="B104:B107"/>
     <mergeCell ref="B109:B110"/>
@@ -14733,6 +14668,41 @@
     <mergeCell ref="B121:B123"/>
     <mergeCell ref="B125:B130"/>
     <mergeCell ref="B132:B133"/>
+    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="B90:B92"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -14741,13 +14711,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3:F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14767,1108 +14737,1059 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="76" t="s">
         <v>969</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="86"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="46" t="s">
         <v>617</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="46" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>551</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="49">
+        <v>1</v>
+      </c>
+      <c r="B3" s="79" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D3" s="53">
+        <v>43657</v>
+      </c>
+      <c r="E3" s="64" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F3" s="85" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G3" s="50"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+    </row>
+    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="49">
+        <v>2</v>
+      </c>
+      <c r="B4" s="81"/>
+      <c r="C4" s="52" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D4" s="53">
+        <v>43657</v>
+      </c>
+      <c r="E4" s="64" t="s">
+        <v>1211</v>
+      </c>
+      <c r="F4" s="85" t="s">
+        <v>1178</v>
+      </c>
+      <c r="G4" s="50"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="49">
+        <v>3</v>
+      </c>
+      <c r="B5" s="79" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D5" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F5" s="85" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G5" s="49"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+    </row>
+    <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="49">
+        <v>4</v>
+      </c>
+      <c r="B6" s="80"/>
+      <c r="C6" s="52" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D6" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E6" s="63" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F6" s="85" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G6" s="49"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+    </row>
+    <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="49">
+        <v>5</v>
+      </c>
+      <c r="B7" s="80"/>
+      <c r="C7" s="52" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D7" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>1201</v>
+      </c>
+      <c r="F7" s="85" t="s">
+        <v>1143</v>
+      </c>
+      <c r="G7" s="49"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+    </row>
+    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="49">
+        <v>6</v>
+      </c>
+      <c r="B8" s="80"/>
+      <c r="C8" s="52" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D8" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E8" s="63" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F8" s="85" t="s">
+        <v>1144</v>
+      </c>
+      <c r="G8" s="49"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="49">
+        <v>7</v>
+      </c>
+      <c r="B9" s="80"/>
+      <c r="C9" s="52" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D9" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E9" s="63" t="s">
+        <v>1215</v>
+      </c>
+      <c r="F9" s="85" t="s">
+        <v>1145</v>
+      </c>
+      <c r="G9" s="49"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="49">
+        <v>8</v>
+      </c>
+      <c r="B10" s="80"/>
+      <c r="C10" s="52" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D10" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E10" s="63" t="s">
         <v>1202</v>
       </c>
-      <c r="E2" s="50" t="s">
-        <v>551</v>
-      </c>
-      <c r="F2" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="51" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="52">
-        <v>1</v>
-      </c>
-      <c r="B3" s="87" t="s">
-        <v>1184</v>
-      </c>
-      <c r="C3" s="53" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D3" s="48">
-        <v>43657</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F3" s="67" t="s">
-        <v>1159</v>
-      </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-    </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="52">
-        <v>2</v>
-      </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="47" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D4" s="48">
-        <v>43657</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>1214</v>
-      </c>
-      <c r="F4" s="67" t="s">
+      <c r="F10" s="85" t="s">
+        <v>1146</v>
+      </c>
+      <c r="G10" s="49"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+    </row>
+    <row r="11" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="49">
+        <v>10</v>
+      </c>
+      <c r="B11" s="80"/>
+      <c r="C11" s="52" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D11" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>1203</v>
+      </c>
+      <c r="F11" s="85" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G11" s="49"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="49">
+        <v>11</v>
+      </c>
+      <c r="B12" s="80"/>
+      <c r="C12" s="52" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D12" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E12" s="63" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F12" s="85" t="s">
+        <v>1176</v>
+      </c>
+      <c r="G12" s="49"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="49">
+        <v>13</v>
+      </c>
+      <c r="B13" s="80"/>
+      <c r="C13" s="52" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D13" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>1205</v>
+      </c>
+      <c r="F13" s="85" t="s">
+        <v>1179</v>
+      </c>
+      <c r="G13" s="49"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="49">
+        <v>14</v>
+      </c>
+      <c r="B14" s="81"/>
+      <c r="C14" s="52" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D14" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E14" s="63" t="s">
+        <v>1206</v>
+      </c>
+      <c r="F14" s="85" t="s">
         <v>1180</v>
       </c>
-      <c r="G4" s="54"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="52">
-        <v>3</v>
-      </c>
-      <c r="B5" s="87" t="s">
-        <v>1183</v>
-      </c>
-      <c r="C5" s="56" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D5" s="57">
-        <v>43664</v>
-      </c>
-      <c r="E5" s="70" t="s">
-        <v>1210</v>
-      </c>
-      <c r="F5" s="71" t="s">
-        <v>1179</v>
-      </c>
-      <c r="G5" s="52"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-    </row>
-    <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52">
-        <v>4</v>
-      </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="47" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D6" s="48">
-        <v>43664</v>
-      </c>
-      <c r="E6" s="46" t="s">
-        <v>1203</v>
-      </c>
-      <c r="F6" s="90" t="s">
-        <v>1142</v>
-      </c>
-      <c r="G6" s="52"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-    </row>
-    <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52">
-        <v>5</v>
-      </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="56" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D7" s="57">
-        <v>43664</v>
-      </c>
-      <c r="E7" s="70" t="s">
-        <v>1204</v>
-      </c>
-      <c r="F7" s="71" t="s">
-        <v>1143</v>
-      </c>
-      <c r="G7" s="52"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-    </row>
-    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52">
-        <v>6</v>
-      </c>
-      <c r="B8" s="88"/>
-      <c r="C8" s="56" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D8" s="57">
-        <v>43664</v>
-      </c>
-      <c r="E8" s="70" t="s">
-        <v>1219</v>
-      </c>
-      <c r="F8" s="71" t="s">
-        <v>1144</v>
-      </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="52">
-        <v>7</v>
-      </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="56" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D9" s="57">
-        <v>43664</v>
-      </c>
-      <c r="E9" s="70" t="s">
-        <v>1218</v>
-      </c>
-      <c r="F9" s="71" t="s">
-        <v>1145</v>
-      </c>
-      <c r="G9" s="52"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="52">
-        <v>8</v>
-      </c>
-      <c r="B10" s="88"/>
-      <c r="C10" s="56" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D10" s="57">
-        <v>43664</v>
-      </c>
-      <c r="E10" s="70" t="s">
-        <v>1205</v>
-      </c>
-      <c r="F10" s="71" t="s">
-        <v>1146</v>
-      </c>
-      <c r="G10" s="52"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-    </row>
-    <row r="11" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="52">
-        <v>10</v>
-      </c>
-      <c r="B11" s="88"/>
-      <c r="C11" s="47" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D11" s="48">
-        <v>43664</v>
-      </c>
-      <c r="E11" s="46" t="s">
-        <v>1206</v>
-      </c>
-      <c r="F11" s="67" t="s">
-        <v>1177</v>
-      </c>
-      <c r="G11" s="52"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="52">
-        <v>11</v>
-      </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="47" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D12" s="48">
-        <v>43664</v>
-      </c>
-      <c r="E12" s="46" t="s">
-        <v>1207</v>
-      </c>
-      <c r="F12" s="90" t="s">
-        <v>1178</v>
-      </c>
-      <c r="G12" s="52"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="52">
-        <v>13</v>
-      </c>
-      <c r="B13" s="88"/>
-      <c r="C13" s="47" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D13" s="48">
-        <v>43664</v>
-      </c>
-      <c r="E13" s="46" t="s">
-        <v>1208</v>
-      </c>
-      <c r="F13" s="90" t="s">
-        <v>1181</v>
-      </c>
-      <c r="G13" s="52"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="52">
-        <v>14</v>
-      </c>
-      <c r="B14" s="89"/>
-      <c r="C14" s="56" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D14" s="57">
-        <v>43664</v>
-      </c>
-      <c r="E14" s="70" t="s">
-        <v>1209</v>
-      </c>
-      <c r="F14" s="71" t="s">
-        <v>1182</v>
-      </c>
-      <c r="G14" s="52"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="52">
+      <c r="A15" s="49">
         <v>15</v>
       </c>
-      <c r="B15" s="54" t="s">
-        <v>1190</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>1201</v>
-      </c>
-      <c r="D15" s="48">
+      <c r="B15" s="50" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D15" s="53">
         <v>43670</v>
       </c>
       <c r="E15" s="54" t="s">
         <v>1126</v>
       </c>
-      <c r="F15" s="90" t="s">
+      <c r="F15" s="85" t="s">
         <v>1156</v>
       </c>
-      <c r="G15" s="52"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="52">
+      <c r="A16" s="49">
         <v>16</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="50" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C16" s="55" t="s">
         <v>1195</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="D16" s="53">
+        <v>43654</v>
+      </c>
+      <c r="E16" s="54" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F16" s="82" t="s">
+        <v>1167</v>
+      </c>
+      <c r="G16" s="49"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="49">
+        <v>17</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C17" s="55" t="s">
         <v>1198</v>
       </c>
-      <c r="D16" s="57">
-        <v>43654</v>
-      </c>
-      <c r="E16" s="58" t="s">
-        <v>1133</v>
-      </c>
-      <c r="F16" s="59" t="s">
-        <v>1169</v>
-      </c>
-      <c r="G16" s="52"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="52">
-        <v>17</v>
-      </c>
-      <c r="B17" s="54" t="s">
-        <v>1196</v>
-      </c>
-      <c r="C17" s="52" t="s">
-        <v>1201</v>
-      </c>
-      <c r="D17" s="48">
+      <c r="D17" s="53">
         <v>43670</v>
       </c>
       <c r="E17" s="54" t="s">
         <v>1134</v>
       </c>
-      <c r="F17" s="90" t="s">
-        <v>1170</v>
-      </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="55"/>
+      <c r="F17" s="85" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G17" s="49"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="52">
+      <c r="A18" s="49">
         <v>18</v>
       </c>
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="50" t="s">
         <v>448</v>
       </c>
-      <c r="C18" s="47" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D18" s="48">
+      <c r="C18" s="52" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D18" s="53">
         <v>43664</v>
       </c>
       <c r="E18" s="54" t="s">
         <v>1125</v>
       </c>
-      <c r="F18" s="90" t="s">
+      <c r="F18" s="85" t="s">
         <v>1155</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="52">
+      <c r="A19" s="49">
         <v>19</v>
       </c>
-      <c r="B19" s="87" t="s">
+      <c r="B19" s="79" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D19" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F19" s="84" t="s">
+        <v>1141</v>
+      </c>
+      <c r="G19" s="49"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="49">
+        <v>20</v>
+      </c>
+      <c r="B20" s="80"/>
+      <c r="C20" s="56" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D20" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F20" s="84" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G20" s="49"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="49">
+        <v>21</v>
+      </c>
+      <c r="B21" s="80"/>
+      <c r="C21" s="56" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D21" s="53">
+        <v>43657</v>
+      </c>
+      <c r="E21" s="54" t="s">
+        <v>1118</v>
+      </c>
+      <c r="F21" s="84" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G21" s="49"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="49">
+        <v>22</v>
+      </c>
+      <c r="B22" s="80"/>
+      <c r="C22" s="56" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D22" s="53">
+        <v>43657</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F22" s="84" t="s">
+        <v>1149</v>
+      </c>
+      <c r="G22" s="49"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="49">
+        <v>23</v>
+      </c>
+      <c r="B23" s="80"/>
+      <c r="C23" s="56" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D23" s="53">
+        <v>43657</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F23" s="84" t="s">
+        <v>1158</v>
+      </c>
+      <c r="G23" s="49"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+    </row>
+    <row r="24" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="49"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="56" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D24" s="53">
+        <v>43657</v>
+      </c>
+      <c r="E24" s="62" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F24" s="84" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G24" s="49"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="49">
+        <v>24</v>
+      </c>
+      <c r="B25" s="81"/>
+      <c r="C25" s="55" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D25" s="53">
+        <v>43657</v>
+      </c>
+      <c r="E25" s="54" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F25" s="84" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G25" s="49"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="51"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="49">
+        <v>25</v>
+      </c>
+      <c r="B26" s="79" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C26" s="56" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D26" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E26" s="64" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F26" s="85" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G26" s="49"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="51"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="49">
+        <v>26</v>
+      </c>
+      <c r="B27" s="81"/>
+      <c r="C27" s="52" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D27" s="53">
+        <v>43664</v>
+      </c>
+      <c r="E27" s="64" t="s">
+        <v>1214</v>
+      </c>
+      <c r="F27" s="85" t="s">
+        <v>1169</v>
+      </c>
+      <c r="G27" s="49"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="49">
+        <v>27</v>
+      </c>
+      <c r="B28" s="79" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D28" s="53">
+        <v>43657</v>
+      </c>
+      <c r="E28" s="54" t="s">
+        <v>1120</v>
+      </c>
+      <c r="F28" s="84" t="s">
+        <v>1150</v>
+      </c>
+      <c r="G28" s="49"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="51"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="49">
+        <v>28</v>
+      </c>
+      <c r="B29" s="81"/>
+      <c r="C29" s="55" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D29" s="53">
+        <v>43657</v>
+      </c>
+      <c r="E29" s="54" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F29" s="84" t="s">
+        <v>1161</v>
+      </c>
+      <c r="G29" s="49"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="51"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="49">
+        <v>29</v>
+      </c>
+      <c r="B30" s="79" t="s">
         <v>1186</v>
       </c>
-      <c r="C19" s="60" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D19" s="57">
-        <v>43664</v>
-      </c>
-      <c r="E19" s="58" t="s">
-        <v>1116</v>
-      </c>
-      <c r="F19" s="68" t="s">
-        <v>1141</v>
-      </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="55"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="52">
-        <v>20</v>
-      </c>
-      <c r="B20" s="88"/>
-      <c r="C20" s="60" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D20" s="57">
-        <v>43664</v>
-      </c>
-      <c r="E20" s="58" t="s">
-        <v>1117</v>
-      </c>
-      <c r="F20" s="68" t="s">
-        <v>1147</v>
-      </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="55"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="52">
-        <v>21</v>
-      </c>
-      <c r="B21" s="88"/>
-      <c r="C21" s="60" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D21" s="57">
-        <v>43657</v>
-      </c>
-      <c r="E21" s="58" t="s">
-        <v>1118</v>
-      </c>
-      <c r="F21" s="68" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G21" s="52"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="55"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="52">
-        <v>22</v>
-      </c>
-      <c r="B22" s="88"/>
-      <c r="C22" s="60" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D22" s="57">
-        <v>43657</v>
-      </c>
-      <c r="E22" s="58" t="s">
-        <v>1119</v>
-      </c>
-      <c r="F22" s="68" t="s">
-        <v>1149</v>
-      </c>
-      <c r="G22" s="52"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="55"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="52">
-        <v>23</v>
-      </c>
-      <c r="B23" s="88"/>
-      <c r="C23" s="60" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D23" s="57">
-        <v>43657</v>
-      </c>
-      <c r="E23" s="58" t="s">
-        <v>1192</v>
-      </c>
-      <c r="F23" s="68" t="s">
-        <v>1160</v>
-      </c>
-      <c r="G23" s="52"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="55"/>
-    </row>
-    <row r="24" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="52"/>
-      <c r="B24" s="88"/>
-      <c r="C24" s="60" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D24" s="57">
-        <v>43657</v>
-      </c>
-      <c r="E24" s="69" t="s">
-        <v>1216</v>
-      </c>
-      <c r="F24" s="68" t="s">
-        <v>1215</v>
-      </c>
-      <c r="G24" s="52"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="52">
-        <v>24</v>
-      </c>
-      <c r="B25" s="89"/>
-      <c r="C25" s="59" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D25" s="57">
-        <v>43657</v>
-      </c>
-      <c r="E25" s="58" t="s">
-        <v>1193</v>
-      </c>
-      <c r="F25" s="68" t="s">
-        <v>1161</v>
-      </c>
-      <c r="G25" s="52"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="52">
-        <v>25</v>
-      </c>
-      <c r="B26" s="87" t="s">
+      <c r="C30" s="56" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D30" s="53">
+        <v>43654</v>
+      </c>
+      <c r="E30" s="54" t="s">
+        <v>1121</v>
+      </c>
+      <c r="F30" s="82" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G30" s="49"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="51"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="49">
+        <v>30</v>
+      </c>
+      <c r="B31" s="80"/>
+      <c r="C31" s="57" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D31" s="53">
+        <v>43654</v>
+      </c>
+      <c r="E31" s="54" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F31" s="82" t="s">
+        <v>1152</v>
+      </c>
+      <c r="G31" s="49"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="51"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="49">
+        <v>31</v>
+      </c>
+      <c r="B32" s="80"/>
+      <c r="C32" s="57" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D32" s="53">
+        <v>43654</v>
+      </c>
+      <c r="E32" s="54" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F32" s="82" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G32" s="49"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="51"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="49">
+        <v>32</v>
+      </c>
+      <c r="B33" s="80"/>
+      <c r="C33" s="57" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D33" s="53">
+        <v>43654</v>
+      </c>
+      <c r="E33" s="54" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F33" s="82" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G33" s="49"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="51"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="49"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="58" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D34" s="59">
+        <v>43654</v>
+      </c>
+      <c r="E34" s="60" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F34" s="83" t="s">
+        <v>1209</v>
+      </c>
+      <c r="G34" s="49"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="51"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="49">
+        <v>33</v>
+      </c>
+      <c r="B35" s="81"/>
+      <c r="C35" s="57" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D35" s="53">
+        <v>43654</v>
+      </c>
+      <c r="E35" s="54" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F35" s="82" t="s">
+        <v>1164</v>
+      </c>
+      <c r="G35" s="49"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="51"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="49">
+        <v>34</v>
+      </c>
+      <c r="B36" s="79" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C36" s="52" t="s">
         <v>1194</v>
       </c>
-      <c r="C26" s="60" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D26" s="57">
-        <v>43664</v>
-      </c>
-      <c r="E26" s="72" t="s">
-        <v>1135</v>
-      </c>
-      <c r="F26" s="71" t="s">
-        <v>1162</v>
-      </c>
-      <c r="G26" s="52"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="52">
-        <v>26</v>
-      </c>
-      <c r="B27" s="89"/>
-      <c r="C27" s="56" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D27" s="57">
-        <v>43664</v>
-      </c>
-      <c r="E27" s="72" t="s">
-        <v>1217</v>
-      </c>
-      <c r="F27" s="71" t="s">
+      <c r="D36" s="53">
+        <v>43647</v>
+      </c>
+      <c r="E36" s="54" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F36" s="82" t="s">
+        <v>1153</v>
+      </c>
+      <c r="G36" s="49"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="51"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="49">
+        <v>35</v>
+      </c>
+      <c r="B37" s="80"/>
+      <c r="C37" s="52" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D37" s="53">
+        <v>43647</v>
+      </c>
+      <c r="E37" s="54" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F37" s="82" t="s">
+        <v>1154</v>
+      </c>
+      <c r="G37" s="49"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="49">
+        <v>36</v>
+      </c>
+      <c r="B38" s="80"/>
+      <c r="C38" s="52" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D38" s="53">
+        <v>43647</v>
+      </c>
+      <c r="E38" s="54" t="s">
+        <v>1131</v>
+      </c>
+      <c r="F38" s="82" t="s">
+        <v>1165</v>
+      </c>
+      <c r="G38" s="49"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="51"/>
+      <c r="K38" s="51"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="49">
+        <v>37</v>
+      </c>
+      <c r="B39" s="81"/>
+      <c r="C39" s="52" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D39" s="53">
+        <v>43647</v>
+      </c>
+      <c r="E39" s="54" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F39" s="82" t="s">
+        <v>1166</v>
+      </c>
+      <c r="G39" s="49"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="49">
+        <v>40</v>
+      </c>
+      <c r="B40" s="49" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C40" s="57" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D40" s="53">
+        <v>43654</v>
+      </c>
+      <c r="E40" s="54" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F40" s="82" t="s">
+        <v>1174</v>
+      </c>
+      <c r="G40" s="49"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="51"/>
+    </row>
+    <row r="41" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="49">
+        <v>49</v>
+      </c>
+      <c r="B41" s="80"/>
+      <c r="C41" s="52" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D41" s="53">
+        <v>43647</v>
+      </c>
+      <c r="E41" s="54" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F41" s="82" t="s">
+        <v>1170</v>
+      </c>
+      <c r="G41" s="49"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="51"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="51"/>
+    </row>
+    <row r="42" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="49">
+        <v>50</v>
+      </c>
+      <c r="B42" s="80"/>
+      <c r="C42" s="52" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D42" s="53">
+        <v>43647</v>
+      </c>
+      <c r="E42" s="54" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F42" s="82" t="s">
         <v>1171</v>
       </c>
-      <c r="G27" s="52"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="55"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="52">
-        <v>27</v>
-      </c>
-      <c r="B28" s="87" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C28" s="60" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D28" s="57">
-        <v>43657</v>
-      </c>
-      <c r="E28" s="58" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F28" s="68" t="s">
-        <v>1150</v>
-      </c>
-      <c r="G28" s="52"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="52">
-        <v>28</v>
-      </c>
-      <c r="B29" s="89"/>
-      <c r="C29" s="59" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D29" s="57">
-        <v>43657</v>
-      </c>
-      <c r="E29" s="58" t="s">
-        <v>1127</v>
-      </c>
-      <c r="F29" s="68" t="s">
-        <v>1163</v>
-      </c>
-      <c r="G29" s="52"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="55"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="52">
-        <v>29</v>
-      </c>
-      <c r="B30" s="87" t="s">
-        <v>1188</v>
-      </c>
-      <c r="C30" s="60" t="s">
-        <v>1198</v>
-      </c>
-      <c r="D30" s="57">
-        <v>43654</v>
-      </c>
-      <c r="E30" s="58" t="s">
-        <v>1121</v>
-      </c>
-      <c r="F30" s="59" t="s">
-        <v>1151</v>
-      </c>
-      <c r="G30" s="52"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="55"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="52">
-        <v>30</v>
-      </c>
-      <c r="B31" s="88"/>
-      <c r="C31" s="61" t="s">
-        <v>1198</v>
-      </c>
-      <c r="D31" s="57">
-        <v>43654</v>
-      </c>
-      <c r="E31" s="58" t="s">
-        <v>1122</v>
-      </c>
-      <c r="F31" s="59" t="s">
-        <v>1152</v>
-      </c>
-      <c r="G31" s="52"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="55"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="52">
-        <v>31</v>
-      </c>
-      <c r="B32" s="88"/>
-      <c r="C32" s="61" t="s">
-        <v>1198</v>
-      </c>
-      <c r="D32" s="57">
-        <v>43654</v>
-      </c>
-      <c r="E32" s="58" t="s">
-        <v>1128</v>
-      </c>
-      <c r="F32" s="59" t="s">
-        <v>1164</v>
-      </c>
-      <c r="G32" s="52"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="55"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="52">
-        <v>32</v>
-      </c>
-      <c r="B33" s="88"/>
-      <c r="C33" s="61" t="s">
-        <v>1198</v>
-      </c>
-      <c r="D33" s="57">
-        <v>43654</v>
-      </c>
-      <c r="E33" s="58" t="s">
-        <v>1129</v>
-      </c>
-      <c r="F33" s="59" t="s">
-        <v>1165</v>
-      </c>
-      <c r="G33" s="52"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="55"/>
-      <c r="K33" s="55"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="52"/>
-      <c r="B34" s="88"/>
-      <c r="C34" s="62" t="s">
-        <v>1198</v>
-      </c>
-      <c r="D34" s="63">
-        <v>43654</v>
-      </c>
-      <c r="E34" s="64" t="s">
-        <v>1211</v>
-      </c>
-      <c r="F34" s="65" t="s">
-        <v>1212</v>
-      </c>
-      <c r="G34" s="52"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="55"/>
-      <c r="K34" s="55"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="52">
-        <v>33</v>
-      </c>
-      <c r="B35" s="89"/>
-      <c r="C35" s="61" t="s">
-        <v>1198</v>
-      </c>
-      <c r="D35" s="57">
-        <v>43654</v>
-      </c>
-      <c r="E35" s="58" t="s">
-        <v>1130</v>
-      </c>
-      <c r="F35" s="59" t="s">
-        <v>1166</v>
-      </c>
-      <c r="G35" s="52"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="55"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="52">
-        <v>34</v>
-      </c>
-      <c r="B36" s="87" t="s">
-        <v>1189</v>
-      </c>
-      <c r="C36" s="56" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D36" s="57">
+      <c r="G42" s="49"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="51"/>
+      <c r="K42" s="51"/>
+    </row>
+    <row r="43" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="49">
+        <v>51</v>
+      </c>
+      <c r="B43" s="80"/>
+      <c r="C43" s="52" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D43" s="53">
         <v>43647</v>
       </c>
-      <c r="E36" s="58" t="s">
-        <v>1123</v>
-      </c>
-      <c r="F36" s="59" t="s">
-        <v>1153</v>
-      </c>
-      <c r="G36" s="52"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="55"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="52">
-        <v>35</v>
-      </c>
-      <c r="B37" s="88"/>
-      <c r="C37" s="56" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D37" s="57">
+      <c r="E43" s="54" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F43" s="82" t="s">
+        <v>1172</v>
+      </c>
+      <c r="G43" s="49"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
+      <c r="K43" s="51"/>
+    </row>
+    <row r="44" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="49">
+        <v>52</v>
+      </c>
+      <c r="B44" s="81"/>
+      <c r="C44" s="52" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D44" s="53">
         <v>43647</v>
       </c>
-      <c r="E37" s="58" t="s">
-        <v>1124</v>
-      </c>
-      <c r="F37" s="59" t="s">
-        <v>1154</v>
-      </c>
-      <c r="G37" s="52"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="55"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="52">
-        <v>36</v>
-      </c>
-      <c r="B38" s="88"/>
-      <c r="C38" s="56" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D38" s="57">
-        <v>43647</v>
-      </c>
-      <c r="E38" s="58" t="s">
-        <v>1131</v>
-      </c>
-      <c r="F38" s="59" t="s">
-        <v>1167</v>
-      </c>
-      <c r="G38" s="52"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="55"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="52">
-        <v>37</v>
-      </c>
-      <c r="B39" s="89"/>
-      <c r="C39" s="56" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D39" s="57">
-        <v>43647</v>
-      </c>
-      <c r="E39" s="58" t="s">
-        <v>1132</v>
-      </c>
-      <c r="F39" s="59" t="s">
-        <v>1168</v>
-      </c>
-      <c r="G39" s="52"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="55"/>
-      <c r="K39" s="55"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="52">
-        <v>38</v>
-      </c>
-      <c r="B40" s="87" t="s">
-        <v>1191</v>
-      </c>
-      <c r="C40" s="53" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D40" s="48">
-        <v>43657</v>
-      </c>
-      <c r="E40" s="54" t="s">
-        <v>1220</v>
-      </c>
-      <c r="F40" s="52" t="s">
-        <v>1157</v>
-      </c>
-      <c r="G40" s="52"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="55"/>
-      <c r="K40" s="55"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="52">
-        <v>39</v>
-      </c>
-      <c r="B41" s="89"/>
-      <c r="C41" s="47" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D41" s="48">
-        <v>43657</v>
-      </c>
-      <c r="E41" s="54" t="s">
-        <v>1221</v>
-      </c>
-      <c r="F41" s="52" t="s">
-        <v>1158</v>
-      </c>
-      <c r="G41" s="52"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="55"/>
-      <c r="K41" s="55"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="52">
-        <v>40</v>
-      </c>
-      <c r="B42" s="52" t="s">
-        <v>1185</v>
-      </c>
-      <c r="C42" s="61" t="s">
-        <v>1198</v>
-      </c>
-      <c r="D42" s="57">
-        <v>43654</v>
-      </c>
-      <c r="E42" s="58" t="s">
-        <v>1140</v>
-      </c>
-      <c r="F42" s="59" t="s">
-        <v>1176</v>
-      </c>
-      <c r="G42" s="52"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="55"/>
-      <c r="K42" s="55"/>
-    </row>
-    <row r="43" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="52">
-        <v>49</v>
-      </c>
-      <c r="B43" s="88"/>
-      <c r="C43" s="56" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D43" s="57">
-        <v>43647</v>
-      </c>
-      <c r="E43" s="58" t="s">
-        <v>1136</v>
-      </c>
-      <c r="F43" s="59" t="s">
-        <v>1172</v>
-      </c>
-      <c r="G43" s="52"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
-      <c r="K43" s="55"/>
-    </row>
-    <row r="44" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="52">
-        <v>50</v>
-      </c>
-      <c r="B44" s="88"/>
-      <c r="C44" s="56" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D44" s="57">
-        <v>43647</v>
-      </c>
-      <c r="E44" s="58" t="s">
-        <v>1137</v>
-      </c>
-      <c r="F44" s="59" t="s">
+      <c r="E44" s="54" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F44" s="82" t="s">
         <v>1173</v>
       </c>
-      <c r="G44" s="52"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="55"/>
-    </row>
-    <row r="45" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="52">
-        <v>51</v>
-      </c>
-      <c r="B45" s="88"/>
-      <c r="C45" s="56" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D45" s="57">
-        <v>43647</v>
-      </c>
-      <c r="E45" s="58" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F45" s="59" t="s">
-        <v>1174</v>
-      </c>
-      <c r="G45" s="52"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="55"/>
-    </row>
-    <row r="46" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="52">
-        <v>52</v>
-      </c>
-      <c r="B46" s="89"/>
-      <c r="C46" s="56" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D46" s="57">
-        <v>43647</v>
-      </c>
-      <c r="E46" s="58" t="s">
-        <v>1139</v>
-      </c>
-      <c r="F46" s="59" t="s">
-        <v>1175</v>
-      </c>
-      <c r="G46" s="52"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="55"/>
-      <c r="K46" s="55"/>
-    </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E57" s="66"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="51"/>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E55" s="61"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:K46" xr:uid="{C6B0F034-955C-4BFB-9151-0B32E8F7F8DB}"/>
-  <sortState ref="A3:K46">
-    <sortCondition ref="B3:B46"/>
+  <autoFilter ref="A2:K44" xr:uid="{C6B0F034-955C-4BFB-9151-0B32E8F7F8DB}"/>
+  <sortState ref="A3:K44">
+    <sortCondition ref="B3:B44"/>
   </sortState>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="B19:B25"/>
-    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B14"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="B30:B35"/>
     <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -15876,41 +15797,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16117,32 +16003,42 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7F7E23-FE37-4AB8-A4B3-5025B5D9E450}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16159,4 +16055,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4574461-DD7B-4995-B8CC-A8415FBC904F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8EC3877-83FF-480B-8819-7751D3BFBA2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>